<commit_message>
:sparkles: Make DocumentReference.type mandatory
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D8BF7-8851-47EB-BAC2-67E217F15551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9918B140-DDC0-4F1B-A8EB-F6DE30608AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="901" firstSheet="11" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -859,7 +859,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4239" uniqueCount="1554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="1555">
   <si>
     <t>Required</t>
   </si>
@@ -5535,6 +5535,9 @@
   </si>
   <si>
     <t>230060001</t>
+  </si>
+  <si>
+    <t>Kind of document.</t>
   </si>
 </sst>
 </file>
@@ -5878,22 +5881,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6898,8 +6901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1770B9A2-CDA6-4E37-82EC-A9C07EE24319}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7273,13 +7276,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -7290,6 +7286,13 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7968,7 +7971,7 @@
         <v>465</v>
       </c>
       <c r="D38" s="54"/>
-      <c r="E38" s="58"/>
+      <c r="E38" s="56"/>
       <c r="F38" s="59" t="s">
         <v>466</v>
       </c>
@@ -7983,11 +7986,11 @@
       <c r="B39" s="42" t="s">
         <v>468</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="57" t="s">
         <v>469</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="58"/>
       <c r="F39" s="55"/>
       <c r="G39" s="53"/>
       <c r="H39" s="53"/>
@@ -8000,11 +8003,11 @@
       <c r="B40" s="42" t="s">
         <v>471</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="57" t="s">
         <v>472</v>
       </c>
-      <c r="D40" s="56"/>
-      <c r="E40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="58"/>
       <c r="F40" s="55"/>
       <c r="G40" s="53"/>
       <c r="H40" s="53"/>
@@ -8017,11 +8020,11 @@
       <c r="B41" s="42" t="s">
         <v>474</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="57" t="s">
         <v>475</v>
       </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="58"/>
       <c r="F41" s="55"/>
       <c r="G41" s="53"/>
       <c r="H41" s="53"/>
@@ -8034,11 +8037,11 @@
       <c r="B42" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="57" t="s">
         <v>1505</v>
       </c>
-      <c r="D42" s="56"/>
-      <c r="E42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="58"/>
       <c r="F42" s="55"/>
       <c r="G42" s="53"/>
       <c r="H42" s="53"/>
@@ -8051,11 +8054,11 @@
       <c r="B43" s="42" t="s">
         <v>479</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="57" t="s">
         <v>480</v>
       </c>
-      <c r="D43" s="56"/>
-      <c r="E43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="58"/>
       <c r="F43" s="55"/>
       <c r="G43" s="53"/>
       <c r="H43" s="53"/>
@@ -8068,11 +8071,11 @@
       <c r="B44" s="42" t="s">
         <v>482</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="57" t="s">
         <v>483</v>
       </c>
-      <c r="D44" s="56"/>
-      <c r="E44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="58"/>
       <c r="F44" s="55"/>
       <c r="G44" s="53"/>
       <c r="H44" s="53"/>
@@ -8085,11 +8088,11 @@
       <c r="B45" s="42" t="s">
         <v>485</v>
       </c>
-      <c r="C45" s="56" t="s">
+      <c r="C45" s="57" t="s">
         <v>486</v>
       </c>
-      <c r="D45" s="56"/>
-      <c r="E45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="58"/>
       <c r="F45" s="55"/>
       <c r="G45" s="53"/>
       <c r="H45" s="53"/>
@@ -8102,11 +8105,11 @@
       <c r="B46" s="42" t="s">
         <v>488</v>
       </c>
-      <c r="C46" s="56" t="s">
+      <c r="C46" s="57" t="s">
         <v>489</v>
       </c>
-      <c r="D46" s="56"/>
-      <c r="E46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="58"/>
       <c r="F46" s="55"/>
       <c r="G46" s="53"/>
       <c r="H46" s="53"/>
@@ -8119,11 +8122,11 @@
       <c r="B47" s="42" t="s">
         <v>491</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="57" t="s">
         <v>492</v>
       </c>
-      <c r="D47" s="56"/>
-      <c r="E47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="55"/>
       <c r="G47" s="53"/>
       <c r="H47" s="53"/>
@@ -8136,11 +8139,11 @@
       <c r="B48" s="42" t="s">
         <v>494</v>
       </c>
-      <c r="C48" s="56" t="s">
+      <c r="C48" s="57" t="s">
         <v>495</v>
       </c>
-      <c r="D48" s="56"/>
-      <c r="E48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="58"/>
       <c r="F48" s="55"/>
       <c r="G48" s="53"/>
       <c r="H48" s="53"/>
@@ -8153,11 +8156,11 @@
       <c r="B49" s="42" t="s">
         <v>497</v>
       </c>
-      <c r="C49" s="56" t="s">
+      <c r="C49" s="57" t="s">
         <v>498</v>
       </c>
-      <c r="D49" s="56"/>
-      <c r="E49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="58"/>
       <c r="F49" s="55"/>
       <c r="G49" s="53"/>
       <c r="H49" s="53"/>
@@ -8170,11 +8173,11 @@
       <c r="B50" s="42" t="s">
         <v>500</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C50" s="57" t="s">
         <v>501</v>
       </c>
-      <c r="D50" s="56"/>
-      <c r="E50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="58"/>
       <c r="F50" s="55"/>
       <c r="G50" s="53"/>
       <c r="H50" s="53"/>
@@ -8187,11 +8190,11 @@
       <c r="B51" s="42" t="s">
         <v>503</v>
       </c>
-      <c r="C51" s="56" t="s">
+      <c r="C51" s="57" t="s">
         <v>504</v>
       </c>
-      <c r="D51" s="56"/>
-      <c r="E51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="58"/>
       <c r="F51" s="55"/>
       <c r="G51" s="53"/>
       <c r="H51" s="53"/>
@@ -8204,11 +8207,11 @@
       <c r="B52" s="42" t="s">
         <v>506</v>
       </c>
-      <c r="C52" s="56" t="s">
+      <c r="C52" s="57" t="s">
         <v>507</v>
       </c>
-      <c r="D52" s="56"/>
-      <c r="E52" s="57"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="58"/>
       <c r="F52" s="55"/>
       <c r="G52" s="53"/>
       <c r="H52" s="53"/>
@@ -8221,11 +8224,11 @@
       <c r="B53" s="42" t="s">
         <v>509</v>
       </c>
-      <c r="C53" s="56" t="s">
+      <c r="C53" s="57" t="s">
         <v>510</v>
       </c>
-      <c r="D53" s="56"/>
-      <c r="E53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="58"/>
       <c r="F53" s="55"/>
       <c r="G53" s="53"/>
       <c r="H53" s="53"/>
@@ -8238,11 +8241,11 @@
       <c r="B54" s="42" t="s">
         <v>512</v>
       </c>
-      <c r="C54" s="56" t="s">
+      <c r="C54" s="57" t="s">
         <v>513</v>
       </c>
-      <c r="D54" s="56"/>
-      <c r="E54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="58"/>
       <c r="F54" s="55"/>
       <c r="G54" s="53"/>
       <c r="H54" s="53"/>
@@ -8255,11 +8258,11 @@
       <c r="B55" s="42" t="s">
         <v>515</v>
       </c>
-      <c r="C55" s="56" t="s">
+      <c r="C55" s="57" t="s">
         <v>516</v>
       </c>
-      <c r="D55" s="56"/>
-      <c r="E55" s="57"/>
+      <c r="D55" s="57"/>
+      <c r="E55" s="58"/>
       <c r="F55" s="55"/>
       <c r="G55" s="53"/>
       <c r="H55" s="53"/>
@@ -8272,11 +8275,11 @@
       <c r="B56" s="42" t="s">
         <v>518</v>
       </c>
-      <c r="C56" s="56" t="s">
+      <c r="C56" s="57" t="s">
         <v>519</v>
       </c>
-      <c r="D56" s="56"/>
-      <c r="E56" s="57"/>
+      <c r="D56" s="57"/>
+      <c r="E56" s="58"/>
       <c r="F56" s="55"/>
       <c r="G56" s="53"/>
       <c r="H56" s="53"/>
@@ -8289,11 +8292,11 @@
       <c r="B57" s="42" t="s">
         <v>521</v>
       </c>
-      <c r="C57" s="56" t="s">
+      <c r="C57" s="57" t="s">
         <v>522</v>
       </c>
-      <c r="D57" s="56"/>
-      <c r="E57" s="57"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="58"/>
       <c r="F57" s="55"/>
       <c r="G57" s="53"/>
       <c r="H57" s="53"/>
@@ -8306,11 +8309,11 @@
       <c r="B58" s="42" t="s">
         <v>524</v>
       </c>
-      <c r="C58" s="56" t="s">
+      <c r="C58" s="57" t="s">
         <v>525</v>
       </c>
-      <c r="D58" s="56"/>
-      <c r="E58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="58"/>
       <c r="F58" s="55"/>
       <c r="G58" s="53"/>
       <c r="H58" s="53"/>
@@ -8323,11 +8326,11 @@
       <c r="B59" s="42" t="s">
         <v>527</v>
       </c>
-      <c r="C59" s="56" t="s">
+      <c r="C59" s="57" t="s">
         <v>528</v>
       </c>
-      <c r="D59" s="56"/>
-      <c r="E59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="58"/>
       <c r="F59" s="55"/>
       <c r="G59" s="53"/>
       <c r="H59" s="53"/>
@@ -8340,11 +8343,11 @@
       <c r="B60" s="42" t="s">
         <v>530</v>
       </c>
-      <c r="C60" s="56" t="s">
+      <c r="C60" s="57" t="s">
         <v>531</v>
       </c>
-      <c r="D60" s="56"/>
-      <c r="E60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="58"/>
       <c r="F60" s="55"/>
       <c r="G60" s="53"/>
       <c r="H60" s="53"/>
@@ -8357,11 +8360,11 @@
       <c r="B61" s="42" t="s">
         <v>533</v>
       </c>
-      <c r="C61" s="56" t="s">
+      <c r="C61" s="57" t="s">
         <v>534</v>
       </c>
-      <c r="D61" s="56"/>
-      <c r="E61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="58"/>
       <c r="F61" s="55"/>
       <c r="G61" s="53"/>
       <c r="H61" s="53"/>
@@ -8374,11 +8377,11 @@
       <c r="B62" s="42" t="s">
         <v>536</v>
       </c>
-      <c r="C62" s="56" t="s">
+      <c r="C62" s="57" t="s">
         <v>537</v>
       </c>
-      <c r="D62" s="56"/>
-      <c r="E62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="58"/>
       <c r="F62" s="55"/>
       <c r="G62" s="53"/>
       <c r="H62" s="53"/>
@@ -8391,11 +8394,11 @@
       <c r="B63" s="42" t="s">
         <v>538</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C63" s="57" t="s">
         <v>539</v>
       </c>
-      <c r="D63" s="56"/>
-      <c r="E63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="58"/>
       <c r="F63" s="55"/>
       <c r="G63" s="53"/>
       <c r="H63" s="53"/>
@@ -8408,11 +8411,11 @@
       <c r="B64" s="42" t="s">
         <v>541</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="57" t="s">
         <v>542</v>
       </c>
-      <c r="D64" s="56"/>
-      <c r="E64" s="57"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="58"/>
       <c r="F64" s="55"/>
       <c r="G64" s="53"/>
       <c r="H64" s="53"/>
@@ -8425,11 +8428,11 @@
       <c r="B65" s="42" t="s">
         <v>544</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="57" t="s">
         <v>545</v>
       </c>
-      <c r="D65" s="56"/>
-      <c r="E65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="58"/>
       <c r="F65" s="55"/>
       <c r="G65" s="53"/>
       <c r="H65" s="53"/>
@@ -8442,11 +8445,11 @@
       <c r="B66" s="42" t="s">
         <v>547</v>
       </c>
-      <c r="C66" s="56" t="s">
+      <c r="C66" s="57" t="s">
         <v>548</v>
       </c>
-      <c r="D66" s="56"/>
-      <c r="E66" s="57"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="58"/>
       <c r="F66" s="55"/>
       <c r="G66" s="53"/>
       <c r="H66" s="53"/>
@@ -8459,11 +8462,11 @@
       <c r="B67" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="C67" s="56" t="s">
+      <c r="C67" s="57" t="s">
         <v>551</v>
       </c>
-      <c r="D67" s="56"/>
-      <c r="E67" s="57"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="58"/>
       <c r="F67" s="55"/>
       <c r="G67" s="53"/>
       <c r="H67" s="53"/>
@@ -8476,11 +8479,11 @@
       <c r="B68" s="42" t="s">
         <v>553</v>
       </c>
-      <c r="C68" s="56" t="s">
+      <c r="C68" s="57" t="s">
         <v>554</v>
       </c>
-      <c r="D68" s="56"/>
-      <c r="E68" s="57"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="58"/>
       <c r="F68" s="55"/>
       <c r="G68" s="53"/>
       <c r="H68" s="53"/>
@@ -8493,11 +8496,11 @@
       <c r="B69" s="42" t="s">
         <v>556</v>
       </c>
-      <c r="C69" s="56" t="s">
+      <c r="C69" s="57" t="s">
         <v>557</v>
       </c>
-      <c r="D69" s="56"/>
-      <c r="E69" s="57"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="58"/>
       <c r="F69" s="55"/>
       <c r="G69" s="53"/>
       <c r="H69" s="53"/>
@@ -8510,11 +8513,11 @@
       <c r="B70" s="42" t="s">
         <v>559</v>
       </c>
-      <c r="C70" s="56" t="s">
+      <c r="C70" s="57" t="s">
         <v>560</v>
       </c>
-      <c r="D70" s="56"/>
-      <c r="E70" s="57"/>
+      <c r="D70" s="57"/>
+      <c r="E70" s="58"/>
       <c r="F70" s="55"/>
       <c r="G70" s="53"/>
       <c r="H70" s="53"/>
@@ -8527,11 +8530,11 @@
       <c r="B71" s="42" t="s">
         <v>562</v>
       </c>
-      <c r="C71" s="56" t="s">
+      <c r="C71" s="57" t="s">
         <v>563</v>
       </c>
-      <c r="D71" s="56"/>
-      <c r="E71" s="57"/>
+      <c r="D71" s="57"/>
+      <c r="E71" s="58"/>
       <c r="F71" s="55"/>
       <c r="G71" s="53"/>
       <c r="H71" s="53"/>
@@ -8544,11 +8547,11 @@
       <c r="B72" s="42" t="s">
         <v>565</v>
       </c>
-      <c r="C72" s="56" t="s">
+      <c r="C72" s="57" t="s">
         <v>566</v>
       </c>
-      <c r="D72" s="56"/>
-      <c r="E72" s="57"/>
+      <c r="D72" s="57"/>
+      <c r="E72" s="58"/>
       <c r="F72" s="55"/>
       <c r="G72" s="53"/>
       <c r="H72" s="53"/>
@@ -8561,11 +8564,11 @@
       <c r="B73" s="42" t="s">
         <v>568</v>
       </c>
-      <c r="C73" s="56" t="s">
+      <c r="C73" s="57" t="s">
         <v>569</v>
       </c>
-      <c r="D73" s="56"/>
-      <c r="E73" s="57"/>
+      <c r="D73" s="57"/>
+      <c r="E73" s="58"/>
       <c r="F73" s="55"/>
       <c r="G73" s="53"/>
       <c r="H73" s="53"/>
@@ -8578,11 +8581,11 @@
       <c r="B74" s="42" t="s">
         <v>571</v>
       </c>
-      <c r="C74" s="56" t="s">
+      <c r="C74" s="57" t="s">
         <v>572</v>
       </c>
-      <c r="D74" s="56"/>
-      <c r="E74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="58"/>
       <c r="F74" s="55"/>
       <c r="G74" s="53"/>
       <c r="H74" s="53"/>
@@ -8595,11 +8598,11 @@
       <c r="B75" s="42" t="s">
         <v>574</v>
       </c>
-      <c r="C75" s="56" t="s">
+      <c r="C75" s="57" t="s">
         <v>575</v>
       </c>
-      <c r="D75" s="56"/>
-      <c r="E75" s="57"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="58"/>
       <c r="F75" s="55"/>
       <c r="G75" s="53"/>
       <c r="H75" s="53"/>
@@ -8612,11 +8615,11 @@
       <c r="B76" s="42" t="s">
         <v>577</v>
       </c>
-      <c r="C76" s="56" t="s">
+      <c r="C76" s="57" t="s">
         <v>578</v>
       </c>
-      <c r="D76" s="56"/>
-      <c r="E76" s="57"/>
+      <c r="D76" s="57"/>
+      <c r="E76" s="58"/>
       <c r="F76" s="55"/>
       <c r="G76" s="53"/>
       <c r="H76" s="53"/>
@@ -8629,11 +8632,11 @@
       <c r="B77" s="42" t="s">
         <v>580</v>
       </c>
-      <c r="C77" s="56" t="s">
+      <c r="C77" s="57" t="s">
         <v>581</v>
       </c>
-      <c r="D77" s="56"/>
-      <c r="E77" s="57"/>
+      <c r="D77" s="57"/>
+      <c r="E77" s="58"/>
       <c r="F77" s="55"/>
       <c r="G77" s="53"/>
       <c r="H77" s="53"/>
@@ -8646,11 +8649,11 @@
       <c r="B78" s="42" t="s">
         <v>583</v>
       </c>
-      <c r="C78" s="56" t="s">
+      <c r="C78" s="57" t="s">
         <v>584</v>
       </c>
-      <c r="D78" s="56"/>
-      <c r="E78" s="57"/>
+      <c r="D78" s="57"/>
+      <c r="E78" s="58"/>
       <c r="F78" s="55"/>
       <c r="G78" s="53"/>
       <c r="H78" s="53"/>
@@ -8663,11 +8666,11 @@
       <c r="B79" s="42" t="s">
         <v>586</v>
       </c>
-      <c r="C79" s="56" t="s">
+      <c r="C79" s="57" t="s">
         <v>587</v>
       </c>
-      <c r="D79" s="56"/>
-      <c r="E79" s="57"/>
+      <c r="D79" s="57"/>
+      <c r="E79" s="58"/>
       <c r="F79" s="55"/>
       <c r="G79" s="53"/>
       <c r="H79" s="53"/>
@@ -8680,11 +8683,11 @@
       <c r="B80" s="42" t="s">
         <v>589</v>
       </c>
-      <c r="C80" s="56" t="s">
+      <c r="C80" s="57" t="s">
         <v>590</v>
       </c>
-      <c r="D80" s="56"/>
-      <c r="E80" s="57"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="58"/>
       <c r="F80" s="55"/>
       <c r="G80" s="53"/>
       <c r="H80" s="53"/>
@@ -8692,6 +8695,99 @@
     </row>
   </sheetData>
   <mergeCells count="117">
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F43:I43"/>
@@ -8716,99 +8812,6 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="F26:I26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9672,41 +9675,14 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -9723,14 +9699,41 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -10616,13 +10619,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -10633,6 +10629,13 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E19" xr:uid="{EA762E0C-5AF2-4B96-902B-4972A6BA0D33}">
@@ -11729,23 +11732,25 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
     <mergeCell ref="F43:I43"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="F31:I31"/>
@@ -11758,25 +11763,23 @@
     <mergeCell ref="F38:I38"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -19013,31 +19016,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="F110:I110"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="F112:I112"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="F109:I109"/>
     <mergeCell ref="F100:I100"/>
     <mergeCell ref="F101:I101"/>
     <mergeCell ref="F102:I102"/>
@@ -19048,6 +19026,31 @@
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
+    <mergeCell ref="F110:I110"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="F112:I112"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F108:I108"/>
+    <mergeCell ref="F109:I109"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -19080,10 +19083,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19561EC6-A7BE-4A68-B7B3-8285DC687376}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19205,10 +19208,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>1050</v>
+        <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>1051</v>
+        <v>1054</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -19217,15 +19220,19 @@
         <v>20</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>1052</v>
-      </c>
+        <v>1554</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="B7" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -19234,36 +19241,32 @@
         <v>20</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>124</v>
+        <v>1053</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>1054</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>1056</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+        <v>1055</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1057</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>1058</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -19272,7 +19275,7 @@
         <v>119</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -19281,43 +19284,55 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>1060</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>1061</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
         <v>1062</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="52" t="s">
-        <v>1063</v>
-      </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
@@ -19337,11 +19352,20 @@
       <c r="D15" s="52"/>
       <c r="E15" s="34"/>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="52" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="34"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -19351,19 +19375,19 @@
           <x14:formula1>
             <xm:f>'Dataset Intro'!$Q$2:$Q$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F5 F8:F9</xm:sqref>
+          <xm:sqref>F3:F6 F9:F10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1609AB07-BC92-430D-87FC-95A519940B84}">
           <x14:formula1>
             <xm:f>'Dataset Intro'!$Q$19:$Q$25</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H5 H8:H9</xm:sqref>
+          <xm:sqref>H3:H6 H9:H10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BBA0E270-78EE-4801-B179-241277F6B81C}">
           <x14:formula1>
             <xm:f>'Dataset Intro'!$Q$13:$Q$15</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G5 G8:G9</xm:sqref>
+          <xm:sqref>G3:G6 G9:G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -21205,48 +21229,109 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
@@ -21271,109 +21356,48 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21919,7 +21943,7 @@
         <v>1122</v>
       </c>
       <c r="D14" s="54"/>
-      <c r="E14" s="58"/>
+      <c r="E14" s="56"/>
       <c r="F14" s="59" t="s">
         <v>466</v>
       </c>
@@ -21928,201 +21952,201 @@
       <c r="I14" s="59"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="61" t="s">
         <v>1123</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1124</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="57" t="s">
         <v>1125</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="55"/>
       <c r="G15" s="53"/>
       <c r="H15" s="53"/>
       <c r="I15" s="53"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="42" t="s">
         <v>1126</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="57" t="s">
         <v>1127</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="58"/>
       <c r="F16" s="55"/>
       <c r="G16" s="53"/>
       <c r="H16" s="53"/>
       <c r="I16" s="53"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="57" t="s">
         <v>1129</v>
       </c>
-      <c r="D17" s="56"/>
-      <c r="E17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
       <c r="F17" s="55"/>
       <c r="G17" s="53"/>
       <c r="H17" s="53"/>
       <c r="I17" s="53"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="62"/>
+      <c r="A18" s="61"/>
       <c r="B18" s="42" t="s">
         <v>1130</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="58" t="s">
         <v>1131</v>
       </c>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
       <c r="F18" s="55"/>
       <c r="G18" s="53"/>
       <c r="H18" s="53"/>
       <c r="I18" s="53"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="62"/>
+      <c r="A19" s="61"/>
       <c r="B19" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="58" t="s">
         <v>1133</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="55"/>
       <c r="G19" s="53"/>
       <c r="H19" s="53"/>
       <c r="I19" s="53"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>1134</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1135</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="58" t="s">
         <v>1136</v>
       </c>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
       <c r="F20" s="55"/>
       <c r="G20" s="53"/>
       <c r="H20" s="53"/>
       <c r="I20" s="53"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="63"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="42" t="s">
         <v>1137</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="58" t="s">
         <v>1138</v>
       </c>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="55"/>
       <c r="G21" s="53"/>
       <c r="H21" s="53"/>
       <c r="I21" s="53"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="63"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="42" t="s">
         <v>1139</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="58" t="s">
         <v>1140</v>
       </c>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
       <c r="F22" s="55"/>
       <c r="G22" s="53"/>
       <c r="H22" s="53"/>
       <c r="I22" s="53"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="42" t="s">
         <v>1141</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="58" t="s">
         <v>1142</v>
       </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="55"/>
       <c r="G23" s="53"/>
       <c r="H23" s="53"/>
       <c r="I23" s="53"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="62" t="s">
         <v>1143</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1135</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="58" t="s">
         <v>1144</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="55"/>
       <c r="G24" s="53"/>
       <c r="H24" s="53"/>
       <c r="I24" s="53"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="42" t="s">
         <v>1145</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="58" t="s">
         <v>1146</v>
       </c>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="55"/>
       <c r="G25" s="53"/>
       <c r="H25" s="53"/>
       <c r="I25" s="53"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="42" t="s">
         <v>1139</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="58" t="s">
         <v>1147</v>
       </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="55"/>
       <c r="G26" s="53"/>
       <c r="H26" s="53"/>
       <c r="I26" s="53"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="63"/>
+      <c r="A27" s="62"/>
       <c r="B27" s="42" t="s">
         <v>1141</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="63" t="s">
         <v>1148</v>
       </c>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
       <c r="F27" s="55"/>
       <c r="G27" s="53"/>
       <c r="H27" s="53"/>
@@ -22135,137 +22159,137 @@
       <c r="B28" s="45" t="s">
         <v>1150</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="63" t="s">
         <v>1151</v>
       </c>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
       <c r="F28" s="55"/>
       <c r="G28" s="53"/>
       <c r="H28" s="53"/>
       <c r="I28" s="53"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="62" t="s">
         <v>1152</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1153</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="63" t="s">
         <v>1154</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="61"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
       <c r="F29" s="55"/>
       <c r="G29" s="53"/>
       <c r="H29" s="53"/>
       <c r="I29" s="53"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="63"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="45" t="s">
         <v>1155</v>
       </c>
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="63" t="s">
         <v>1156</v>
       </c>
-      <c r="D30" s="61"/>
-      <c r="E30" s="61"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
       <c r="F30" s="55"/>
       <c r="G30" s="53"/>
       <c r="H30" s="53"/>
       <c r="I30" s="53"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="62" t="s">
         <v>1157</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1158</v>
       </c>
-      <c r="C31" s="61" t="s">
+      <c r="C31" s="63" t="s">
         <v>1159</v>
       </c>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
       <c r="F31" s="55"/>
       <c r="G31" s="53"/>
       <c r="H31" s="53"/>
       <c r="I31" s="53"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="63"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="45" t="s">
         <v>1160</v>
       </c>
-      <c r="C32" s="61" t="s">
+      <c r="C32" s="63" t="s">
         <v>1161</v>
       </c>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
       <c r="F32" s="55"/>
       <c r="G32" s="53"/>
       <c r="H32" s="53"/>
       <c r="I32" s="53"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="62" t="s">
         <v>1162</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1135</v>
       </c>
-      <c r="C33" s="61" t="s">
+      <c r="C33" s="63" t="s">
         <v>1163</v>
       </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
       <c r="F33" s="55"/>
       <c r="G33" s="53"/>
       <c r="H33" s="53"/>
       <c r="I33" s="53"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="63"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="45" t="s">
         <v>1164</v>
       </c>
-      <c r="C34" s="61" t="s">
+      <c r="C34" s="63" t="s">
         <v>1165</v>
       </c>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
       <c r="F34" s="55"/>
       <c r="G34" s="53"/>
       <c r="H34" s="53"/>
       <c r="I34" s="53"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="63"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="45" t="s">
         <v>1166</v>
       </c>
-      <c r="C35" s="61" t="s">
+      <c r="C35" s="63" t="s">
         <v>1167</v>
       </c>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
       <c r="F35" s="55"/>
       <c r="G35" s="53"/>
       <c r="H35" s="53"/>
       <c r="I35" s="53"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="63"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="61" t="s">
+      <c r="C36" s="63" t="s">
         <v>1168</v>
       </c>
-      <c r="D36" s="61"/>
-      <c r="E36" s="61"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
       <c r="F36" s="55"/>
       <c r="G36" s="53"/>
       <c r="H36" s="53"/>
@@ -22278,97 +22302,97 @@
       <c r="B37" s="45" t="s">
         <v>1150</v>
       </c>
-      <c r="C37" s="61" t="s">
+      <c r="C37" s="63" t="s">
         <v>1170</v>
       </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
       <c r="F37" s="55"/>
       <c r="G37" s="53"/>
       <c r="H37" s="53"/>
       <c r="I37" s="53"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="62" t="s">
         <v>1171</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1172</v>
       </c>
-      <c r="C38" s="61" t="s">
+      <c r="C38" s="63" t="s">
         <v>1173</v>
       </c>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
       <c r="F38" s="55"/>
       <c r="G38" s="53"/>
       <c r="H38" s="53"/>
       <c r="I38" s="53"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="63"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="45" t="s">
         <v>1174</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="63" t="s">
         <v>1175</v>
       </c>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
       <c r="F39" s="55"/>
       <c r="G39" s="53"/>
       <c r="H39" s="53"/>
       <c r="I39" s="53"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="63"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="45" t="s">
         <v>1176</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="63" t="s">
         <v>1177</v>
       </c>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
       <c r="F40" s="55"/>
       <c r="G40" s="53"/>
       <c r="H40" s="53"/>
       <c r="I40" s="53"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="63" t="s">
+      <c r="A41" s="62" t="s">
         <v>1178</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1179</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="63" t="s">
         <v>1180</v>
       </c>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
       <c r="F41" s="55"/>
       <c r="G41" s="53"/>
       <c r="H41" s="53"/>
       <c r="I41" s="53"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="63"/>
+      <c r="A42" s="62"/>
       <c r="B42" s="45" t="s">
         <v>1181</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="63" t="s">
         <v>1182</v>
       </c>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
       <c r="F42" s="55"/>
       <c r="G42" s="53"/>
       <c r="H42" s="53"/>
       <c r="I42" s="53"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="63"/>
+      <c r="A43" s="62"/>
       <c r="B43" s="45" t="s">
         <v>1183</v>
       </c>
@@ -22383,47 +22407,47 @@
       <c r="I43" s="53"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="63"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="45" t="s">
         <v>1185</v>
       </c>
-      <c r="C44" s="62" t="s">
+      <c r="C44" s="61" t="s">
         <v>1186</v>
       </c>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
       <c r="F44" s="55"/>
       <c r="G44" s="53"/>
       <c r="H44" s="53"/>
       <c r="I44" s="53"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="63" t="s">
+      <c r="A45" s="62" t="s">
         <v>1187</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1188</v>
       </c>
-      <c r="C45" s="62" t="s">
+      <c r="C45" s="61" t="s">
         <v>1189</v>
       </c>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
       <c r="F45" s="55"/>
       <c r="G45" s="53"/>
       <c r="H45" s="53"/>
       <c r="I45" s="53"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="63"/>
+      <c r="A46" s="62"/>
       <c r="B46" s="45" t="s">
         <v>1190</v>
       </c>
-      <c r="C46" s="62" t="s">
+      <c r="C46" s="61" t="s">
         <v>1191</v>
       </c>
-      <c r="D46" s="62"/>
-      <c r="E46" s="62"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
       <c r="F46" s="55"/>
       <c r="G46" s="53"/>
       <c r="H46" s="53"/>
@@ -22436,11 +22460,11 @@
       <c r="B47" s="45" t="s">
         <v>1150</v>
       </c>
-      <c r="C47" s="62" t="s">
+      <c r="C47" s="61" t="s">
         <v>1193</v>
       </c>
-      <c r="D47" s="62"/>
-      <c r="E47" s="62"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
       <c r="F47" s="55"/>
       <c r="G47" s="53"/>
       <c r="H47" s="53"/>
@@ -22453,165 +22477,165 @@
       <c r="B48" s="45" t="s">
         <v>1195</v>
       </c>
-      <c r="C48" s="62" t="s">
+      <c r="C48" s="61" t="s">
         <v>1196</v>
       </c>
-      <c r="D48" s="62"/>
-      <c r="E48" s="62"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
       <c r="F48" s="55"/>
       <c r="G48" s="53"/>
       <c r="H48" s="53"/>
       <c r="I48" s="53"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="63" t="s">
+      <c r="A49" s="62" t="s">
         <v>1197</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1198</v>
       </c>
-      <c r="C49" s="62" t="s">
+      <c r="C49" s="61" t="s">
         <v>1199</v>
       </c>
-      <c r="D49" s="62"/>
-      <c r="E49" s="62"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
       <c r="F49" s="55"/>
       <c r="G49" s="53"/>
       <c r="H49" s="53"/>
       <c r="I49" s="53"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="63"/>
+      <c r="A50" s="62"/>
       <c r="B50" s="45" t="s">
         <v>1200</v>
       </c>
-      <c r="C50" s="62" t="s">
+      <c r="C50" s="61" t="s">
         <v>1201</v>
       </c>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
       <c r="F50" s="55"/>
       <c r="G50" s="53"/>
       <c r="H50" s="53"/>
       <c r="I50" s="53"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="63"/>
+      <c r="A51" s="62"/>
       <c r="B51" s="45" t="s">
         <v>1145</v>
       </c>
-      <c r="C51" s="62" t="s">
+      <c r="C51" s="61" t="s">
         <v>1202</v>
       </c>
-      <c r="D51" s="62"/>
-      <c r="E51" s="62"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
       <c r="F51" s="55"/>
       <c r="G51" s="53"/>
       <c r="H51" s="53"/>
       <c r="I51" s="53"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="63"/>
+      <c r="A52" s="62"/>
       <c r="B52" s="45" t="s">
         <v>1203</v>
       </c>
-      <c r="C52" s="62" t="s">
+      <c r="C52" s="61" t="s">
         <v>1204</v>
       </c>
-      <c r="D52" s="62"/>
-      <c r="E52" s="62"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
       <c r="F52" s="55"/>
       <c r="G52" s="53"/>
       <c r="H52" s="53"/>
       <c r="I52" s="53"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="63"/>
+      <c r="A53" s="62"/>
       <c r="B53" s="45" t="s">
         <v>1141</v>
       </c>
-      <c r="C53" s="62" t="s">
+      <c r="C53" s="61" t="s">
         <v>1205</v>
       </c>
-      <c r="D53" s="62"/>
-      <c r="E53" s="62"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
       <c r="F53" s="55"/>
       <c r="G53" s="53"/>
       <c r="H53" s="53"/>
       <c r="I53" s="53"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="63" t="s">
+      <c r="A54" s="62" t="s">
         <v>1206</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1207</v>
       </c>
-      <c r="C54" s="62" t="s">
+      <c r="C54" s="61" t="s">
         <v>1208</v>
       </c>
-      <c r="D54" s="62"/>
-      <c r="E54" s="62"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
       <c r="F54" s="55"/>
       <c r="G54" s="53"/>
       <c r="H54" s="53"/>
       <c r="I54" s="53"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="63"/>
+      <c r="A55" s="62"/>
       <c r="B55" s="5" t="s">
         <v>1209</v>
       </c>
-      <c r="C55" s="62" t="s">
+      <c r="C55" s="61" t="s">
         <v>1210</v>
       </c>
-      <c r="D55" s="62"/>
-      <c r="E55" s="62"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
       <c r="F55" s="55"/>
       <c r="G55" s="53"/>
       <c r="H55" s="53"/>
       <c r="I55" s="53"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="63"/>
+      <c r="A56" s="62"/>
       <c r="B56" s="5" t="s">
         <v>1211</v>
       </c>
-      <c r="C56" s="62" t="s">
+      <c r="C56" s="61" t="s">
         <v>1212</v>
       </c>
-      <c r="D56" s="62"/>
-      <c r="E56" s="62"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="61"/>
       <c r="F56" s="55"/>
       <c r="G56" s="53"/>
       <c r="H56" s="53"/>
       <c r="I56" s="53"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="63"/>
+      <c r="A57" s="62"/>
       <c r="B57" s="5" t="s">
         <v>1213</v>
       </c>
-      <c r="C57" s="62" t="s">
+      <c r="C57" s="61" t="s">
         <v>1214</v>
       </c>
-      <c r="D57" s="62"/>
-      <c r="E57" s="62"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
       <c r="F57" s="55"/>
       <c r="G57" s="53"/>
       <c r="H57" s="53"/>
       <c r="I57" s="53"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="63"/>
+      <c r="A58" s="62"/>
       <c r="B58" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="C58" s="62" t="s">
+      <c r="C58" s="61" t="s">
         <v>1216</v>
       </c>
-      <c r="D58" s="62"/>
-      <c r="E58" s="62"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
       <c r="F58" s="55"/>
       <c r="G58" s="53"/>
       <c r="H58" s="53"/>
@@ -22624,88 +22648,88 @@
       <c r="B59" s="5" t="s">
         <v>1150</v>
       </c>
-      <c r="C59" s="62" t="s">
+      <c r="C59" s="61" t="s">
         <v>1218</v>
       </c>
-      <c r="D59" s="62"/>
-      <c r="E59" s="62"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="61"/>
       <c r="F59" s="55"/>
       <c r="G59" s="53"/>
       <c r="H59" s="53"/>
       <c r="I59" s="53"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="63" t="s">
+      <c r="A60" s="62" t="s">
         <v>1219</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1220</v>
       </c>
-      <c r="C60" s="62" t="s">
+      <c r="C60" s="61" t="s">
         <v>1221</v>
       </c>
-      <c r="D60" s="62"/>
-      <c r="E60" s="62"/>
+      <c r="D60" s="61"/>
+      <c r="E60" s="61"/>
       <c r="F60" s="55"/>
       <c r="G60" s="53"/>
       <c r="H60" s="53"/>
       <c r="I60" s="53"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="63"/>
+      <c r="A61" s="62"/>
       <c r="B61" s="5" t="s">
         <v>1222</v>
       </c>
-      <c r="C61" s="62" t="s">
+      <c r="C61" s="61" t="s">
         <v>1223</v>
       </c>
-      <c r="D61" s="62"/>
-      <c r="E61" s="62"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="61"/>
       <c r="F61" s="55"/>
       <c r="G61" s="53"/>
       <c r="H61" s="53"/>
       <c r="I61" s="53"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="63"/>
+      <c r="A62" s="62"/>
       <c r="B62" s="5" t="s">
         <v>1224</v>
       </c>
-      <c r="C62" s="62" t="s">
+      <c r="C62" s="61" t="s">
         <v>1225</v>
       </c>
-      <c r="D62" s="62"/>
-      <c r="E62" s="62"/>
+      <c r="D62" s="61"/>
+      <c r="E62" s="61"/>
       <c r="F62" s="55"/>
       <c r="G62" s="53"/>
       <c r="H62" s="53"/>
       <c r="I62" s="53"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="63"/>
+      <c r="A63" s="62"/>
       <c r="B63" s="5" t="s">
         <v>1226</v>
       </c>
-      <c r="C63" s="62" t="s">
+      <c r="C63" s="61" t="s">
         <v>1227</v>
       </c>
-      <c r="D63" s="62"/>
-      <c r="E63" s="62"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="61"/>
       <c r="F63" s="55"/>
       <c r="G63" s="53"/>
       <c r="H63" s="53"/>
       <c r="I63" s="53"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="63"/>
+      <c r="A64" s="62"/>
       <c r="B64" s="5" t="s">
         <v>1228</v>
       </c>
-      <c r="C64" s="62" t="s">
+      <c r="C64" s="61" t="s">
         <v>1229</v>
       </c>
-      <c r="D64" s="62"/>
-      <c r="E64" s="62"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
       <c r="F64" s="55"/>
       <c r="G64" s="53"/>
       <c r="H64" s="53"/>
@@ -22713,36 +22737,66 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="C64:E64"/>
     <mergeCell ref="A54:A58"/>
@@ -22767,66 +22821,36 @@
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -24162,6 +24186,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -24174,13 +24205,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24551,6 +24575,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F9:I9"/>
@@ -24558,18 +24594,6 @@
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:I11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -25036,19 +25060,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -25062,6 +25073,19 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -25925,19 +25949,33 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="C23:D23"/>
@@ -25951,33 +25989,19 @@
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26462,13 +26486,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -26479,6 +26496,13 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -26886,6 +26910,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -26898,11 +26927,6 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26934,6 +26958,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -27162,27 +27206,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27199,29 +27248,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:sparkles: Make encounter mandatory for MedicationAdministration profile
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\db\dt4h\common-data-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D370FAE-026F-461D-84E2-BD6E2AA943C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560E2985-0F0D-4B95-9286-6CD5F561977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" tabRatio="901" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="901" firstSheet="7" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -6615,22 +6615,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7635,7 +7635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1770B9A2-CDA6-4E37-82EC-A9C07EE24319}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -8010,6 +8010,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -8020,13 +8027,6 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8726,7 +8726,7 @@
         <v>463</v>
       </c>
       <c r="D39" s="57"/>
-      <c r="E39" s="59"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="62" t="s">
         <v>464</v>
       </c>
@@ -8741,11 +8741,11 @@
       <c r="B40" s="42" t="s">
         <v>466</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="59" t="s">
         <v>467</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
@@ -8758,11 +8758,11 @@
       <c r="B41" s="42" t="s">
         <v>469</v>
       </c>
-      <c r="C41" s="60" t="s">
+      <c r="C41" s="59" t="s">
         <v>470</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="61"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
@@ -8775,11 +8775,11 @@
       <c r="B42" s="42" t="s">
         <v>472</v>
       </c>
-      <c r="C42" s="60" t="s">
+      <c r="C42" s="59" t="s">
         <v>473</v>
       </c>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
@@ -8792,11 +8792,11 @@
       <c r="B43" s="42" t="s">
         <v>475</v>
       </c>
-      <c r="C43" s="60" t="s">
+      <c r="C43" s="59" t="s">
         <v>1380</v>
       </c>
-      <c r="D43" s="60"/>
-      <c r="E43" s="61"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="58"/>
       <c r="G43" s="56"/>
       <c r="H43" s="56"/>
@@ -8809,11 +8809,11 @@
       <c r="B44" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="59" t="s">
         <v>478</v>
       </c>
-      <c r="D44" s="60"/>
-      <c r="E44" s="61"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="60"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
@@ -8826,11 +8826,11 @@
       <c r="B45" s="42" t="s">
         <v>480</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="59" t="s">
         <v>481</v>
       </c>
-      <c r="D45" s="60"/>
-      <c r="E45" s="61"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
@@ -8843,11 +8843,11 @@
       <c r="B46" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="C46" s="60" t="s">
+      <c r="C46" s="59" t="s">
         <v>484</v>
       </c>
-      <c r="D46" s="60"/>
-      <c r="E46" s="61"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -8860,11 +8860,11 @@
       <c r="B47" s="42" t="s">
         <v>486</v>
       </c>
-      <c r="C47" s="60" t="s">
+      <c r="C47" s="59" t="s">
         <v>487</v>
       </c>
-      <c r="D47" s="60"/>
-      <c r="E47" s="61"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -8877,11 +8877,11 @@
       <c r="B48" s="42" t="s">
         <v>489</v>
       </c>
-      <c r="C48" s="60" t="s">
+      <c r="C48" s="59" t="s">
         <v>490</v>
       </c>
-      <c r="D48" s="60"/>
-      <c r="E48" s="61"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="60"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
@@ -8894,11 +8894,11 @@
       <c r="B49" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="C49" s="60" t="s">
+      <c r="C49" s="59" t="s">
         <v>493</v>
       </c>
-      <c r="D49" s="60"/>
-      <c r="E49" s="61"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="60"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
@@ -8911,11 +8911,11 @@
       <c r="B50" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="C50" s="60" t="s">
+      <c r="C50" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="D50" s="60"/>
-      <c r="E50" s="61"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="60"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
@@ -8928,11 +8928,11 @@
       <c r="B51" s="42" t="s">
         <v>498</v>
       </c>
-      <c r="C51" s="60" t="s">
+      <c r="C51" s="59" t="s">
         <v>499</v>
       </c>
-      <c r="D51" s="60"/>
-      <c r="E51" s="61"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="60"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
@@ -8945,11 +8945,11 @@
       <c r="B52" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="60" t="s">
+      <c r="C52" s="59" t="s">
         <v>502</v>
       </c>
-      <c r="D52" s="60"/>
-      <c r="E52" s="61"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="60"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
@@ -8962,11 +8962,11 @@
       <c r="B53" s="42" t="s">
         <v>504</v>
       </c>
-      <c r="C53" s="60" t="s">
+      <c r="C53" s="59" t="s">
         <v>505</v>
       </c>
-      <c r="D53" s="60"/>
-      <c r="E53" s="61"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="60"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
@@ -8979,11 +8979,11 @@
       <c r="B54" s="42" t="s">
         <v>507</v>
       </c>
-      <c r="C54" s="60" t="s">
+      <c r="C54" s="59" t="s">
         <v>508</v>
       </c>
-      <c r="D54" s="60"/>
-      <c r="E54" s="61"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="60"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
@@ -8996,11 +8996,11 @@
       <c r="B55" s="42" t="s">
         <v>510</v>
       </c>
-      <c r="C55" s="60" t="s">
+      <c r="C55" s="59" t="s">
         <v>511</v>
       </c>
-      <c r="D55" s="60"/>
-      <c r="E55" s="61"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
@@ -9013,11 +9013,11 @@
       <c r="B56" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C56" s="60" t="s">
+      <c r="C56" s="59" t="s">
         <v>514</v>
       </c>
-      <c r="D56" s="60"/>
-      <c r="E56" s="61"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="60"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
@@ -9030,11 +9030,11 @@
       <c r="B57" s="42" t="s">
         <v>516</v>
       </c>
-      <c r="C57" s="60" t="s">
+      <c r="C57" s="59" t="s">
         <v>517</v>
       </c>
-      <c r="D57" s="60"/>
-      <c r="E57" s="61"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="60"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
@@ -9047,11 +9047,11 @@
       <c r="B58" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="C58" s="60" t="s">
+      <c r="C58" s="59" t="s">
         <v>520</v>
       </c>
-      <c r="D58" s="60"/>
-      <c r="E58" s="61"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="60"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -9064,11 +9064,11 @@
       <c r="B59" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="C59" s="60" t="s">
+      <c r="C59" s="59" t="s">
         <v>523</v>
       </c>
-      <c r="D59" s="60"/>
-      <c r="E59" s="61"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
@@ -9081,11 +9081,11 @@
       <c r="B60" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="C60" s="60" t="s">
+      <c r="C60" s="59" t="s">
         <v>526</v>
       </c>
-      <c r="D60" s="60"/>
-      <c r="E60" s="61"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
@@ -9098,11 +9098,11 @@
       <c r="B61" s="42" t="s">
         <v>528</v>
       </c>
-      <c r="C61" s="60" t="s">
+      <c r="C61" s="59" t="s">
         <v>529</v>
       </c>
-      <c r="D61" s="60"/>
-      <c r="E61" s="61"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="60"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
@@ -9115,11 +9115,11 @@
       <c r="B62" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C62" s="60" t="s">
+      <c r="C62" s="59" t="s">
         <v>532</v>
       </c>
-      <c r="D62" s="60"/>
-      <c r="E62" s="61"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="60"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
@@ -9132,11 +9132,11 @@
       <c r="B63" s="42" t="s">
         <v>534</v>
       </c>
-      <c r="C63" s="60" t="s">
+      <c r="C63" s="59" t="s">
         <v>535</v>
       </c>
-      <c r="D63" s="60"/>
-      <c r="E63" s="61"/>
+      <c r="D63" s="59"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
@@ -9149,11 +9149,11 @@
       <c r="B64" s="42" t="s">
         <v>536</v>
       </c>
-      <c r="C64" s="60" t="s">
+      <c r="C64" s="59" t="s">
         <v>537</v>
       </c>
-      <c r="D64" s="60"/>
-      <c r="E64" s="61"/>
+      <c r="D64" s="59"/>
+      <c r="E64" s="60"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -9166,11 +9166,11 @@
       <c r="B65" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C65" s="60" t="s">
+      <c r="C65" s="59" t="s">
         <v>540</v>
       </c>
-      <c r="D65" s="60"/>
-      <c r="E65" s="61"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="60"/>
       <c r="F65" s="58"/>
       <c r="G65" s="56"/>
       <c r="H65" s="56"/>
@@ -9183,11 +9183,11 @@
       <c r="B66" s="42" t="s">
         <v>542</v>
       </c>
-      <c r="C66" s="60" t="s">
+      <c r="C66" s="59" t="s">
         <v>543</v>
       </c>
-      <c r="D66" s="60"/>
-      <c r="E66" s="61"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="60"/>
       <c r="F66" s="58"/>
       <c r="G66" s="56"/>
       <c r="H66" s="56"/>
@@ -9200,11 +9200,11 @@
       <c r="B67" s="42" t="s">
         <v>545</v>
       </c>
-      <c r="C67" s="60" t="s">
+      <c r="C67" s="59" t="s">
         <v>546</v>
       </c>
-      <c r="D67" s="60"/>
-      <c r="E67" s="61"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="60"/>
       <c r="F67" s="58"/>
       <c r="G67" s="56"/>
       <c r="H67" s="56"/>
@@ -9217,11 +9217,11 @@
       <c r="B68" s="42" t="s">
         <v>548</v>
       </c>
-      <c r="C68" s="60" t="s">
+      <c r="C68" s="59" t="s">
         <v>549</v>
       </c>
-      <c r="D68" s="60"/>
-      <c r="E68" s="61"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="60"/>
       <c r="F68" s="58"/>
       <c r="G68" s="56"/>
       <c r="H68" s="56"/>
@@ -9234,11 +9234,11 @@
       <c r="B69" s="42" t="s">
         <v>551</v>
       </c>
-      <c r="C69" s="60" t="s">
+      <c r="C69" s="59" t="s">
         <v>552</v>
       </c>
-      <c r="D69" s="60"/>
-      <c r="E69" s="61"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="60"/>
       <c r="F69" s="58"/>
       <c r="G69" s="56"/>
       <c r="H69" s="56"/>
@@ -9251,11 +9251,11 @@
       <c r="B70" s="42" t="s">
         <v>554</v>
       </c>
-      <c r="C70" s="60" t="s">
+      <c r="C70" s="59" t="s">
         <v>555</v>
       </c>
-      <c r="D70" s="60"/>
-      <c r="E70" s="61"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="60"/>
       <c r="F70" s="58"/>
       <c r="G70" s="56"/>
       <c r="H70" s="56"/>
@@ -9268,11 +9268,11 @@
       <c r="B71" s="42" t="s">
         <v>557</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="59" t="s">
         <v>558</v>
       </c>
-      <c r="D71" s="60"/>
-      <c r="E71" s="61"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="60"/>
       <c r="F71" s="58"/>
       <c r="G71" s="56"/>
       <c r="H71" s="56"/>
@@ -9285,11 +9285,11 @@
       <c r="B72" s="42" t="s">
         <v>560</v>
       </c>
-      <c r="C72" s="60" t="s">
+      <c r="C72" s="59" t="s">
         <v>561</v>
       </c>
-      <c r="D72" s="60"/>
-      <c r="E72" s="61"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="60"/>
       <c r="F72" s="58"/>
       <c r="G72" s="56"/>
       <c r="H72" s="56"/>
@@ -9302,11 +9302,11 @@
       <c r="B73" s="42" t="s">
         <v>563</v>
       </c>
-      <c r="C73" s="60" t="s">
+      <c r="C73" s="59" t="s">
         <v>564</v>
       </c>
-      <c r="D73" s="60"/>
-      <c r="E73" s="61"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="60"/>
       <c r="F73" s="58"/>
       <c r="G73" s="56"/>
       <c r="H73" s="56"/>
@@ -9319,11 +9319,11 @@
       <c r="B74" s="42" t="s">
         <v>566</v>
       </c>
-      <c r="C74" s="60" t="s">
+      <c r="C74" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="D74" s="60"/>
-      <c r="E74" s="61"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="60"/>
       <c r="F74" s="58"/>
       <c r="G74" s="56"/>
       <c r="H74" s="56"/>
@@ -9336,11 +9336,11 @@
       <c r="B75" s="42" t="s">
         <v>569</v>
       </c>
-      <c r="C75" s="60" t="s">
+      <c r="C75" s="59" t="s">
         <v>570</v>
       </c>
-      <c r="D75" s="60"/>
-      <c r="E75" s="61"/>
+      <c r="D75" s="59"/>
+      <c r="E75" s="60"/>
       <c r="F75" s="58"/>
       <c r="G75" s="56"/>
       <c r="H75" s="56"/>
@@ -9353,11 +9353,11 @@
       <c r="B76" s="42" t="s">
         <v>572</v>
       </c>
-      <c r="C76" s="60" t="s">
+      <c r="C76" s="59" t="s">
         <v>573</v>
       </c>
-      <c r="D76" s="60"/>
-      <c r="E76" s="61"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="60"/>
       <c r="F76" s="58"/>
       <c r="G76" s="56"/>
       <c r="H76" s="56"/>
@@ -9370,11 +9370,11 @@
       <c r="B77" s="42" t="s">
         <v>575</v>
       </c>
-      <c r="C77" s="60" t="s">
+      <c r="C77" s="59" t="s">
         <v>576</v>
       </c>
-      <c r="D77" s="60"/>
-      <c r="E77" s="61"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="60"/>
       <c r="F77" s="58"/>
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
@@ -9387,11 +9387,11 @@
       <c r="B78" s="42" t="s">
         <v>578</v>
       </c>
-      <c r="C78" s="60" t="s">
+      <c r="C78" s="59" t="s">
         <v>579</v>
       </c>
-      <c r="D78" s="60"/>
-      <c r="E78" s="61"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="60"/>
       <c r="F78" s="58"/>
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
@@ -9404,11 +9404,11 @@
       <c r="B79" s="42" t="s">
         <v>581</v>
       </c>
-      <c r="C79" s="60" t="s">
+      <c r="C79" s="59" t="s">
         <v>582</v>
       </c>
-      <c r="D79" s="60"/>
-      <c r="E79" s="61"/>
+      <c r="D79" s="59"/>
+      <c r="E79" s="60"/>
       <c r="F79" s="58"/>
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
@@ -9421,11 +9421,11 @@
       <c r="B80" s="42" t="s">
         <v>584</v>
       </c>
-      <c r="C80" s="60" t="s">
+      <c r="C80" s="59" t="s">
         <v>585</v>
       </c>
-      <c r="D80" s="60"/>
-      <c r="E80" s="61"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="60"/>
       <c r="F80" s="58"/>
       <c r="G80" s="56"/>
       <c r="H80" s="56"/>
@@ -9438,11 +9438,11 @@
       <c r="B81" s="42" t="s">
         <v>587</v>
       </c>
-      <c r="C81" s="60" t="s">
+      <c r="C81" s="59" t="s">
         <v>588</v>
       </c>
-      <c r="D81" s="60"/>
-      <c r="E81" s="61"/>
+      <c r="D81" s="59"/>
+      <c r="E81" s="60"/>
       <c r="F81" s="58"/>
       <c r="G81" s="56"/>
       <c r="H81" s="56"/>
@@ -9450,36 +9450,69 @@
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="F48:I48"/>
     <mergeCell ref="F49:I49"/>
@@ -9504,69 +9537,36 @@
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="F55:I55"/>
     <mergeCell ref="F56:I56"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10430,14 +10430,41 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -10454,41 +10481,14 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -11678,7 +11678,7 @@
       <c r="H37" s="56"/>
       <c r="I37" s="56"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A38" s="49" t="s">
         <v>1786</v>
       </c>
@@ -11699,38 +11699,11 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -11747,11 +11720,38 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E20" xr:uid="{7FAB08B6-9907-44B4-A82A-4A3E200D36A8}">
@@ -12848,25 +12848,23 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
     <mergeCell ref="F43:I43"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="F31:I31"/>
@@ -12879,23 +12877,25 @@
     <mergeCell ref="F38:I38"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -18494,24 +18494,87 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="111">
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H140:K140"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H134:K134"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="H136:K136"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="H138:K138"/>
+    <mergeCell ref="H139:K139"/>
+    <mergeCell ref="H128:K128"/>
+    <mergeCell ref="H129:K129"/>
+    <mergeCell ref="H130:K130"/>
+    <mergeCell ref="H131:K131"/>
+    <mergeCell ref="H132:K132"/>
+    <mergeCell ref="H133:K133"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="H125:K125"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="H121:K121"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="H106:K106"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H66:K66"/>
+    <mergeCell ref="H67:K67"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="H73:K73"/>
     <mergeCell ref="H59:K59"/>
     <mergeCell ref="H60:K60"/>
     <mergeCell ref="H61:K61"/>
@@ -18524,87 +18587,24 @@
     <mergeCell ref="H55:K55"/>
     <mergeCell ref="H57:K57"/>
     <mergeCell ref="H58:K58"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="H67:K67"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="H106:K106"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="H134:K134"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="H136:K136"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="H138:K138"/>
-    <mergeCell ref="H139:K139"/>
-    <mergeCell ref="H128:K128"/>
-    <mergeCell ref="H129:K129"/>
-    <mergeCell ref="H130:K130"/>
-    <mergeCell ref="H131:K131"/>
-    <mergeCell ref="H132:K132"/>
-    <mergeCell ref="H133:K133"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="H140:K140"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H45:K45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20680,6 +20680,31 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="F110:I110"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="F112:I112"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F108:I108"/>
+    <mergeCell ref="F109:I109"/>
     <mergeCell ref="F100:I100"/>
     <mergeCell ref="F101:I101"/>
     <mergeCell ref="F102:I102"/>
@@ -20690,31 +20715,6 @@
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
-    <mergeCell ref="F110:I110"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="F112:I112"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="F109:I109"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -22893,49 +22893,108 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="C80:D80"/>
@@ -22960,108 +23019,49 @@
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23607,7 +23607,7 @@
         <v>1115</v>
       </c>
       <c r="D14" s="57"/>
-      <c r="E14" s="59"/>
+      <c r="E14" s="61"/>
       <c r="F14" s="62" t="s">
         <v>464</v>
       </c>
@@ -23616,201 +23616,201 @@
       <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="65" t="s">
         <v>1116</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1117</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="59" t="s">
         <v>1118</v>
       </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="58"/>
       <c r="G15" s="56"/>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="42" t="s">
         <v>1119</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="59" t="s">
         <v>1120</v>
       </c>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
       <c r="F16" s="58"/>
       <c r="G16" s="56"/>
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="42" t="s">
         <v>1121</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="59" t="s">
         <v>1122</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="58"/>
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="42" t="s">
         <v>1123</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="60" t="s">
         <v>1124</v>
       </c>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="58"/>
       <c r="G18" s="56"/>
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="42" t="s">
         <v>1125</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="60" t="s">
         <v>1126</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="58"/>
       <c r="G19" s="56"/>
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="66" t="s">
         <v>1127</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="60" t="s">
         <v>1129</v>
       </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
       <c r="F20" s="58"/>
       <c r="G20" s="56"/>
       <c r="H20" s="56"/>
       <c r="I20" s="56"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="66"/>
       <c r="B21" s="42" t="s">
         <v>1130</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="60" t="s">
         <v>1131</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
       <c r="F21" s="58"/>
       <c r="G21" s="56"/>
       <c r="H21" s="56"/>
       <c r="I21" s="56"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="66"/>
       <c r="B22" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="60" t="s">
         <v>1133</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
       <c r="F22" s="58"/>
       <c r="G22" s="56"/>
       <c r="H22" s="56"/>
       <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="66"/>
       <c r="B23" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="60" t="s">
         <v>1135</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="58"/>
       <c r="G23" s="56"/>
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="66" t="s">
         <v>1136</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="60" t="s">
         <v>1137</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
       <c r="F24" s="58"/>
       <c r="G24" s="56"/>
       <c r="H24" s="56"/>
       <c r="I24" s="56"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="42" t="s">
         <v>1138</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="60" t="s">
         <v>1139</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
       <c r="F25" s="58"/>
       <c r="G25" s="56"/>
       <c r="H25" s="56"/>
       <c r="I25" s="56"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="60" t="s">
         <v>1140</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
       <c r="F26" s="58"/>
       <c r="G26" s="56"/>
       <c r="H26" s="56"/>
       <c r="I26" s="56"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="66"/>
       <c r="B27" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="64" t="s">
         <v>1141</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="58"/>
       <c r="G27" s="56"/>
       <c r="H27" s="56"/>
@@ -23823,137 +23823,137 @@
       <c r="B28" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="64" t="s">
         <v>1144</v>
       </c>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
       <c r="F28" s="58"/>
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
       <c r="I28" s="56"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="66" t="s">
         <v>1145</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1146</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="64" t="s">
         <v>1147</v>
       </c>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
       <c r="F29" s="58"/>
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="56"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="66"/>
       <c r="B30" s="45" t="s">
         <v>1148</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="64" t="s">
         <v>1149</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
       <c r="F30" s="58"/>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
       <c r="I30" s="56"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="66" t="s">
         <v>1150</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1151</v>
       </c>
-      <c r="C31" s="66" t="s">
+      <c r="C31" s="64" t="s">
         <v>1152</v>
       </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
       <c r="F31" s="58"/>
       <c r="G31" s="56"/>
       <c r="H31" s="56"/>
       <c r="I31" s="56"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="66"/>
       <c r="B32" s="45" t="s">
         <v>1153</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="64" t="s">
         <v>1154</v>
       </c>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="58"/>
       <c r="G32" s="56"/>
       <c r="H32" s="56"/>
       <c r="I32" s="56"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="66" t="s">
         <v>1155</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1128</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="64" t="s">
         <v>1156</v>
       </c>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
       <c r="F33" s="58"/>
       <c r="G33" s="56"/>
       <c r="H33" s="56"/>
       <c r="I33" s="56"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
+      <c r="A34" s="66"/>
       <c r="B34" s="45" t="s">
         <v>1157</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="64" t="s">
         <v>1158</v>
       </c>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
       <c r="F34" s="58"/>
       <c r="G34" s="56"/>
       <c r="H34" s="56"/>
       <c r="I34" s="56"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="65"/>
+      <c r="A35" s="66"/>
       <c r="B35" s="45" t="s">
         <v>1159</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="64" t="s">
         <v>1160</v>
       </c>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
       <c r="F35" s="58"/>
       <c r="G35" s="56"/>
       <c r="H35" s="56"/>
       <c r="I35" s="56"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="65"/>
+      <c r="A36" s="66"/>
       <c r="B36" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="66" t="s">
+      <c r="C36" s="64" t="s">
         <v>1161</v>
       </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
       <c r="F36" s="58"/>
       <c r="G36" s="56"/>
       <c r="H36" s="56"/>
@@ -23966,97 +23966,97 @@
       <c r="B37" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="66" t="s">
+      <c r="C37" s="64" t="s">
         <v>1163</v>
       </c>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
       <c r="F37" s="58"/>
       <c r="G37" s="56"/>
       <c r="H37" s="56"/>
       <c r="I37" s="56"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="65" t="s">
+      <c r="A38" s="66" t="s">
         <v>1164</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1165</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="64" t="s">
         <v>1166</v>
       </c>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="58"/>
       <c r="G38" s="56"/>
       <c r="H38" s="56"/>
       <c r="I38" s="56"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="65"/>
+      <c r="A39" s="66"/>
       <c r="B39" s="45" t="s">
         <v>1167</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="64" t="s">
         <v>1168</v>
       </c>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="58"/>
       <c r="G39" s="56"/>
       <c r="H39" s="56"/>
       <c r="I39" s="56"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="65"/>
+      <c r="A40" s="66"/>
       <c r="B40" s="45" t="s">
         <v>1169</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="64" t="s">
         <v>1170</v>
       </c>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
       <c r="I40" s="56"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="65" t="s">
+      <c r="A41" s="66" t="s">
         <v>1171</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1172</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="64" t="s">
         <v>1173</v>
       </c>
-      <c r="D41" s="66"/>
-      <c r="E41" s="66"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="65"/>
+      <c r="A42" s="66"/>
       <c r="B42" s="45" t="s">
         <v>1174</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="64" t="s">
         <v>1175</v>
       </c>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
       <c r="I42" s="56"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="65"/>
+      <c r="A43" s="66"/>
       <c r="B43" s="45" t="s">
         <v>1176</v>
       </c>
@@ -24071,47 +24071,47 @@
       <c r="I43" s="56"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="65"/>
+      <c r="A44" s="66"/>
       <c r="B44" s="45" t="s">
         <v>1178</v>
       </c>
-      <c r="C44" s="64" t="s">
+      <c r="C44" s="65" t="s">
         <v>1179</v>
       </c>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
       <c r="I44" s="56"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="65" t="s">
+      <c r="A45" s="66" t="s">
         <v>1180</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1181</v>
       </c>
-      <c r="C45" s="64" t="s">
+      <c r="C45" s="65" t="s">
         <v>1182</v>
       </c>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="65"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="45" t="s">
         <v>1183</v>
       </c>
-      <c r="C46" s="64" t="s">
+      <c r="C46" s="65" t="s">
         <v>1184</v>
       </c>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -24124,11 +24124,11 @@
       <c r="B47" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C47" s="64" t="s">
+      <c r="C47" s="65" t="s">
         <v>1186</v>
       </c>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -24141,165 +24141,165 @@
       <c r="B48" s="45" t="s">
         <v>1188</v>
       </c>
-      <c r="C48" s="64" t="s">
+      <c r="C48" s="65" t="s">
         <v>1189</v>
       </c>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
       <c r="I48" s="56"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="65" t="s">
+      <c r="A49" s="66" t="s">
         <v>1190</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1191</v>
       </c>
-      <c r="C49" s="64" t="s">
+      <c r="C49" s="65" t="s">
         <v>1192</v>
       </c>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
       <c r="I49" s="56"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="65"/>
+      <c r="A50" s="66"/>
       <c r="B50" s="45" t="s">
         <v>1193</v>
       </c>
-      <c r="C50" s="64" t="s">
+      <c r="C50" s="65" t="s">
         <v>1194</v>
       </c>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
       <c r="I50" s="56"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="65"/>
+      <c r="A51" s="66"/>
       <c r="B51" s="45" t="s">
         <v>1138</v>
       </c>
-      <c r="C51" s="64" t="s">
+      <c r="C51" s="65" t="s">
         <v>1195</v>
       </c>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="65"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
       <c r="I51" s="56"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="65"/>
+      <c r="A52" s="66"/>
       <c r="B52" s="45" t="s">
         <v>1196</v>
       </c>
-      <c r="C52" s="64" t="s">
+      <c r="C52" s="65" t="s">
         <v>1197</v>
       </c>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
       <c r="I52" s="56"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="65"/>
+      <c r="A53" s="66"/>
       <c r="B53" s="45" t="s">
         <v>1134</v>
       </c>
-      <c r="C53" s="64" t="s">
+      <c r="C53" s="65" t="s">
         <v>1198</v>
       </c>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="65"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
       <c r="I53" s="56"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="65" t="s">
+      <c r="A54" s="66" t="s">
         <v>1199</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1200</v>
       </c>
-      <c r="C54" s="64" t="s">
+      <c r="C54" s="65" t="s">
         <v>1201</v>
       </c>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="65"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
       <c r="I54" s="56"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="65"/>
+      <c r="A55" s="66"/>
       <c r="B55" s="5" t="s">
         <v>1202</v>
       </c>
-      <c r="C55" s="64" t="s">
+      <c r="C55" s="65" t="s">
         <v>1203</v>
       </c>
-      <c r="D55" s="64"/>
-      <c r="E55" s="64"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="65"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
       <c r="I55" s="56"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="65"/>
+      <c r="A56" s="66"/>
       <c r="B56" s="5" t="s">
         <v>1204</v>
       </c>
-      <c r="C56" s="64" t="s">
+      <c r="C56" s="65" t="s">
         <v>1205</v>
       </c>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="65"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
       <c r="I56" s="56"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="65"/>
+      <c r="A57" s="66"/>
       <c r="B57" s="5" t="s">
         <v>1206</v>
       </c>
-      <c r="C57" s="64" t="s">
+      <c r="C57" s="65" t="s">
         <v>1207</v>
       </c>
-      <c r="D57" s="64"/>
-      <c r="E57" s="64"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="65"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
       <c r="I57" s="56"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="65"/>
+      <c r="A58" s="66"/>
       <c r="B58" s="5" t="s">
         <v>1208</v>
       </c>
-      <c r="C58" s="64" t="s">
+      <c r="C58" s="65" t="s">
         <v>1209</v>
       </c>
-      <c r="D58" s="64"/>
-      <c r="E58" s="64"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="65"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -24312,88 +24312,88 @@
       <c r="B59" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C59" s="64" t="s">
+      <c r="C59" s="65" t="s">
         <v>1211</v>
       </c>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="65"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
       <c r="I59" s="56"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="65" t="s">
+      <c r="A60" s="66" t="s">
         <v>1212</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1213</v>
       </c>
-      <c r="C60" s="64" t="s">
+      <c r="C60" s="65" t="s">
         <v>1214</v>
       </c>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="65"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
       <c r="I60" s="56"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="65"/>
+      <c r="A61" s="66"/>
       <c r="B61" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="C61" s="64" t="s">
+      <c r="C61" s="65" t="s">
         <v>1216</v>
       </c>
-      <c r="D61" s="64"/>
-      <c r="E61" s="64"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="65"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
       <c r="I61" s="56"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="65"/>
+      <c r="A62" s="66"/>
       <c r="B62" s="5" t="s">
         <v>1217</v>
       </c>
-      <c r="C62" s="64" t="s">
+      <c r="C62" s="65" t="s">
         <v>1218</v>
       </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
       <c r="I62" s="56"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="65"/>
+      <c r="A63" s="66"/>
       <c r="B63" s="5" t="s">
         <v>1219</v>
       </c>
-      <c r="C63" s="64" t="s">
+      <c r="C63" s="65" t="s">
         <v>1220</v>
       </c>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
       <c r="I63" s="56"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="65"/>
+      <c r="A64" s="66"/>
       <c r="B64" s="5" t="s">
         <v>1221</v>
       </c>
-      <c r="C64" s="64" t="s">
+      <c r="C64" s="65" t="s">
         <v>1222</v>
       </c>
-      <c r="D64" s="64"/>
-      <c r="E64" s="64"/>
+      <c r="D64" s="65"/>
+      <c r="E64" s="65"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -24401,30 +24401,72 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
@@ -24449,72 +24491,30 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -24548,8 +24548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D896FB-80F4-4D48-93D9-6DBE34ADD468}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24656,10 +24656,10 @@
         <v>332</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>1225</v>
@@ -25850,13 +25850,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -25869,6 +25862,13 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26239,6 +26239,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
@@ -26246,18 +26258,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -26724,6 +26724,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -26737,19 +26750,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -27634,33 +27634,19 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:I23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="C24:D24"/>
@@ -27674,19 +27660,33 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28171,6 +28171,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -28181,13 +28188,6 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -28595,11 +28595,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -28612,6 +28607,11 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28643,15 +28643,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -28880,6 +28871,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -28892,14 +28892,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28914,6 +28906,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
:sparkles: Create a value set to keep medication groups
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1712959C-6C56-43A7-889C-EC087B7CDBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C41954-E627-47D4-A5D7-A10007BC4501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -859,7 +859,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4323" uniqueCount="1795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4361" uniqueCount="1810">
   <si>
     <t>Required</t>
   </si>
@@ -6259,6 +6259,51 @@
   </si>
   <si>
     <t>Date and time or the time period of the socioeconomic status observation indicated with a start and end time. If the smoking status is current, the ending time of the time period should be omitted. If there is no date and no other record, we can assume that the patient has had that status all her life.</t>
+  </si>
+  <si>
+    <t>List of medication groups</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>RASi</t>
+  </si>
+  <si>
+    <t>ACEI</t>
+  </si>
+  <si>
+    <t>ARB</t>
+  </si>
+  <si>
+    <t>ARNI</t>
+  </si>
+  <si>
+    <t>MRA</t>
+  </si>
+  <si>
+    <t>CCB</t>
+  </si>
+  <si>
+    <t>VasoD</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>OAC</t>
+  </si>
+  <si>
+    <t>Digoxin</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>AAD</t>
+  </si>
+  <si>
+    <t>SGLT2I</t>
   </si>
 </sst>
 </file>
@@ -6615,22 +6660,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8010,13 +8055,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -8027,6 +8065,13 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8726,7 +8771,7 @@
         <v>463</v>
       </c>
       <c r="D39" s="57"/>
-      <c r="E39" s="61"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="62" t="s">
         <v>464</v>
       </c>
@@ -8741,11 +8786,11 @@
       <c r="B40" s="42" t="s">
         <v>466</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="60" t="s">
         <v>467</v>
       </c>
-      <c r="D40" s="59"/>
-      <c r="E40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="61"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
@@ -8758,11 +8803,11 @@
       <c r="B41" s="42" t="s">
         <v>469</v>
       </c>
-      <c r="C41" s="59" t="s">
+      <c r="C41" s="60" t="s">
         <v>470</v>
       </c>
-      <c r="D41" s="59"/>
-      <c r="E41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="61"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
@@ -8775,11 +8820,11 @@
       <c r="B42" s="42" t="s">
         <v>472</v>
       </c>
-      <c r="C42" s="59" t="s">
+      <c r="C42" s="60" t="s">
         <v>473</v>
       </c>
-      <c r="D42" s="59"/>
-      <c r="E42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="61"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
@@ -8792,11 +8837,11 @@
       <c r="B43" s="42" t="s">
         <v>475</v>
       </c>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="60" t="s">
         <v>1380</v>
       </c>
-      <c r="D43" s="59"/>
-      <c r="E43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="61"/>
       <c r="F43" s="58"/>
       <c r="G43" s="56"/>
       <c r="H43" s="56"/>
@@ -8809,11 +8854,11 @@
       <c r="B44" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="60" t="s">
         <v>478</v>
       </c>
-      <c r="D44" s="59"/>
-      <c r="E44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="61"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
@@ -8826,11 +8871,11 @@
       <c r="B45" s="42" t="s">
         <v>480</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="60" t="s">
         <v>481</v>
       </c>
-      <c r="D45" s="59"/>
-      <c r="E45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="61"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
@@ -8843,11 +8888,11 @@
       <c r="B46" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="60" t="s">
         <v>484</v>
       </c>
-      <c r="D46" s="59"/>
-      <c r="E46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="61"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -8860,11 +8905,11 @@
       <c r="B47" s="42" t="s">
         <v>486</v>
       </c>
-      <c r="C47" s="59" t="s">
+      <c r="C47" s="60" t="s">
         <v>487</v>
       </c>
-      <c r="D47" s="59"/>
-      <c r="E47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="61"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -8877,11 +8922,11 @@
       <c r="B48" s="42" t="s">
         <v>489</v>
       </c>
-      <c r="C48" s="59" t="s">
+      <c r="C48" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="D48" s="59"/>
-      <c r="E48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="61"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
@@ -8894,11 +8939,11 @@
       <c r="B49" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="C49" s="59" t="s">
+      <c r="C49" s="60" t="s">
         <v>493</v>
       </c>
-      <c r="D49" s="59"/>
-      <c r="E49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="61"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
@@ -8911,11 +8956,11 @@
       <c r="B50" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="C50" s="59" t="s">
+      <c r="C50" s="60" t="s">
         <v>496</v>
       </c>
-      <c r="D50" s="59"/>
-      <c r="E50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="61"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
@@ -8928,11 +8973,11 @@
       <c r="B51" s="42" t="s">
         <v>498</v>
       </c>
-      <c r="C51" s="59" t="s">
+      <c r="C51" s="60" t="s">
         <v>499</v>
       </c>
-      <c r="D51" s="59"/>
-      <c r="E51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="61"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
@@ -8945,11 +8990,11 @@
       <c r="B52" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="59" t="s">
+      <c r="C52" s="60" t="s">
         <v>502</v>
       </c>
-      <c r="D52" s="59"/>
-      <c r="E52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="61"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
@@ -8962,11 +9007,11 @@
       <c r="B53" s="42" t="s">
         <v>504</v>
       </c>
-      <c r="C53" s="59" t="s">
+      <c r="C53" s="60" t="s">
         <v>505</v>
       </c>
-      <c r="D53" s="59"/>
-      <c r="E53" s="60"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="61"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
@@ -8979,11 +9024,11 @@
       <c r="B54" s="42" t="s">
         <v>507</v>
       </c>
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="60" t="s">
         <v>508</v>
       </c>
-      <c r="D54" s="59"/>
-      <c r="E54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="61"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
@@ -8996,11 +9041,11 @@
       <c r="B55" s="42" t="s">
         <v>510</v>
       </c>
-      <c r="C55" s="59" t="s">
+      <c r="C55" s="60" t="s">
         <v>511</v>
       </c>
-      <c r="D55" s="59"/>
-      <c r="E55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="61"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
@@ -9013,11 +9058,11 @@
       <c r="B56" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C56" s="59" t="s">
+      <c r="C56" s="60" t="s">
         <v>514</v>
       </c>
-      <c r="D56" s="59"/>
-      <c r="E56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="61"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
@@ -9030,11 +9075,11 @@
       <c r="B57" s="42" t="s">
         <v>516</v>
       </c>
-      <c r="C57" s="59" t="s">
+      <c r="C57" s="60" t="s">
         <v>517</v>
       </c>
-      <c r="D57" s="59"/>
-      <c r="E57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="61"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
@@ -9047,11 +9092,11 @@
       <c r="B58" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="C58" s="59" t="s">
+      <c r="C58" s="60" t="s">
         <v>520</v>
       </c>
-      <c r="D58" s="59"/>
-      <c r="E58" s="60"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="61"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -9064,11 +9109,11 @@
       <c r="B59" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="C59" s="59" t="s">
+      <c r="C59" s="60" t="s">
         <v>523</v>
       </c>
-      <c r="D59" s="59"/>
-      <c r="E59" s="60"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="61"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
@@ -9081,11 +9126,11 @@
       <c r="B60" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="C60" s="59" t="s">
+      <c r="C60" s="60" t="s">
         <v>526</v>
       </c>
-      <c r="D60" s="59"/>
-      <c r="E60" s="60"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="61"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
@@ -9098,11 +9143,11 @@
       <c r="B61" s="42" t="s">
         <v>528</v>
       </c>
-      <c r="C61" s="59" t="s">
+      <c r="C61" s="60" t="s">
         <v>529</v>
       </c>
-      <c r="D61" s="59"/>
-      <c r="E61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="61"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
@@ -9115,11 +9160,11 @@
       <c r="B62" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C62" s="59" t="s">
+      <c r="C62" s="60" t="s">
         <v>532</v>
       </c>
-      <c r="D62" s="59"/>
-      <c r="E62" s="60"/>
+      <c r="D62" s="60"/>
+      <c r="E62" s="61"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
@@ -9132,11 +9177,11 @@
       <c r="B63" s="42" t="s">
         <v>534</v>
       </c>
-      <c r="C63" s="59" t="s">
+      <c r="C63" s="60" t="s">
         <v>535</v>
       </c>
-      <c r="D63" s="59"/>
-      <c r="E63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="61"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
@@ -9149,11 +9194,11 @@
       <c r="B64" s="42" t="s">
         <v>536</v>
       </c>
-      <c r="C64" s="59" t="s">
+      <c r="C64" s="60" t="s">
         <v>537</v>
       </c>
-      <c r="D64" s="59"/>
-      <c r="E64" s="60"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="61"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -9166,11 +9211,11 @@
       <c r="B65" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C65" s="59" t="s">
+      <c r="C65" s="60" t="s">
         <v>540</v>
       </c>
-      <c r="D65" s="59"/>
-      <c r="E65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="61"/>
       <c r="F65" s="58"/>
       <c r="G65" s="56"/>
       <c r="H65" s="56"/>
@@ -9183,11 +9228,11 @@
       <c r="B66" s="42" t="s">
         <v>542</v>
       </c>
-      <c r="C66" s="59" t="s">
+      <c r="C66" s="60" t="s">
         <v>543</v>
       </c>
-      <c r="D66" s="59"/>
-      <c r="E66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
       <c r="F66" s="58"/>
       <c r="G66" s="56"/>
       <c r="H66" s="56"/>
@@ -9200,11 +9245,11 @@
       <c r="B67" s="42" t="s">
         <v>545</v>
       </c>
-      <c r="C67" s="59" t="s">
+      <c r="C67" s="60" t="s">
         <v>546</v>
       </c>
-      <c r="D67" s="59"/>
-      <c r="E67" s="60"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="61"/>
       <c r="F67" s="58"/>
       <c r="G67" s="56"/>
       <c r="H67" s="56"/>
@@ -9217,11 +9262,11 @@
       <c r="B68" s="42" t="s">
         <v>548</v>
       </c>
-      <c r="C68" s="59" t="s">
+      <c r="C68" s="60" t="s">
         <v>549</v>
       </c>
-      <c r="D68" s="59"/>
-      <c r="E68" s="60"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="61"/>
       <c r="F68" s="58"/>
       <c r="G68" s="56"/>
       <c r="H68" s="56"/>
@@ -9234,11 +9279,11 @@
       <c r="B69" s="42" t="s">
         <v>551</v>
       </c>
-      <c r="C69" s="59" t="s">
+      <c r="C69" s="60" t="s">
         <v>552</v>
       </c>
-      <c r="D69" s="59"/>
-      <c r="E69" s="60"/>
+      <c r="D69" s="60"/>
+      <c r="E69" s="61"/>
       <c r="F69" s="58"/>
       <c r="G69" s="56"/>
       <c r="H69" s="56"/>
@@ -9251,11 +9296,11 @@
       <c r="B70" s="42" t="s">
         <v>554</v>
       </c>
-      <c r="C70" s="59" t="s">
+      <c r="C70" s="60" t="s">
         <v>555</v>
       </c>
-      <c r="D70" s="59"/>
-      <c r="E70" s="60"/>
+      <c r="D70" s="60"/>
+      <c r="E70" s="61"/>
       <c r="F70" s="58"/>
       <c r="G70" s="56"/>
       <c r="H70" s="56"/>
@@ -9268,11 +9313,11 @@
       <c r="B71" s="42" t="s">
         <v>557</v>
       </c>
-      <c r="C71" s="59" t="s">
+      <c r="C71" s="60" t="s">
         <v>558</v>
       </c>
-      <c r="D71" s="59"/>
-      <c r="E71" s="60"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="61"/>
       <c r="F71" s="58"/>
       <c r="G71" s="56"/>
       <c r="H71" s="56"/>
@@ -9285,11 +9330,11 @@
       <c r="B72" s="42" t="s">
         <v>560</v>
       </c>
-      <c r="C72" s="59" t="s">
+      <c r="C72" s="60" t="s">
         <v>561</v>
       </c>
-      <c r="D72" s="59"/>
-      <c r="E72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="61"/>
       <c r="F72" s="58"/>
       <c r="G72" s="56"/>
       <c r="H72" s="56"/>
@@ -9302,11 +9347,11 @@
       <c r="B73" s="42" t="s">
         <v>563</v>
       </c>
-      <c r="C73" s="59" t="s">
+      <c r="C73" s="60" t="s">
         <v>564</v>
       </c>
-      <c r="D73" s="59"/>
-      <c r="E73" s="60"/>
+      <c r="D73" s="60"/>
+      <c r="E73" s="61"/>
       <c r="F73" s="58"/>
       <c r="G73" s="56"/>
       <c r="H73" s="56"/>
@@ -9319,11 +9364,11 @@
       <c r="B74" s="42" t="s">
         <v>566</v>
       </c>
-      <c r="C74" s="59" t="s">
+      <c r="C74" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="D74" s="59"/>
-      <c r="E74" s="60"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="61"/>
       <c r="F74" s="58"/>
       <c r="G74" s="56"/>
       <c r="H74" s="56"/>
@@ -9336,11 +9381,11 @@
       <c r="B75" s="42" t="s">
         <v>569</v>
       </c>
-      <c r="C75" s="59" t="s">
+      <c r="C75" s="60" t="s">
         <v>570</v>
       </c>
-      <c r="D75" s="59"/>
-      <c r="E75" s="60"/>
+      <c r="D75" s="60"/>
+      <c r="E75" s="61"/>
       <c r="F75" s="58"/>
       <c r="G75" s="56"/>
       <c r="H75" s="56"/>
@@ -9353,11 +9398,11 @@
       <c r="B76" s="42" t="s">
         <v>572</v>
       </c>
-      <c r="C76" s="59" t="s">
+      <c r="C76" s="60" t="s">
         <v>573</v>
       </c>
-      <c r="D76" s="59"/>
-      <c r="E76" s="60"/>
+      <c r="D76" s="60"/>
+      <c r="E76" s="61"/>
       <c r="F76" s="58"/>
       <c r="G76" s="56"/>
       <c r="H76" s="56"/>
@@ -9370,11 +9415,11 @@
       <c r="B77" s="42" t="s">
         <v>575</v>
       </c>
-      <c r="C77" s="59" t="s">
+      <c r="C77" s="60" t="s">
         <v>576</v>
       </c>
-      <c r="D77" s="59"/>
-      <c r="E77" s="60"/>
+      <c r="D77" s="60"/>
+      <c r="E77" s="61"/>
       <c r="F77" s="58"/>
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
@@ -9387,11 +9432,11 @@
       <c r="B78" s="42" t="s">
         <v>578</v>
       </c>
-      <c r="C78" s="59" t="s">
+      <c r="C78" s="60" t="s">
         <v>579</v>
       </c>
-      <c r="D78" s="59"/>
-      <c r="E78" s="60"/>
+      <c r="D78" s="60"/>
+      <c r="E78" s="61"/>
       <c r="F78" s="58"/>
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
@@ -9404,11 +9449,11 @@
       <c r="B79" s="42" t="s">
         <v>581</v>
       </c>
-      <c r="C79" s="59" t="s">
+      <c r="C79" s="60" t="s">
         <v>582</v>
       </c>
-      <c r="D79" s="59"/>
-      <c r="E79" s="60"/>
+      <c r="D79" s="60"/>
+      <c r="E79" s="61"/>
       <c r="F79" s="58"/>
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
@@ -9421,11 +9466,11 @@
       <c r="B80" s="42" t="s">
         <v>584</v>
       </c>
-      <c r="C80" s="59" t="s">
+      <c r="C80" s="60" t="s">
         <v>585</v>
       </c>
-      <c r="D80" s="59"/>
-      <c r="E80" s="60"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="61"/>
       <c r="F80" s="58"/>
       <c r="G80" s="56"/>
       <c r="H80" s="56"/>
@@ -9438,11 +9483,11 @@
       <c r="B81" s="42" t="s">
         <v>587</v>
       </c>
-      <c r="C81" s="59" t="s">
+      <c r="C81" s="60" t="s">
         <v>588</v>
       </c>
-      <c r="D81" s="59"/>
-      <c r="E81" s="60"/>
+      <c r="D81" s="60"/>
+      <c r="E81" s="61"/>
       <c r="F81" s="58"/>
       <c r="G81" s="56"/>
       <c r="H81" s="56"/>
@@ -9450,6 +9495,99 @@
     </row>
   </sheetData>
   <mergeCells count="117">
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F44:I44"/>
@@ -9474,99 +9612,6 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10430,41 +10475,14 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -10481,14 +10499,41 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -11699,11 +11744,38 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -11720,38 +11792,11 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E20" xr:uid="{7FAB08B6-9907-44B4-A82A-4A3E200D36A8}">
@@ -11791,7 +11836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BB695D-4821-4052-8E37-D71854C5F317}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -12848,23 +12893,25 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
     <mergeCell ref="F43:I43"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="F31:I31"/>
@@ -12877,25 +12924,23 @@
     <mergeCell ref="F38:I38"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -18494,15 +18539,96 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="111">
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="H140:K140"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H59:K59"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="H61:K61"/>
+    <mergeCell ref="H62:K62"/>
+    <mergeCell ref="H63:K63"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H57:K57"/>
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H66:K66"/>
+    <mergeCell ref="H67:K67"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="H106:K106"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="H125:K125"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="H121:K121"/>
     <mergeCell ref="H134:K134"/>
     <mergeCell ref="H135:K135"/>
     <mergeCell ref="H136:K136"/>
@@ -18515,96 +18641,15 @@
     <mergeCell ref="H131:K131"/>
     <mergeCell ref="H132:K132"/>
     <mergeCell ref="H133:K133"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="H106:K106"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="H67:K67"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="H59:K59"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="H61:K61"/>
-    <mergeCell ref="H62:K62"/>
-    <mergeCell ref="H63:K63"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H57:K57"/>
-    <mergeCell ref="H58:K58"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H140:K140"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20680,31 +20725,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="F110:I110"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="F112:I112"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="F109:I109"/>
     <mergeCell ref="F100:I100"/>
     <mergeCell ref="F101:I101"/>
     <mergeCell ref="F102:I102"/>
@@ -20715,6 +20735,31 @@
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
+    <mergeCell ref="F110:I110"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="F112:I112"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F108:I108"/>
+    <mergeCell ref="F109:I109"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -22893,48 +22938,109 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
@@ -22959,109 +23065,48 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23607,7 +23652,7 @@
         <v>1115</v>
       </c>
       <c r="D14" s="57"/>
-      <c r="E14" s="61"/>
+      <c r="E14" s="59"/>
       <c r="F14" s="62" t="s">
         <v>464</v>
       </c>
@@ -23616,201 +23661,201 @@
       <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="64" t="s">
         <v>1116</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1117</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="60" t="s">
         <v>1118</v>
       </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
       <c r="F15" s="58"/>
       <c r="G15" s="56"/>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="42" t="s">
         <v>1119</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="60" t="s">
         <v>1120</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
       <c r="F16" s="58"/>
       <c r="G16" s="56"/>
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="42" t="s">
         <v>1121</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="60" t="s">
         <v>1122</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="61"/>
       <c r="F17" s="58"/>
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="42" t="s">
         <v>1123</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="61" t="s">
         <v>1124</v>
       </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
       <c r="F18" s="58"/>
       <c r="G18" s="56"/>
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="42" t="s">
         <v>1125</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="61" t="s">
         <v>1126</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
       <c r="F19" s="58"/>
       <c r="G19" s="56"/>
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="65" t="s">
         <v>1127</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="61" t="s">
         <v>1129</v>
       </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
       <c r="F20" s="58"/>
       <c r="G20" s="56"/>
       <c r="H20" s="56"/>
       <c r="I20" s="56"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="66"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="42" t="s">
         <v>1130</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="61" t="s">
         <v>1131</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
       <c r="F21" s="58"/>
       <c r="G21" s="56"/>
       <c r="H21" s="56"/>
       <c r="I21" s="56"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="66"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="61" t="s">
         <v>1133</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="58"/>
       <c r="G22" s="56"/>
       <c r="H22" s="56"/>
       <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="66"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="61" t="s">
         <v>1135</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="58"/>
       <c r="G23" s="56"/>
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="65" t="s">
         <v>1136</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="61" t="s">
         <v>1137</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
       <c r="F24" s="58"/>
       <c r="G24" s="56"/>
       <c r="H24" s="56"/>
       <c r="I24" s="56"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="42" t="s">
         <v>1138</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="61" t="s">
         <v>1139</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
       <c r="F25" s="58"/>
       <c r="G25" s="56"/>
       <c r="H25" s="56"/>
       <c r="I25" s="56"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="66"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="61" t="s">
         <v>1140</v>
       </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
       <c r="F26" s="58"/>
       <c r="G26" s="56"/>
       <c r="H26" s="56"/>
       <c r="I26" s="56"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="66"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="66" t="s">
         <v>1141</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
       <c r="F27" s="58"/>
       <c r="G27" s="56"/>
       <c r="H27" s="56"/>
@@ -23823,137 +23868,137 @@
       <c r="B28" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="66" t="s">
         <v>1144</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
       <c r="F28" s="58"/>
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
       <c r="I28" s="56"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="65" t="s">
         <v>1145</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1146</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="66" t="s">
         <v>1147</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
       <c r="F29" s="58"/>
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="56"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="66"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="45" t="s">
         <v>1148</v>
       </c>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="66" t="s">
         <v>1149</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
       <c r="F30" s="58"/>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
       <c r="I30" s="56"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="65" t="s">
         <v>1150</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1151</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="66" t="s">
         <v>1152</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
       <c r="F31" s="58"/>
       <c r="G31" s="56"/>
       <c r="H31" s="56"/>
       <c r="I31" s="56"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="66"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="45" t="s">
         <v>1153</v>
       </c>
-      <c r="C32" s="64" t="s">
+      <c r="C32" s="66" t="s">
         <v>1154</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
       <c r="F32" s="58"/>
       <c r="G32" s="56"/>
       <c r="H32" s="56"/>
       <c r="I32" s="56"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="65" t="s">
         <v>1155</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1128</v>
       </c>
-      <c r="C33" s="64" t="s">
+      <c r="C33" s="66" t="s">
         <v>1156</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
       <c r="F33" s="58"/>
       <c r="G33" s="56"/>
       <c r="H33" s="56"/>
       <c r="I33" s="56"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="66"/>
+      <c r="A34" s="65"/>
       <c r="B34" s="45" t="s">
         <v>1157</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="66" t="s">
         <v>1158</v>
       </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
       <c r="F34" s="58"/>
       <c r="G34" s="56"/>
       <c r="H34" s="56"/>
       <c r="I34" s="56"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="66"/>
+      <c r="A35" s="65"/>
       <c r="B35" s="45" t="s">
         <v>1159</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="66" t="s">
         <v>1160</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
       <c r="F35" s="58"/>
       <c r="G35" s="56"/>
       <c r="H35" s="56"/>
       <c r="I35" s="56"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
+      <c r="A36" s="65"/>
       <c r="B36" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="66" t="s">
         <v>1161</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
       <c r="F36" s="58"/>
       <c r="G36" s="56"/>
       <c r="H36" s="56"/>
@@ -23966,97 +24011,97 @@
       <c r="B37" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="64" t="s">
+      <c r="C37" s="66" t="s">
         <v>1163</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
       <c r="F37" s="58"/>
       <c r="G37" s="56"/>
       <c r="H37" s="56"/>
       <c r="I37" s="56"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="65" t="s">
         <v>1164</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1165</v>
       </c>
-      <c r="C38" s="64" t="s">
+      <c r="C38" s="66" t="s">
         <v>1166</v>
       </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
       <c r="F38" s="58"/>
       <c r="G38" s="56"/>
       <c r="H38" s="56"/>
       <c r="I38" s="56"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="66"/>
+      <c r="A39" s="65"/>
       <c r="B39" s="45" t="s">
         <v>1167</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="C39" s="66" t="s">
         <v>1168</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
       <c r="F39" s="58"/>
       <c r="G39" s="56"/>
       <c r="H39" s="56"/>
       <c r="I39" s="56"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="66"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="45" t="s">
         <v>1169</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="C40" s="66" t="s">
         <v>1170</v>
       </c>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
       <c r="I40" s="56"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="65" t="s">
         <v>1171</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1172</v>
       </c>
-      <c r="C41" s="64" t="s">
+      <c r="C41" s="66" t="s">
         <v>1173</v>
       </c>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="66"/>
+      <c r="A42" s="65"/>
       <c r="B42" s="45" t="s">
         <v>1174</v>
       </c>
-      <c r="C42" s="64" t="s">
+      <c r="C42" s="66" t="s">
         <v>1175</v>
       </c>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
       <c r="I42" s="56"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="66"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="45" t="s">
         <v>1176</v>
       </c>
@@ -24071,47 +24116,47 @@
       <c r="I43" s="56"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="66"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="45" t="s">
         <v>1178</v>
       </c>
-      <c r="C44" s="65" t="s">
+      <c r="C44" s="64" t="s">
         <v>1179</v>
       </c>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
       <c r="I44" s="56"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="65" t="s">
         <v>1180</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1181</v>
       </c>
-      <c r="C45" s="65" t="s">
+      <c r="C45" s="64" t="s">
         <v>1182</v>
       </c>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="66"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="45" t="s">
         <v>1183</v>
       </c>
-      <c r="C46" s="65" t="s">
+      <c r="C46" s="64" t="s">
         <v>1184</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="65"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -24124,11 +24169,11 @@
       <c r="B47" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C47" s="65" t="s">
+      <c r="C47" s="64" t="s">
         <v>1186</v>
       </c>
-      <c r="D47" s="65"/>
-      <c r="E47" s="65"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -24141,165 +24186,165 @@
       <c r="B48" s="45" t="s">
         <v>1188</v>
       </c>
-      <c r="C48" s="65" t="s">
+      <c r="C48" s="64" t="s">
         <v>1189</v>
       </c>
-      <c r="D48" s="65"/>
-      <c r="E48" s="65"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
       <c r="I48" s="56"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="65" t="s">
         <v>1190</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1191</v>
       </c>
-      <c r="C49" s="65" t="s">
+      <c r="C49" s="64" t="s">
         <v>1192</v>
       </c>
-      <c r="D49" s="65"/>
-      <c r="E49" s="65"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
       <c r="I49" s="56"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="66"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="45" t="s">
         <v>1193</v>
       </c>
-      <c r="C50" s="65" t="s">
+      <c r="C50" s="64" t="s">
         <v>1194</v>
       </c>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
       <c r="I50" s="56"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="66"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="45" t="s">
         <v>1138</v>
       </c>
-      <c r="C51" s="65" t="s">
+      <c r="C51" s="64" t="s">
         <v>1195</v>
       </c>
-      <c r="D51" s="65"/>
-      <c r="E51" s="65"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
       <c r="I51" s="56"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="66"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="45" t="s">
         <v>1196</v>
       </c>
-      <c r="C52" s="65" t="s">
+      <c r="C52" s="64" t="s">
         <v>1197</v>
       </c>
-      <c r="D52" s="65"/>
-      <c r="E52" s="65"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="64"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
       <c r="I52" s="56"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="66"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="45" t="s">
         <v>1134</v>
       </c>
-      <c r="C53" s="65" t="s">
+      <c r="C53" s="64" t="s">
         <v>1198</v>
       </c>
-      <c r="D53" s="65"/>
-      <c r="E53" s="65"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
       <c r="I53" s="56"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="65" t="s">
         <v>1199</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1200</v>
       </c>
-      <c r="C54" s="65" t="s">
+      <c r="C54" s="64" t="s">
         <v>1201</v>
       </c>
-      <c r="D54" s="65"/>
-      <c r="E54" s="65"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="64"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
       <c r="I54" s="56"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="66"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="5" t="s">
         <v>1202</v>
       </c>
-      <c r="C55" s="65" t="s">
+      <c r="C55" s="64" t="s">
         <v>1203</v>
       </c>
-      <c r="D55" s="65"/>
-      <c r="E55" s="65"/>
+      <c r="D55" s="64"/>
+      <c r="E55" s="64"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
       <c r="I55" s="56"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="66"/>
+      <c r="A56" s="65"/>
       <c r="B56" s="5" t="s">
         <v>1204</v>
       </c>
-      <c r="C56" s="65" t="s">
+      <c r="C56" s="64" t="s">
         <v>1205</v>
       </c>
-      <c r="D56" s="65"/>
-      <c r="E56" s="65"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
       <c r="I56" s="56"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="66"/>
+      <c r="A57" s="65"/>
       <c r="B57" s="5" t="s">
         <v>1206</v>
       </c>
-      <c r="C57" s="65" t="s">
+      <c r="C57" s="64" t="s">
         <v>1207</v>
       </c>
-      <c r="D57" s="65"/>
-      <c r="E57" s="65"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="64"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
       <c r="I57" s="56"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="66"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="5" t="s">
         <v>1208</v>
       </c>
-      <c r="C58" s="65" t="s">
+      <c r="C58" s="64" t="s">
         <v>1209</v>
       </c>
-      <c r="D58" s="65"/>
-      <c r="E58" s="65"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -24312,88 +24357,88 @@
       <c r="B59" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C59" s="65" t="s">
+      <c r="C59" s="64" t="s">
         <v>1211</v>
       </c>
-      <c r="D59" s="65"/>
-      <c r="E59" s="65"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
       <c r="I59" s="56"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="65" t="s">
         <v>1212</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1213</v>
       </c>
-      <c r="C60" s="65" t="s">
+      <c r="C60" s="64" t="s">
         <v>1214</v>
       </c>
-      <c r="D60" s="65"/>
-      <c r="E60" s="65"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
       <c r="I60" s="56"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="66"/>
+      <c r="A61" s="65"/>
       <c r="B61" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="64" t="s">
         <v>1216</v>
       </c>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
       <c r="I61" s="56"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="66"/>
+      <c r="A62" s="65"/>
       <c r="B62" s="5" t="s">
         <v>1217</v>
       </c>
-      <c r="C62" s="65" t="s">
+      <c r="C62" s="64" t="s">
         <v>1218</v>
       </c>
-      <c r="D62" s="65"/>
-      <c r="E62" s="65"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
       <c r="I62" s="56"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="66"/>
+      <c r="A63" s="65"/>
       <c r="B63" s="5" t="s">
         <v>1219</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C63" s="64" t="s">
         <v>1220</v>
       </c>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
       <c r="I63" s="56"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="66"/>
+      <c r="A64" s="65"/>
       <c r="B64" s="5" t="s">
         <v>1221</v>
       </c>
-      <c r="C64" s="65" t="s">
+      <c r="C64" s="64" t="s">
         <v>1222</v>
       </c>
-      <c r="D64" s="65"/>
-      <c r="E64" s="65"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -24401,36 +24446,66 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="C64:E64"/>
     <mergeCell ref="A54:A58"/>
@@ -24455,66 +24530,36 @@
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -24546,10 +24591,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D896FB-80F4-4D48-93D9-6DBE34ADD468}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24749,7 +24794,255 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
     </row>
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C14" s="58"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C15" s="58"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C18" s="58"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C19" s="58"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>563</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C20" s="58"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C21" s="58"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C22" s="58"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C23" s="58"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C24" s="58"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C25" s="58"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C26" s="58"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C27" s="58"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C28" s="58"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C29" s="58"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C30" s="58"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+    </row>
   </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -25850,6 +26143,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -25862,13 +26162,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26239,6 +26532,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F9:I9"/>
@@ -26246,18 +26551,6 @@
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:I11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -26724,19 +27017,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -26750,6 +27030,19 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -27634,19 +27927,33 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="C24:D24"/>
@@ -27660,33 +27967,19 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28171,13 +28464,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -28188,6 +28474,13 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -28595,6 +28888,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -28607,11 +28905,6 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28643,6 +28936,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -28871,27 +29184,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28908,29 +29226,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:sparkles: Remove max cardinality restriction from cause of death mapping
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560E2985-0F0D-4B95-9286-6CD5F561977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB75181C-62B1-42B2-8E73-4975B72E46A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="901" firstSheet="7" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -6615,22 +6615,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8010,13 +8010,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -8027,6 +8020,13 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8726,7 +8726,7 @@
         <v>463</v>
       </c>
       <c r="D39" s="57"/>
-      <c r="E39" s="61"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="62" t="s">
         <v>464</v>
       </c>
@@ -8741,11 +8741,11 @@
       <c r="B40" s="42" t="s">
         <v>466</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="60" t="s">
         <v>467</v>
       </c>
-      <c r="D40" s="59"/>
-      <c r="E40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="61"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
@@ -8758,11 +8758,11 @@
       <c r="B41" s="42" t="s">
         <v>469</v>
       </c>
-      <c r="C41" s="59" t="s">
+      <c r="C41" s="60" t="s">
         <v>470</v>
       </c>
-      <c r="D41" s="59"/>
-      <c r="E41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="61"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
@@ -8775,11 +8775,11 @@
       <c r="B42" s="42" t="s">
         <v>472</v>
       </c>
-      <c r="C42" s="59" t="s">
+      <c r="C42" s="60" t="s">
         <v>473</v>
       </c>
-      <c r="D42" s="59"/>
-      <c r="E42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="61"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
@@ -8792,11 +8792,11 @@
       <c r="B43" s="42" t="s">
         <v>475</v>
       </c>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="60" t="s">
         <v>1380</v>
       </c>
-      <c r="D43" s="59"/>
-      <c r="E43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="61"/>
       <c r="F43" s="58"/>
       <c r="G43" s="56"/>
       <c r="H43" s="56"/>
@@ -8809,11 +8809,11 @@
       <c r="B44" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="60" t="s">
         <v>478</v>
       </c>
-      <c r="D44" s="59"/>
-      <c r="E44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="61"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
@@ -8826,11 +8826,11 @@
       <c r="B45" s="42" t="s">
         <v>480</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="60" t="s">
         <v>481</v>
       </c>
-      <c r="D45" s="59"/>
-      <c r="E45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="61"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
@@ -8843,11 +8843,11 @@
       <c r="B46" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="60" t="s">
         <v>484</v>
       </c>
-      <c r="D46" s="59"/>
-      <c r="E46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="61"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -8860,11 +8860,11 @@
       <c r="B47" s="42" t="s">
         <v>486</v>
       </c>
-      <c r="C47" s="59" t="s">
+      <c r="C47" s="60" t="s">
         <v>487</v>
       </c>
-      <c r="D47" s="59"/>
-      <c r="E47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="61"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -8877,11 +8877,11 @@
       <c r="B48" s="42" t="s">
         <v>489</v>
       </c>
-      <c r="C48" s="59" t="s">
+      <c r="C48" s="60" t="s">
         <v>490</v>
       </c>
-      <c r="D48" s="59"/>
-      <c r="E48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="61"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
@@ -8894,11 +8894,11 @@
       <c r="B49" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="C49" s="59" t="s">
+      <c r="C49" s="60" t="s">
         <v>493</v>
       </c>
-      <c r="D49" s="59"/>
-      <c r="E49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="61"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
@@ -8911,11 +8911,11 @@
       <c r="B50" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="C50" s="59" t="s">
+      <c r="C50" s="60" t="s">
         <v>496</v>
       </c>
-      <c r="D50" s="59"/>
-      <c r="E50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="61"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
@@ -8928,11 +8928,11 @@
       <c r="B51" s="42" t="s">
         <v>498</v>
       </c>
-      <c r="C51" s="59" t="s">
+      <c r="C51" s="60" t="s">
         <v>499</v>
       </c>
-      <c r="D51" s="59"/>
-      <c r="E51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="61"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
@@ -8945,11 +8945,11 @@
       <c r="B52" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="59" t="s">
+      <c r="C52" s="60" t="s">
         <v>502</v>
       </c>
-      <c r="D52" s="59"/>
-      <c r="E52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="61"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
@@ -8962,11 +8962,11 @@
       <c r="B53" s="42" t="s">
         <v>504</v>
       </c>
-      <c r="C53" s="59" t="s">
+      <c r="C53" s="60" t="s">
         <v>505</v>
       </c>
-      <c r="D53" s="59"/>
-      <c r="E53" s="60"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="61"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
@@ -8979,11 +8979,11 @@
       <c r="B54" s="42" t="s">
         <v>507</v>
       </c>
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="60" t="s">
         <v>508</v>
       </c>
-      <c r="D54" s="59"/>
-      <c r="E54" s="60"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="61"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
@@ -8996,11 +8996,11 @@
       <c r="B55" s="42" t="s">
         <v>510</v>
       </c>
-      <c r="C55" s="59" t="s">
+      <c r="C55" s="60" t="s">
         <v>511</v>
       </c>
-      <c r="D55" s="59"/>
-      <c r="E55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="61"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
@@ -9013,11 +9013,11 @@
       <c r="B56" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C56" s="59" t="s">
+      <c r="C56" s="60" t="s">
         <v>514</v>
       </c>
-      <c r="D56" s="59"/>
-      <c r="E56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="61"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
@@ -9030,11 +9030,11 @@
       <c r="B57" s="42" t="s">
         <v>516</v>
       </c>
-      <c r="C57" s="59" t="s">
+      <c r="C57" s="60" t="s">
         <v>517</v>
       </c>
-      <c r="D57" s="59"/>
-      <c r="E57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="61"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
@@ -9047,11 +9047,11 @@
       <c r="B58" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="C58" s="59" t="s">
+      <c r="C58" s="60" t="s">
         <v>520</v>
       </c>
-      <c r="D58" s="59"/>
-      <c r="E58" s="60"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="61"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -9064,11 +9064,11 @@
       <c r="B59" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="C59" s="59" t="s">
+      <c r="C59" s="60" t="s">
         <v>523</v>
       </c>
-      <c r="D59" s="59"/>
-      <c r="E59" s="60"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="61"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
@@ -9081,11 +9081,11 @@
       <c r="B60" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="C60" s="59" t="s">
+      <c r="C60" s="60" t="s">
         <v>526</v>
       </c>
-      <c r="D60" s="59"/>
-      <c r="E60" s="60"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="61"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
@@ -9098,11 +9098,11 @@
       <c r="B61" s="42" t="s">
         <v>528</v>
       </c>
-      <c r="C61" s="59" t="s">
+      <c r="C61" s="60" t="s">
         <v>529</v>
       </c>
-      <c r="D61" s="59"/>
-      <c r="E61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="61"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
@@ -9115,11 +9115,11 @@
       <c r="B62" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C62" s="59" t="s">
+      <c r="C62" s="60" t="s">
         <v>532</v>
       </c>
-      <c r="D62" s="59"/>
-      <c r="E62" s="60"/>
+      <c r="D62" s="60"/>
+      <c r="E62" s="61"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
@@ -9132,11 +9132,11 @@
       <c r="B63" s="42" t="s">
         <v>534</v>
       </c>
-      <c r="C63" s="59" t="s">
+      <c r="C63" s="60" t="s">
         <v>535</v>
       </c>
-      <c r="D63" s="59"/>
-      <c r="E63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="61"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
@@ -9149,11 +9149,11 @@
       <c r="B64" s="42" t="s">
         <v>536</v>
       </c>
-      <c r="C64" s="59" t="s">
+      <c r="C64" s="60" t="s">
         <v>537</v>
       </c>
-      <c r="D64" s="59"/>
-      <c r="E64" s="60"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="61"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -9166,11 +9166,11 @@
       <c r="B65" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C65" s="59" t="s">
+      <c r="C65" s="60" t="s">
         <v>540</v>
       </c>
-      <c r="D65" s="59"/>
-      <c r="E65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="61"/>
       <c r="F65" s="58"/>
       <c r="G65" s="56"/>
       <c r="H65" s="56"/>
@@ -9183,11 +9183,11 @@
       <c r="B66" s="42" t="s">
         <v>542</v>
       </c>
-      <c r="C66" s="59" t="s">
+      <c r="C66" s="60" t="s">
         <v>543</v>
       </c>
-      <c r="D66" s="59"/>
-      <c r="E66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
       <c r="F66" s="58"/>
       <c r="G66" s="56"/>
       <c r="H66" s="56"/>
@@ -9200,11 +9200,11 @@
       <c r="B67" s="42" t="s">
         <v>545</v>
       </c>
-      <c r="C67" s="59" t="s">
+      <c r="C67" s="60" t="s">
         <v>546</v>
       </c>
-      <c r="D67" s="59"/>
-      <c r="E67" s="60"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="61"/>
       <c r="F67" s="58"/>
       <c r="G67" s="56"/>
       <c r="H67" s="56"/>
@@ -9217,11 +9217,11 @@
       <c r="B68" s="42" t="s">
         <v>548</v>
       </c>
-      <c r="C68" s="59" t="s">
+      <c r="C68" s="60" t="s">
         <v>549</v>
       </c>
-      <c r="D68" s="59"/>
-      <c r="E68" s="60"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="61"/>
       <c r="F68" s="58"/>
       <c r="G68" s="56"/>
       <c r="H68" s="56"/>
@@ -9234,11 +9234,11 @@
       <c r="B69" s="42" t="s">
         <v>551</v>
       </c>
-      <c r="C69" s="59" t="s">
+      <c r="C69" s="60" t="s">
         <v>552</v>
       </c>
-      <c r="D69" s="59"/>
-      <c r="E69" s="60"/>
+      <c r="D69" s="60"/>
+      <c r="E69" s="61"/>
       <c r="F69" s="58"/>
       <c r="G69" s="56"/>
       <c r="H69" s="56"/>
@@ -9251,11 +9251,11 @@
       <c r="B70" s="42" t="s">
         <v>554</v>
       </c>
-      <c r="C70" s="59" t="s">
+      <c r="C70" s="60" t="s">
         <v>555</v>
       </c>
-      <c r="D70" s="59"/>
-      <c r="E70" s="60"/>
+      <c r="D70" s="60"/>
+      <c r="E70" s="61"/>
       <c r="F70" s="58"/>
       <c r="G70" s="56"/>
       <c r="H70" s="56"/>
@@ -9268,11 +9268,11 @@
       <c r="B71" s="42" t="s">
         <v>557</v>
       </c>
-      <c r="C71" s="59" t="s">
+      <c r="C71" s="60" t="s">
         <v>558</v>
       </c>
-      <c r="D71" s="59"/>
-      <c r="E71" s="60"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="61"/>
       <c r="F71" s="58"/>
       <c r="G71" s="56"/>
       <c r="H71" s="56"/>
@@ -9285,11 +9285,11 @@
       <c r="B72" s="42" t="s">
         <v>560</v>
       </c>
-      <c r="C72" s="59" t="s">
+      <c r="C72" s="60" t="s">
         <v>561</v>
       </c>
-      <c r="D72" s="59"/>
-      <c r="E72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="61"/>
       <c r="F72" s="58"/>
       <c r="G72" s="56"/>
       <c r="H72" s="56"/>
@@ -9302,11 +9302,11 @@
       <c r="B73" s="42" t="s">
         <v>563</v>
       </c>
-      <c r="C73" s="59" t="s">
+      <c r="C73" s="60" t="s">
         <v>564</v>
       </c>
-      <c r="D73" s="59"/>
-      <c r="E73" s="60"/>
+      <c r="D73" s="60"/>
+      <c r="E73" s="61"/>
       <c r="F73" s="58"/>
       <c r="G73" s="56"/>
       <c r="H73" s="56"/>
@@ -9319,11 +9319,11 @@
       <c r="B74" s="42" t="s">
         <v>566</v>
       </c>
-      <c r="C74" s="59" t="s">
+      <c r="C74" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="D74" s="59"/>
-      <c r="E74" s="60"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="61"/>
       <c r="F74" s="58"/>
       <c r="G74" s="56"/>
       <c r="H74" s="56"/>
@@ -9336,11 +9336,11 @@
       <c r="B75" s="42" t="s">
         <v>569</v>
       </c>
-      <c r="C75" s="59" t="s">
+      <c r="C75" s="60" t="s">
         <v>570</v>
       </c>
-      <c r="D75" s="59"/>
-      <c r="E75" s="60"/>
+      <c r="D75" s="60"/>
+      <c r="E75" s="61"/>
       <c r="F75" s="58"/>
       <c r="G75" s="56"/>
       <c r="H75" s="56"/>
@@ -9353,11 +9353,11 @@
       <c r="B76" s="42" t="s">
         <v>572</v>
       </c>
-      <c r="C76" s="59" t="s">
+      <c r="C76" s="60" t="s">
         <v>573</v>
       </c>
-      <c r="D76" s="59"/>
-      <c r="E76" s="60"/>
+      <c r="D76" s="60"/>
+      <c r="E76" s="61"/>
       <c r="F76" s="58"/>
       <c r="G76" s="56"/>
       <c r="H76" s="56"/>
@@ -9370,11 +9370,11 @@
       <c r="B77" s="42" t="s">
         <v>575</v>
       </c>
-      <c r="C77" s="59" t="s">
+      <c r="C77" s="60" t="s">
         <v>576</v>
       </c>
-      <c r="D77" s="59"/>
-      <c r="E77" s="60"/>
+      <c r="D77" s="60"/>
+      <c r="E77" s="61"/>
       <c r="F77" s="58"/>
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
@@ -9387,11 +9387,11 @@
       <c r="B78" s="42" t="s">
         <v>578</v>
       </c>
-      <c r="C78" s="59" t="s">
+      <c r="C78" s="60" t="s">
         <v>579</v>
       </c>
-      <c r="D78" s="59"/>
-      <c r="E78" s="60"/>
+      <c r="D78" s="60"/>
+      <c r="E78" s="61"/>
       <c r="F78" s="58"/>
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
@@ -9404,11 +9404,11 @@
       <c r="B79" s="42" t="s">
         <v>581</v>
       </c>
-      <c r="C79" s="59" t="s">
+      <c r="C79" s="60" t="s">
         <v>582</v>
       </c>
-      <c r="D79" s="59"/>
-      <c r="E79" s="60"/>
+      <c r="D79" s="60"/>
+      <c r="E79" s="61"/>
       <c r="F79" s="58"/>
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
@@ -9421,11 +9421,11 @@
       <c r="B80" s="42" t="s">
         <v>584</v>
       </c>
-      <c r="C80" s="59" t="s">
+      <c r="C80" s="60" t="s">
         <v>585</v>
       </c>
-      <c r="D80" s="59"/>
-      <c r="E80" s="60"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="61"/>
       <c r="F80" s="58"/>
       <c r="G80" s="56"/>
       <c r="H80" s="56"/>
@@ -9438,11 +9438,11 @@
       <c r="B81" s="42" t="s">
         <v>587</v>
       </c>
-      <c r="C81" s="59" t="s">
+      <c r="C81" s="60" t="s">
         <v>588</v>
       </c>
-      <c r="D81" s="59"/>
-      <c r="E81" s="60"/>
+      <c r="D81" s="60"/>
+      <c r="E81" s="61"/>
       <c r="F81" s="58"/>
       <c r="G81" s="56"/>
       <c r="H81" s="56"/>
@@ -9450,6 +9450,99 @@
     </row>
   </sheetData>
   <mergeCells count="117">
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F44:I44"/>
@@ -9474,99 +9567,6 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10430,41 +10430,14 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -10481,14 +10454,41 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -10759,8 +10759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2BDBDB-F0FD-45C0-BF16-DF2DA17B063A}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10925,7 +10925,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>645</v>
@@ -11699,11 +11699,38 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -11720,38 +11747,11 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E20" xr:uid="{7FAB08B6-9907-44B4-A82A-4A3E200D36A8}">
@@ -12848,23 +12848,25 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
     <mergeCell ref="F43:I43"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="F31:I31"/>
@@ -12877,25 +12879,23 @@
     <mergeCell ref="F38:I38"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -18494,15 +18494,96 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="111">
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="H140:K140"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H59:K59"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="H61:K61"/>
+    <mergeCell ref="H62:K62"/>
+    <mergeCell ref="H63:K63"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H57:K57"/>
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H66:K66"/>
+    <mergeCell ref="H67:K67"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="H106:K106"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="H125:K125"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="H121:K121"/>
     <mergeCell ref="H134:K134"/>
     <mergeCell ref="H135:K135"/>
     <mergeCell ref="H136:K136"/>
@@ -18515,96 +18596,15 @@
     <mergeCell ref="H131:K131"/>
     <mergeCell ref="H132:K132"/>
     <mergeCell ref="H133:K133"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="H106:K106"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="H67:K67"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="H59:K59"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="H61:K61"/>
-    <mergeCell ref="H62:K62"/>
-    <mergeCell ref="H63:K63"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H57:K57"/>
-    <mergeCell ref="H58:K58"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H140:K140"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20680,31 +20680,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="F110:I110"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="F112:I112"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="F109:I109"/>
     <mergeCell ref="F100:I100"/>
     <mergeCell ref="F101:I101"/>
     <mergeCell ref="F102:I102"/>
@@ -20715,6 +20690,31 @@
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
+    <mergeCell ref="F110:I110"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="F112:I112"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F108:I108"/>
+    <mergeCell ref="F109:I109"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -22893,48 +22893,109 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
@@ -22959,109 +23020,48 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23607,7 +23607,7 @@
         <v>1115</v>
       </c>
       <c r="D14" s="57"/>
-      <c r="E14" s="61"/>
+      <c r="E14" s="59"/>
       <c r="F14" s="62" t="s">
         <v>464</v>
       </c>
@@ -23616,201 +23616,201 @@
       <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="64" t="s">
         <v>1116</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1117</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="60" t="s">
         <v>1118</v>
       </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="61"/>
       <c r="F15" s="58"/>
       <c r="G15" s="56"/>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="42" t="s">
         <v>1119</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="60" t="s">
         <v>1120</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
       <c r="F16" s="58"/>
       <c r="G16" s="56"/>
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="42" t="s">
         <v>1121</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="60" t="s">
         <v>1122</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="61"/>
       <c r="F17" s="58"/>
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="42" t="s">
         <v>1123</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="61" t="s">
         <v>1124</v>
       </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
       <c r="F18" s="58"/>
       <c r="G18" s="56"/>
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="42" t="s">
         <v>1125</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="61" t="s">
         <v>1126</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
       <c r="F19" s="58"/>
       <c r="G19" s="56"/>
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="65" t="s">
         <v>1127</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="61" t="s">
         <v>1129</v>
       </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
       <c r="F20" s="58"/>
       <c r="G20" s="56"/>
       <c r="H20" s="56"/>
       <c r="I20" s="56"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="66"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="42" t="s">
         <v>1130</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="61" t="s">
         <v>1131</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
       <c r="F21" s="58"/>
       <c r="G21" s="56"/>
       <c r="H21" s="56"/>
       <c r="I21" s="56"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="66"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="61" t="s">
         <v>1133</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="58"/>
       <c r="G22" s="56"/>
       <c r="H22" s="56"/>
       <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="66"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="61" t="s">
         <v>1135</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="58"/>
       <c r="G23" s="56"/>
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="65" t="s">
         <v>1136</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="61" t="s">
         <v>1137</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
       <c r="F24" s="58"/>
       <c r="G24" s="56"/>
       <c r="H24" s="56"/>
       <c r="I24" s="56"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="42" t="s">
         <v>1138</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="61" t="s">
         <v>1139</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
       <c r="F25" s="58"/>
       <c r="G25" s="56"/>
       <c r="H25" s="56"/>
       <c r="I25" s="56"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="66"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="61" t="s">
         <v>1140</v>
       </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
       <c r="F26" s="58"/>
       <c r="G26" s="56"/>
       <c r="H26" s="56"/>
       <c r="I26" s="56"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="66"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="66" t="s">
         <v>1141</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
       <c r="F27" s="58"/>
       <c r="G27" s="56"/>
       <c r="H27" s="56"/>
@@ -23823,137 +23823,137 @@
       <c r="B28" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="66" t="s">
         <v>1144</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
       <c r="F28" s="58"/>
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
       <c r="I28" s="56"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="65" t="s">
         <v>1145</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1146</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="66" t="s">
         <v>1147</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
       <c r="F29" s="58"/>
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="56"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="66"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="45" t="s">
         <v>1148</v>
       </c>
-      <c r="C30" s="64" t="s">
+      <c r="C30" s="66" t="s">
         <v>1149</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
       <c r="F30" s="58"/>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
       <c r="I30" s="56"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="65" t="s">
         <v>1150</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1151</v>
       </c>
-      <c r="C31" s="64" t="s">
+      <c r="C31" s="66" t="s">
         <v>1152</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
       <c r="F31" s="58"/>
       <c r="G31" s="56"/>
       <c r="H31" s="56"/>
       <c r="I31" s="56"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="66"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="45" t="s">
         <v>1153</v>
       </c>
-      <c r="C32" s="64" t="s">
+      <c r="C32" s="66" t="s">
         <v>1154</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
       <c r="F32" s="58"/>
       <c r="G32" s="56"/>
       <c r="H32" s="56"/>
       <c r="I32" s="56"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="65" t="s">
         <v>1155</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1128</v>
       </c>
-      <c r="C33" s="64" t="s">
+      <c r="C33" s="66" t="s">
         <v>1156</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
       <c r="F33" s="58"/>
       <c r="G33" s="56"/>
       <c r="H33" s="56"/>
       <c r="I33" s="56"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="66"/>
+      <c r="A34" s="65"/>
       <c r="B34" s="45" t="s">
         <v>1157</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="66" t="s">
         <v>1158</v>
       </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
       <c r="F34" s="58"/>
       <c r="G34" s="56"/>
       <c r="H34" s="56"/>
       <c r="I34" s="56"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="66"/>
+      <c r="A35" s="65"/>
       <c r="B35" s="45" t="s">
         <v>1159</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="66" t="s">
         <v>1160</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
       <c r="F35" s="58"/>
       <c r="G35" s="56"/>
       <c r="H35" s="56"/>
       <c r="I35" s="56"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
+      <c r="A36" s="65"/>
       <c r="B36" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="66" t="s">
         <v>1161</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
       <c r="F36" s="58"/>
       <c r="G36" s="56"/>
       <c r="H36" s="56"/>
@@ -23966,97 +23966,97 @@
       <c r="B37" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="64" t="s">
+      <c r="C37" s="66" t="s">
         <v>1163</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
       <c r="F37" s="58"/>
       <c r="G37" s="56"/>
       <c r="H37" s="56"/>
       <c r="I37" s="56"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="65" t="s">
         <v>1164</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1165</v>
       </c>
-      <c r="C38" s="64" t="s">
+      <c r="C38" s="66" t="s">
         <v>1166</v>
       </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
       <c r="F38" s="58"/>
       <c r="G38" s="56"/>
       <c r="H38" s="56"/>
       <c r="I38" s="56"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="66"/>
+      <c r="A39" s="65"/>
       <c r="B39" s="45" t="s">
         <v>1167</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="C39" s="66" t="s">
         <v>1168</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
       <c r="F39" s="58"/>
       <c r="G39" s="56"/>
       <c r="H39" s="56"/>
       <c r="I39" s="56"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="66"/>
+      <c r="A40" s="65"/>
       <c r="B40" s="45" t="s">
         <v>1169</v>
       </c>
-      <c r="C40" s="64" t="s">
+      <c r="C40" s="66" t="s">
         <v>1170</v>
       </c>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
       <c r="I40" s="56"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="65" t="s">
         <v>1171</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1172</v>
       </c>
-      <c r="C41" s="64" t="s">
+      <c r="C41" s="66" t="s">
         <v>1173</v>
       </c>
-      <c r="D41" s="64"/>
-      <c r="E41" s="64"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="66"/>
+      <c r="A42" s="65"/>
       <c r="B42" s="45" t="s">
         <v>1174</v>
       </c>
-      <c r="C42" s="64" t="s">
+      <c r="C42" s="66" t="s">
         <v>1175</v>
       </c>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
       <c r="I42" s="56"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="66"/>
+      <c r="A43" s="65"/>
       <c r="B43" s="45" t="s">
         <v>1176</v>
       </c>
@@ -24071,47 +24071,47 @@
       <c r="I43" s="56"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="66"/>
+      <c r="A44" s="65"/>
       <c r="B44" s="45" t="s">
         <v>1178</v>
       </c>
-      <c r="C44" s="65" t="s">
+      <c r="C44" s="64" t="s">
         <v>1179</v>
       </c>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
       <c r="I44" s="56"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="65" t="s">
         <v>1180</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1181</v>
       </c>
-      <c r="C45" s="65" t="s">
+      <c r="C45" s="64" t="s">
         <v>1182</v>
       </c>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="66"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="45" t="s">
         <v>1183</v>
       </c>
-      <c r="C46" s="65" t="s">
+      <c r="C46" s="64" t="s">
         <v>1184</v>
       </c>
-      <c r="D46" s="65"/>
-      <c r="E46" s="65"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -24124,11 +24124,11 @@
       <c r="B47" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C47" s="65" t="s">
+      <c r="C47" s="64" t="s">
         <v>1186</v>
       </c>
-      <c r="D47" s="65"/>
-      <c r="E47" s="65"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -24141,165 +24141,165 @@
       <c r="B48" s="45" t="s">
         <v>1188</v>
       </c>
-      <c r="C48" s="65" t="s">
+      <c r="C48" s="64" t="s">
         <v>1189</v>
       </c>
-      <c r="D48" s="65"/>
-      <c r="E48" s="65"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
       <c r="I48" s="56"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="65" t="s">
         <v>1190</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1191</v>
       </c>
-      <c r="C49" s="65" t="s">
+      <c r="C49" s="64" t="s">
         <v>1192</v>
       </c>
-      <c r="D49" s="65"/>
-      <c r="E49" s="65"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
       <c r="I49" s="56"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="66"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="45" t="s">
         <v>1193</v>
       </c>
-      <c r="C50" s="65" t="s">
+      <c r="C50" s="64" t="s">
         <v>1194</v>
       </c>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
       <c r="I50" s="56"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="66"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="45" t="s">
         <v>1138</v>
       </c>
-      <c r="C51" s="65" t="s">
+      <c r="C51" s="64" t="s">
         <v>1195</v>
       </c>
-      <c r="D51" s="65"/>
-      <c r="E51" s="65"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
       <c r="I51" s="56"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="66"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="45" t="s">
         <v>1196</v>
       </c>
-      <c r="C52" s="65" t="s">
+      <c r="C52" s="64" t="s">
         <v>1197</v>
       </c>
-      <c r="D52" s="65"/>
-      <c r="E52" s="65"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="64"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
       <c r="I52" s="56"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="66"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="45" t="s">
         <v>1134</v>
       </c>
-      <c r="C53" s="65" t="s">
+      <c r="C53" s="64" t="s">
         <v>1198</v>
       </c>
-      <c r="D53" s="65"/>
-      <c r="E53" s="65"/>
+      <c r="D53" s="64"/>
+      <c r="E53" s="64"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
       <c r="I53" s="56"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="65" t="s">
         <v>1199</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1200</v>
       </c>
-      <c r="C54" s="65" t="s">
+      <c r="C54" s="64" t="s">
         <v>1201</v>
       </c>
-      <c r="D54" s="65"/>
-      <c r="E54" s="65"/>
+      <c r="D54" s="64"/>
+      <c r="E54" s="64"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
       <c r="I54" s="56"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="66"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="5" t="s">
         <v>1202</v>
       </c>
-      <c r="C55" s="65" t="s">
+      <c r="C55" s="64" t="s">
         <v>1203</v>
       </c>
-      <c r="D55" s="65"/>
-      <c r="E55" s="65"/>
+      <c r="D55" s="64"/>
+      <c r="E55" s="64"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
       <c r="I55" s="56"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="66"/>
+      <c r="A56" s="65"/>
       <c r="B56" s="5" t="s">
         <v>1204</v>
       </c>
-      <c r="C56" s="65" t="s">
+      <c r="C56" s="64" t="s">
         <v>1205</v>
       </c>
-      <c r="D56" s="65"/>
-      <c r="E56" s="65"/>
+      <c r="D56" s="64"/>
+      <c r="E56" s="64"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
       <c r="I56" s="56"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="66"/>
+      <c r="A57" s="65"/>
       <c r="B57" s="5" t="s">
         <v>1206</v>
       </c>
-      <c r="C57" s="65" t="s">
+      <c r="C57" s="64" t="s">
         <v>1207</v>
       </c>
-      <c r="D57" s="65"/>
-      <c r="E57" s="65"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="64"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
       <c r="I57" s="56"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="66"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="5" t="s">
         <v>1208</v>
       </c>
-      <c r="C58" s="65" t="s">
+      <c r="C58" s="64" t="s">
         <v>1209</v>
       </c>
-      <c r="D58" s="65"/>
-      <c r="E58" s="65"/>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -24312,88 +24312,88 @@
       <c r="B59" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C59" s="65" t="s">
+      <c r="C59" s="64" t="s">
         <v>1211</v>
       </c>
-      <c r="D59" s="65"/>
-      <c r="E59" s="65"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
       <c r="I59" s="56"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="65" t="s">
         <v>1212</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1213</v>
       </c>
-      <c r="C60" s="65" t="s">
+      <c r="C60" s="64" t="s">
         <v>1214</v>
       </c>
-      <c r="D60" s="65"/>
-      <c r="E60" s="65"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
       <c r="I60" s="56"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="66"/>
+      <c r="A61" s="65"/>
       <c r="B61" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="64" t="s">
         <v>1216</v>
       </c>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
       <c r="I61" s="56"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="66"/>
+      <c r="A62" s="65"/>
       <c r="B62" s="5" t="s">
         <v>1217</v>
       </c>
-      <c r="C62" s="65" t="s">
+      <c r="C62" s="64" t="s">
         <v>1218</v>
       </c>
-      <c r="D62" s="65"/>
-      <c r="E62" s="65"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
       <c r="I62" s="56"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="66"/>
+      <c r="A63" s="65"/>
       <c r="B63" s="5" t="s">
         <v>1219</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C63" s="64" t="s">
         <v>1220</v>
       </c>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
       <c r="I63" s="56"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="66"/>
+      <c r="A64" s="65"/>
       <c r="B64" s="5" t="s">
         <v>1221</v>
       </c>
-      <c r="C64" s="65" t="s">
+      <c r="C64" s="64" t="s">
         <v>1222</v>
       </c>
-      <c r="D64" s="65"/>
-      <c r="E64" s="65"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -24401,36 +24401,66 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="C64:E64"/>
     <mergeCell ref="A54:A58"/>
@@ -24455,66 +24485,36 @@
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -24548,7 +24548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D896FB-80F4-4D48-93D9-6DBE34ADD468}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -25850,6 +25850,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -25862,13 +25869,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26239,6 +26239,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F9:I9"/>
@@ -26246,18 +26258,6 @@
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:I11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -26724,19 +26724,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -26750,6 +26737,19 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -27634,19 +27634,33 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="C24:D24"/>
@@ -27660,33 +27674,19 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28171,13 +28171,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -28188,6 +28181,13 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -28595,6 +28595,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -28607,11 +28612,6 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28643,6 +28643,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -28871,15 +28880,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -28892,6 +28892,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28906,14 +28914,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
:sparkles: Remove max cardinality restriction from the code of vital sign and lab result
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB75181C-62B1-42B2-8E73-4975B72E46A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1712959C-6C56-43A7-889C-EC087B7CDBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -6615,22 +6615,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8010,6 +8010,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -8020,13 +8027,6 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8726,7 +8726,7 @@
         <v>463</v>
       </c>
       <c r="D39" s="57"/>
-      <c r="E39" s="59"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="62" t="s">
         <v>464</v>
       </c>
@@ -8741,11 +8741,11 @@
       <c r="B40" s="42" t="s">
         <v>466</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="59" t="s">
         <v>467</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
@@ -8758,11 +8758,11 @@
       <c r="B41" s="42" t="s">
         <v>469</v>
       </c>
-      <c r="C41" s="60" t="s">
+      <c r="C41" s="59" t="s">
         <v>470</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="61"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
@@ -8775,11 +8775,11 @@
       <c r="B42" s="42" t="s">
         <v>472</v>
       </c>
-      <c r="C42" s="60" t="s">
+      <c r="C42" s="59" t="s">
         <v>473</v>
       </c>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
@@ -8792,11 +8792,11 @@
       <c r="B43" s="42" t="s">
         <v>475</v>
       </c>
-      <c r="C43" s="60" t="s">
+      <c r="C43" s="59" t="s">
         <v>1380</v>
       </c>
-      <c r="D43" s="60"/>
-      <c r="E43" s="61"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="58"/>
       <c r="G43" s="56"/>
       <c r="H43" s="56"/>
@@ -8809,11 +8809,11 @@
       <c r="B44" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="59" t="s">
         <v>478</v>
       </c>
-      <c r="D44" s="60"/>
-      <c r="E44" s="61"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="60"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
@@ -8826,11 +8826,11 @@
       <c r="B45" s="42" t="s">
         <v>480</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="59" t="s">
         <v>481</v>
       </c>
-      <c r="D45" s="60"/>
-      <c r="E45" s="61"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
@@ -8843,11 +8843,11 @@
       <c r="B46" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="C46" s="60" t="s">
+      <c r="C46" s="59" t="s">
         <v>484</v>
       </c>
-      <c r="D46" s="60"/>
-      <c r="E46" s="61"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -8860,11 +8860,11 @@
       <c r="B47" s="42" t="s">
         <v>486</v>
       </c>
-      <c r="C47" s="60" t="s">
+      <c r="C47" s="59" t="s">
         <v>487</v>
       </c>
-      <c r="D47" s="60"/>
-      <c r="E47" s="61"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -8877,11 +8877,11 @@
       <c r="B48" s="42" t="s">
         <v>489</v>
       </c>
-      <c r="C48" s="60" t="s">
+      <c r="C48" s="59" t="s">
         <v>490</v>
       </c>
-      <c r="D48" s="60"/>
-      <c r="E48" s="61"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="60"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
@@ -8894,11 +8894,11 @@
       <c r="B49" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="C49" s="60" t="s">
+      <c r="C49" s="59" t="s">
         <v>493</v>
       </c>
-      <c r="D49" s="60"/>
-      <c r="E49" s="61"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="60"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
@@ -8911,11 +8911,11 @@
       <c r="B50" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="C50" s="60" t="s">
+      <c r="C50" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="D50" s="60"/>
-      <c r="E50" s="61"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="60"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
@@ -8928,11 +8928,11 @@
       <c r="B51" s="42" t="s">
         <v>498</v>
       </c>
-      <c r="C51" s="60" t="s">
+      <c r="C51" s="59" t="s">
         <v>499</v>
       </c>
-      <c r="D51" s="60"/>
-      <c r="E51" s="61"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="60"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
@@ -8945,11 +8945,11 @@
       <c r="B52" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="C52" s="60" t="s">
+      <c r="C52" s="59" t="s">
         <v>502</v>
       </c>
-      <c r="D52" s="60"/>
-      <c r="E52" s="61"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="60"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
@@ -8962,11 +8962,11 @@
       <c r="B53" s="42" t="s">
         <v>504</v>
       </c>
-      <c r="C53" s="60" t="s">
+      <c r="C53" s="59" t="s">
         <v>505</v>
       </c>
-      <c r="D53" s="60"/>
-      <c r="E53" s="61"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="60"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
@@ -8979,11 +8979,11 @@
       <c r="B54" s="42" t="s">
         <v>507</v>
       </c>
-      <c r="C54" s="60" t="s">
+      <c r="C54" s="59" t="s">
         <v>508</v>
       </c>
-      <c r="D54" s="60"/>
-      <c r="E54" s="61"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="60"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
@@ -8996,11 +8996,11 @@
       <c r="B55" s="42" t="s">
         <v>510</v>
       </c>
-      <c r="C55" s="60" t="s">
+      <c r="C55" s="59" t="s">
         <v>511</v>
       </c>
-      <c r="D55" s="60"/>
-      <c r="E55" s="61"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
@@ -9013,11 +9013,11 @@
       <c r="B56" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C56" s="60" t="s">
+      <c r="C56" s="59" t="s">
         <v>514</v>
       </c>
-      <c r="D56" s="60"/>
-      <c r="E56" s="61"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="60"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
@@ -9030,11 +9030,11 @@
       <c r="B57" s="42" t="s">
         <v>516</v>
       </c>
-      <c r="C57" s="60" t="s">
+      <c r="C57" s="59" t="s">
         <v>517</v>
       </c>
-      <c r="D57" s="60"/>
-      <c r="E57" s="61"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="60"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
@@ -9047,11 +9047,11 @@
       <c r="B58" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="C58" s="60" t="s">
+      <c r="C58" s="59" t="s">
         <v>520</v>
       </c>
-      <c r="D58" s="60"/>
-      <c r="E58" s="61"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="60"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -9064,11 +9064,11 @@
       <c r="B59" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="C59" s="60" t="s">
+      <c r="C59" s="59" t="s">
         <v>523</v>
       </c>
-      <c r="D59" s="60"/>
-      <c r="E59" s="61"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
@@ -9081,11 +9081,11 @@
       <c r="B60" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="C60" s="60" t="s">
+      <c r="C60" s="59" t="s">
         <v>526</v>
       </c>
-      <c r="D60" s="60"/>
-      <c r="E60" s="61"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
@@ -9098,11 +9098,11 @@
       <c r="B61" s="42" t="s">
         <v>528</v>
       </c>
-      <c r="C61" s="60" t="s">
+      <c r="C61" s="59" t="s">
         <v>529</v>
       </c>
-      <c r="D61" s="60"/>
-      <c r="E61" s="61"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="60"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
@@ -9115,11 +9115,11 @@
       <c r="B62" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C62" s="60" t="s">
+      <c r="C62" s="59" t="s">
         <v>532</v>
       </c>
-      <c r="D62" s="60"/>
-      <c r="E62" s="61"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="60"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
@@ -9132,11 +9132,11 @@
       <c r="B63" s="42" t="s">
         <v>534</v>
       </c>
-      <c r="C63" s="60" t="s">
+      <c r="C63" s="59" t="s">
         <v>535</v>
       </c>
-      <c r="D63" s="60"/>
-      <c r="E63" s="61"/>
+      <c r="D63" s="59"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
@@ -9149,11 +9149,11 @@
       <c r="B64" s="42" t="s">
         <v>536</v>
       </c>
-      <c r="C64" s="60" t="s">
+      <c r="C64" s="59" t="s">
         <v>537</v>
       </c>
-      <c r="D64" s="60"/>
-      <c r="E64" s="61"/>
+      <c r="D64" s="59"/>
+      <c r="E64" s="60"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -9166,11 +9166,11 @@
       <c r="B65" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C65" s="60" t="s">
+      <c r="C65" s="59" t="s">
         <v>540</v>
       </c>
-      <c r="D65" s="60"/>
-      <c r="E65" s="61"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="60"/>
       <c r="F65" s="58"/>
       <c r="G65" s="56"/>
       <c r="H65" s="56"/>
@@ -9183,11 +9183,11 @@
       <c r="B66" s="42" t="s">
         <v>542</v>
       </c>
-      <c r="C66" s="60" t="s">
+      <c r="C66" s="59" t="s">
         <v>543</v>
       </c>
-      <c r="D66" s="60"/>
-      <c r="E66" s="61"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="60"/>
       <c r="F66" s="58"/>
       <c r="G66" s="56"/>
       <c r="H66" s="56"/>
@@ -9200,11 +9200,11 @@
       <c r="B67" s="42" t="s">
         <v>545</v>
       </c>
-      <c r="C67" s="60" t="s">
+      <c r="C67" s="59" t="s">
         <v>546</v>
       </c>
-      <c r="D67" s="60"/>
-      <c r="E67" s="61"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="60"/>
       <c r="F67" s="58"/>
       <c r="G67" s="56"/>
       <c r="H67" s="56"/>
@@ -9217,11 +9217,11 @@
       <c r="B68" s="42" t="s">
         <v>548</v>
       </c>
-      <c r="C68" s="60" t="s">
+      <c r="C68" s="59" t="s">
         <v>549</v>
       </c>
-      <c r="D68" s="60"/>
-      <c r="E68" s="61"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="60"/>
       <c r="F68" s="58"/>
       <c r="G68" s="56"/>
       <c r="H68" s="56"/>
@@ -9234,11 +9234,11 @@
       <c r="B69" s="42" t="s">
         <v>551</v>
       </c>
-      <c r="C69" s="60" t="s">
+      <c r="C69" s="59" t="s">
         <v>552</v>
       </c>
-      <c r="D69" s="60"/>
-      <c r="E69" s="61"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="60"/>
       <c r="F69" s="58"/>
       <c r="G69" s="56"/>
       <c r="H69" s="56"/>
@@ -9251,11 +9251,11 @@
       <c r="B70" s="42" t="s">
         <v>554</v>
       </c>
-      <c r="C70" s="60" t="s">
+      <c r="C70" s="59" t="s">
         <v>555</v>
       </c>
-      <c r="D70" s="60"/>
-      <c r="E70" s="61"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="60"/>
       <c r="F70" s="58"/>
       <c r="G70" s="56"/>
       <c r="H70" s="56"/>
@@ -9268,11 +9268,11 @@
       <c r="B71" s="42" t="s">
         <v>557</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="59" t="s">
         <v>558</v>
       </c>
-      <c r="D71" s="60"/>
-      <c r="E71" s="61"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="60"/>
       <c r="F71" s="58"/>
       <c r="G71" s="56"/>
       <c r="H71" s="56"/>
@@ -9285,11 +9285,11 @@
       <c r="B72" s="42" t="s">
         <v>560</v>
       </c>
-      <c r="C72" s="60" t="s">
+      <c r="C72" s="59" t="s">
         <v>561</v>
       </c>
-      <c r="D72" s="60"/>
-      <c r="E72" s="61"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="60"/>
       <c r="F72" s="58"/>
       <c r="G72" s="56"/>
       <c r="H72" s="56"/>
@@ -9302,11 +9302,11 @@
       <c r="B73" s="42" t="s">
         <v>563</v>
       </c>
-      <c r="C73" s="60" t="s">
+      <c r="C73" s="59" t="s">
         <v>564</v>
       </c>
-      <c r="D73" s="60"/>
-      <c r="E73" s="61"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="60"/>
       <c r="F73" s="58"/>
       <c r="G73" s="56"/>
       <c r="H73" s="56"/>
@@ -9319,11 +9319,11 @@
       <c r="B74" s="42" t="s">
         <v>566</v>
       </c>
-      <c r="C74" s="60" t="s">
+      <c r="C74" s="59" t="s">
         <v>567</v>
       </c>
-      <c r="D74" s="60"/>
-      <c r="E74" s="61"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="60"/>
       <c r="F74" s="58"/>
       <c r="G74" s="56"/>
       <c r="H74" s="56"/>
@@ -9336,11 +9336,11 @@
       <c r="B75" s="42" t="s">
         <v>569</v>
       </c>
-      <c r="C75" s="60" t="s">
+      <c r="C75" s="59" t="s">
         <v>570</v>
       </c>
-      <c r="D75" s="60"/>
-      <c r="E75" s="61"/>
+      <c r="D75" s="59"/>
+      <c r="E75" s="60"/>
       <c r="F75" s="58"/>
       <c r="G75" s="56"/>
       <c r="H75" s="56"/>
@@ -9353,11 +9353,11 @@
       <c r="B76" s="42" t="s">
         <v>572</v>
       </c>
-      <c r="C76" s="60" t="s">
+      <c r="C76" s="59" t="s">
         <v>573</v>
       </c>
-      <c r="D76" s="60"/>
-      <c r="E76" s="61"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="60"/>
       <c r="F76" s="58"/>
       <c r="G76" s="56"/>
       <c r="H76" s="56"/>
@@ -9370,11 +9370,11 @@
       <c r="B77" s="42" t="s">
         <v>575</v>
       </c>
-      <c r="C77" s="60" t="s">
+      <c r="C77" s="59" t="s">
         <v>576</v>
       </c>
-      <c r="D77" s="60"/>
-      <c r="E77" s="61"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="60"/>
       <c r="F77" s="58"/>
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
@@ -9387,11 +9387,11 @@
       <c r="B78" s="42" t="s">
         <v>578</v>
       </c>
-      <c r="C78" s="60" t="s">
+      <c r="C78" s="59" t="s">
         <v>579</v>
       </c>
-      <c r="D78" s="60"/>
-      <c r="E78" s="61"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="60"/>
       <c r="F78" s="58"/>
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
@@ -9404,11 +9404,11 @@
       <c r="B79" s="42" t="s">
         <v>581</v>
       </c>
-      <c r="C79" s="60" t="s">
+      <c r="C79" s="59" t="s">
         <v>582</v>
       </c>
-      <c r="D79" s="60"/>
-      <c r="E79" s="61"/>
+      <c r="D79" s="59"/>
+      <c r="E79" s="60"/>
       <c r="F79" s="58"/>
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
@@ -9421,11 +9421,11 @@
       <c r="B80" s="42" t="s">
         <v>584</v>
       </c>
-      <c r="C80" s="60" t="s">
+      <c r="C80" s="59" t="s">
         <v>585</v>
       </c>
-      <c r="D80" s="60"/>
-      <c r="E80" s="61"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="60"/>
       <c r="F80" s="58"/>
       <c r="G80" s="56"/>
       <c r="H80" s="56"/>
@@ -9438,11 +9438,11 @@
       <c r="B81" s="42" t="s">
         <v>587</v>
       </c>
-      <c r="C81" s="60" t="s">
+      <c r="C81" s="59" t="s">
         <v>588</v>
       </c>
-      <c r="D81" s="60"/>
-      <c r="E81" s="61"/>
+      <c r="D81" s="59"/>
+      <c r="E81" s="60"/>
       <c r="F81" s="58"/>
       <c r="G81" s="56"/>
       <c r="H81" s="56"/>
@@ -9450,36 +9450,69 @@
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="F48:I48"/>
     <mergeCell ref="F49:I49"/>
@@ -9504,69 +9537,36 @@
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="F55:I55"/>
     <mergeCell ref="F56:I56"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10430,14 +10430,41 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -10454,41 +10481,14 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -10759,7 +10759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2BDBDB-F0FD-45C0-BF16-DF2DA17B063A}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -10970,7 +10970,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11118,7 +11118,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>648</v>
@@ -11699,38 +11699,11 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -11747,11 +11720,38 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E20" xr:uid="{7FAB08B6-9907-44B4-A82A-4A3E200D36A8}">
@@ -11791,8 +11791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BB695D-4821-4052-8E37-D71854C5F317}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11941,7 +11941,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>677</v>
@@ -12848,25 +12848,23 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
     <mergeCell ref="F43:I43"/>
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="F31:I31"/>
@@ -12879,23 +12877,25 @@
     <mergeCell ref="F38:I38"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -18494,24 +18494,87 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="111">
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H49:K49"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H140:K140"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H134:K134"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="H136:K136"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="H138:K138"/>
+    <mergeCell ref="H139:K139"/>
+    <mergeCell ref="H128:K128"/>
+    <mergeCell ref="H129:K129"/>
+    <mergeCell ref="H130:K130"/>
+    <mergeCell ref="H131:K131"/>
+    <mergeCell ref="H132:K132"/>
+    <mergeCell ref="H133:K133"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="H125:K125"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="H121:K121"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="H106:K106"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H66:K66"/>
+    <mergeCell ref="H67:K67"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="H73:K73"/>
     <mergeCell ref="H59:K59"/>
     <mergeCell ref="H60:K60"/>
     <mergeCell ref="H61:K61"/>
@@ -18524,87 +18587,24 @@
     <mergeCell ref="H55:K55"/>
     <mergeCell ref="H57:K57"/>
     <mergeCell ref="H58:K58"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="H67:K67"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="H106:K106"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="H134:K134"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="H136:K136"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="H138:K138"/>
-    <mergeCell ref="H139:K139"/>
-    <mergeCell ref="H128:K128"/>
-    <mergeCell ref="H129:K129"/>
-    <mergeCell ref="H130:K130"/>
-    <mergeCell ref="H131:K131"/>
-    <mergeCell ref="H132:K132"/>
-    <mergeCell ref="H133:K133"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="H140:K140"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H45:K45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20680,6 +20680,31 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="F110:I110"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="F112:I112"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F108:I108"/>
+    <mergeCell ref="F109:I109"/>
     <mergeCell ref="F100:I100"/>
     <mergeCell ref="F101:I101"/>
     <mergeCell ref="F102:I102"/>
@@ -20690,31 +20715,6 @@
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
-    <mergeCell ref="F110:I110"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="F112:I112"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="F109:I109"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -22893,49 +22893,108 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="C80:D80"/>
@@ -22960,108 +23019,49 @@
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23607,7 +23607,7 @@
         <v>1115</v>
       </c>
       <c r="D14" s="57"/>
-      <c r="E14" s="59"/>
+      <c r="E14" s="61"/>
       <c r="F14" s="62" t="s">
         <v>464</v>
       </c>
@@ -23616,201 +23616,201 @@
       <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="65" t="s">
         <v>1116</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1117</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="59" t="s">
         <v>1118</v>
       </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="58"/>
       <c r="G15" s="56"/>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="42" t="s">
         <v>1119</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="59" t="s">
         <v>1120</v>
       </c>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
       <c r="F16" s="58"/>
       <c r="G16" s="56"/>
       <c r="H16" s="56"/>
       <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="42" t="s">
         <v>1121</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="59" t="s">
         <v>1122</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="58"/>
       <c r="G17" s="56"/>
       <c r="H17" s="56"/>
       <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="42" t="s">
         <v>1123</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="60" t="s">
         <v>1124</v>
       </c>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="58"/>
       <c r="G18" s="56"/>
       <c r="H18" s="56"/>
       <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
+      <c r="A19" s="65"/>
       <c r="B19" s="42" t="s">
         <v>1125</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="60" t="s">
         <v>1126</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="58"/>
       <c r="G19" s="56"/>
       <c r="H19" s="56"/>
       <c r="I19" s="56"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="66" t="s">
         <v>1127</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="60" t="s">
         <v>1129</v>
       </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
       <c r="F20" s="58"/>
       <c r="G20" s="56"/>
       <c r="H20" s="56"/>
       <c r="I20" s="56"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="66"/>
       <c r="B21" s="42" t="s">
         <v>1130</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="60" t="s">
         <v>1131</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
       <c r="F21" s="58"/>
       <c r="G21" s="56"/>
       <c r="H21" s="56"/>
       <c r="I21" s="56"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
+      <c r="A22" s="66"/>
       <c r="B22" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="60" t="s">
         <v>1133</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
       <c r="F22" s="58"/>
       <c r="G22" s="56"/>
       <c r="H22" s="56"/>
       <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="66"/>
       <c r="B23" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="60" t="s">
         <v>1135</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="58"/>
       <c r="G23" s="56"/>
       <c r="H23" s="56"/>
       <c r="I23" s="56"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="66" t="s">
         <v>1136</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1128</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="60" t="s">
         <v>1137</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
       <c r="F24" s="58"/>
       <c r="G24" s="56"/>
       <c r="H24" s="56"/>
       <c r="I24" s="56"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="42" t="s">
         <v>1138</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="60" t="s">
         <v>1139</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
       <c r="F25" s="58"/>
       <c r="G25" s="56"/>
       <c r="H25" s="56"/>
       <c r="I25" s="56"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="65"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="60" t="s">
         <v>1140</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
       <c r="F26" s="58"/>
       <c r="G26" s="56"/>
       <c r="H26" s="56"/>
       <c r="I26" s="56"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="66"/>
       <c r="B27" s="42" t="s">
         <v>1134</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="64" t="s">
         <v>1141</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="58"/>
       <c r="G27" s="56"/>
       <c r="H27" s="56"/>
@@ -23823,137 +23823,137 @@
       <c r="B28" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="64" t="s">
         <v>1144</v>
       </c>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
       <c r="F28" s="58"/>
       <c r="G28" s="56"/>
       <c r="H28" s="56"/>
       <c r="I28" s="56"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="66" t="s">
         <v>1145</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1146</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="64" t="s">
         <v>1147</v>
       </c>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
       <c r="F29" s="58"/>
       <c r="G29" s="56"/>
       <c r="H29" s="56"/>
       <c r="I29" s="56"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
+      <c r="A30" s="66"/>
       <c r="B30" s="45" t="s">
         <v>1148</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="64" t="s">
         <v>1149</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
       <c r="F30" s="58"/>
       <c r="G30" s="56"/>
       <c r="H30" s="56"/>
       <c r="I30" s="56"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="66" t="s">
         <v>1150</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1151</v>
       </c>
-      <c r="C31" s="66" t="s">
+      <c r="C31" s="64" t="s">
         <v>1152</v>
       </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
       <c r="F31" s="58"/>
       <c r="G31" s="56"/>
       <c r="H31" s="56"/>
       <c r="I31" s="56"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
+      <c r="A32" s="66"/>
       <c r="B32" s="45" t="s">
         <v>1153</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="64" t="s">
         <v>1154</v>
       </c>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="58"/>
       <c r="G32" s="56"/>
       <c r="H32" s="56"/>
       <c r="I32" s="56"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="66" t="s">
         <v>1155</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1128</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="64" t="s">
         <v>1156</v>
       </c>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
       <c r="F33" s="58"/>
       <c r="G33" s="56"/>
       <c r="H33" s="56"/>
       <c r="I33" s="56"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
+      <c r="A34" s="66"/>
       <c r="B34" s="45" t="s">
         <v>1157</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="64" t="s">
         <v>1158</v>
       </c>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
       <c r="F34" s="58"/>
       <c r="G34" s="56"/>
       <c r="H34" s="56"/>
       <c r="I34" s="56"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="65"/>
+      <c r="A35" s="66"/>
       <c r="B35" s="45" t="s">
         <v>1159</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="64" t="s">
         <v>1160</v>
       </c>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
       <c r="F35" s="58"/>
       <c r="G35" s="56"/>
       <c r="H35" s="56"/>
       <c r="I35" s="56"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="65"/>
+      <c r="A36" s="66"/>
       <c r="B36" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="66" t="s">
+      <c r="C36" s="64" t="s">
         <v>1161</v>
       </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
       <c r="F36" s="58"/>
       <c r="G36" s="56"/>
       <c r="H36" s="56"/>
@@ -23966,97 +23966,97 @@
       <c r="B37" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C37" s="66" t="s">
+      <c r="C37" s="64" t="s">
         <v>1163</v>
       </c>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
       <c r="F37" s="58"/>
       <c r="G37" s="56"/>
       <c r="H37" s="56"/>
       <c r="I37" s="56"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="65" t="s">
+      <c r="A38" s="66" t="s">
         <v>1164</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1165</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="64" t="s">
         <v>1166</v>
       </c>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="58"/>
       <c r="G38" s="56"/>
       <c r="H38" s="56"/>
       <c r="I38" s="56"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="65"/>
+      <c r="A39" s="66"/>
       <c r="B39" s="45" t="s">
         <v>1167</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="64" t="s">
         <v>1168</v>
       </c>
-      <c r="D39" s="66"/>
-      <c r="E39" s="66"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="58"/>
       <c r="G39" s="56"/>
       <c r="H39" s="56"/>
       <c r="I39" s="56"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="65"/>
+      <c r="A40" s="66"/>
       <c r="B40" s="45" t="s">
         <v>1169</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="64" t="s">
         <v>1170</v>
       </c>
-      <c r="D40" s="66"/>
-      <c r="E40" s="66"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
       <c r="F40" s="58"/>
       <c r="G40" s="56"/>
       <c r="H40" s="56"/>
       <c r="I40" s="56"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="65" t="s">
+      <c r="A41" s="66" t="s">
         <v>1171</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1172</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="64" t="s">
         <v>1173</v>
       </c>
-      <c r="D41" s="66"/>
-      <c r="E41" s="66"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
       <c r="F41" s="58"/>
       <c r="G41" s="56"/>
       <c r="H41" s="56"/>
       <c r="I41" s="56"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="65"/>
+      <c r="A42" s="66"/>
       <c r="B42" s="45" t="s">
         <v>1174</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="64" t="s">
         <v>1175</v>
       </c>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
       <c r="F42" s="58"/>
       <c r="G42" s="56"/>
       <c r="H42" s="56"/>
       <c r="I42" s="56"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="65"/>
+      <c r="A43" s="66"/>
       <c r="B43" s="45" t="s">
         <v>1176</v>
       </c>
@@ -24071,47 +24071,47 @@
       <c r="I43" s="56"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="65"/>
+      <c r="A44" s="66"/>
       <c r="B44" s="45" t="s">
         <v>1178</v>
       </c>
-      <c r="C44" s="64" t="s">
+      <c r="C44" s="65" t="s">
         <v>1179</v>
       </c>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
       <c r="F44" s="58"/>
       <c r="G44" s="56"/>
       <c r="H44" s="56"/>
       <c r="I44" s="56"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="65" t="s">
+      <c r="A45" s="66" t="s">
         <v>1180</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1181</v>
       </c>
-      <c r="C45" s="64" t="s">
+      <c r="C45" s="65" t="s">
         <v>1182</v>
       </c>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
       <c r="F45" s="58"/>
       <c r="G45" s="56"/>
       <c r="H45" s="56"/>
       <c r="I45" s="56"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="65"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="45" t="s">
         <v>1183</v>
       </c>
-      <c r="C46" s="64" t="s">
+      <c r="C46" s="65" t="s">
         <v>1184</v>
       </c>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
       <c r="F46" s="58"/>
       <c r="G46" s="56"/>
       <c r="H46" s="56"/>
@@ -24124,11 +24124,11 @@
       <c r="B47" s="45" t="s">
         <v>1143</v>
       </c>
-      <c r="C47" s="64" t="s">
+      <c r="C47" s="65" t="s">
         <v>1186</v>
       </c>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
       <c r="F47" s="58"/>
       <c r="G47" s="56"/>
       <c r="H47" s="56"/>
@@ -24141,165 +24141,165 @@
       <c r="B48" s="45" t="s">
         <v>1188</v>
       </c>
-      <c r="C48" s="64" t="s">
+      <c r="C48" s="65" t="s">
         <v>1189</v>
       </c>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
       <c r="F48" s="58"/>
       <c r="G48" s="56"/>
       <c r="H48" s="56"/>
       <c r="I48" s="56"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="65" t="s">
+      <c r="A49" s="66" t="s">
         <v>1190</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1191</v>
       </c>
-      <c r="C49" s="64" t="s">
+      <c r="C49" s="65" t="s">
         <v>1192</v>
       </c>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
       <c r="F49" s="58"/>
       <c r="G49" s="56"/>
       <c r="H49" s="56"/>
       <c r="I49" s="56"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="65"/>
+      <c r="A50" s="66"/>
       <c r="B50" s="45" t="s">
         <v>1193</v>
       </c>
-      <c r="C50" s="64" t="s">
+      <c r="C50" s="65" t="s">
         <v>1194</v>
       </c>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
       <c r="F50" s="58"/>
       <c r="G50" s="56"/>
       <c r="H50" s="56"/>
       <c r="I50" s="56"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="65"/>
+      <c r="A51" s="66"/>
       <c r="B51" s="45" t="s">
         <v>1138</v>
       </c>
-      <c r="C51" s="64" t="s">
+      <c r="C51" s="65" t="s">
         <v>1195</v>
       </c>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="65"/>
       <c r="F51" s="58"/>
       <c r="G51" s="56"/>
       <c r="H51" s="56"/>
       <c r="I51" s="56"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="65"/>
+      <c r="A52" s="66"/>
       <c r="B52" s="45" t="s">
         <v>1196</v>
       </c>
-      <c r="C52" s="64" t="s">
+      <c r="C52" s="65" t="s">
         <v>1197</v>
       </c>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
       <c r="F52" s="58"/>
       <c r="G52" s="56"/>
       <c r="H52" s="56"/>
       <c r="I52" s="56"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="65"/>
+      <c r="A53" s="66"/>
       <c r="B53" s="45" t="s">
         <v>1134</v>
       </c>
-      <c r="C53" s="64" t="s">
+      <c r="C53" s="65" t="s">
         <v>1198</v>
       </c>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="65"/>
       <c r="F53" s="58"/>
       <c r="G53" s="56"/>
       <c r="H53" s="56"/>
       <c r="I53" s="56"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="65" t="s">
+      <c r="A54" s="66" t="s">
         <v>1199</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1200</v>
       </c>
-      <c r="C54" s="64" t="s">
+      <c r="C54" s="65" t="s">
         <v>1201</v>
       </c>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="65"/>
       <c r="F54" s="58"/>
       <c r="G54" s="56"/>
       <c r="H54" s="56"/>
       <c r="I54" s="56"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="65"/>
+      <c r="A55" s="66"/>
       <c r="B55" s="5" t="s">
         <v>1202</v>
       </c>
-      <c r="C55" s="64" t="s">
+      <c r="C55" s="65" t="s">
         <v>1203</v>
       </c>
-      <c r="D55" s="64"/>
-      <c r="E55" s="64"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="65"/>
       <c r="F55" s="58"/>
       <c r="G55" s="56"/>
       <c r="H55" s="56"/>
       <c r="I55" s="56"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="65"/>
+      <c r="A56" s="66"/>
       <c r="B56" s="5" t="s">
         <v>1204</v>
       </c>
-      <c r="C56" s="64" t="s">
+      <c r="C56" s="65" t="s">
         <v>1205</v>
       </c>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="65"/>
       <c r="F56" s="58"/>
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
       <c r="I56" s="56"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="65"/>
+      <c r="A57" s="66"/>
       <c r="B57" s="5" t="s">
         <v>1206</v>
       </c>
-      <c r="C57" s="64" t="s">
+      <c r="C57" s="65" t="s">
         <v>1207</v>
       </c>
-      <c r="D57" s="64"/>
-      <c r="E57" s="64"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="65"/>
       <c r="F57" s="58"/>
       <c r="G57" s="56"/>
       <c r="H57" s="56"/>
       <c r="I57" s="56"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="65"/>
+      <c r="A58" s="66"/>
       <c r="B58" s="5" t="s">
         <v>1208</v>
       </c>
-      <c r="C58" s="64" t="s">
+      <c r="C58" s="65" t="s">
         <v>1209</v>
       </c>
-      <c r="D58" s="64"/>
-      <c r="E58" s="64"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="65"/>
       <c r="F58" s="58"/>
       <c r="G58" s="56"/>
       <c r="H58" s="56"/>
@@ -24312,88 +24312,88 @@
       <c r="B59" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C59" s="64" t="s">
+      <c r="C59" s="65" t="s">
         <v>1211</v>
       </c>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="65"/>
       <c r="F59" s="58"/>
       <c r="G59" s="56"/>
       <c r="H59" s="56"/>
       <c r="I59" s="56"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="65" t="s">
+      <c r="A60" s="66" t="s">
         <v>1212</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1213</v>
       </c>
-      <c r="C60" s="64" t="s">
+      <c r="C60" s="65" t="s">
         <v>1214</v>
       </c>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="65"/>
       <c r="F60" s="58"/>
       <c r="G60" s="56"/>
       <c r="H60" s="56"/>
       <c r="I60" s="56"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="65"/>
+      <c r="A61" s="66"/>
       <c r="B61" s="5" t="s">
         <v>1215</v>
       </c>
-      <c r="C61" s="64" t="s">
+      <c r="C61" s="65" t="s">
         <v>1216</v>
       </c>
-      <c r="D61" s="64"/>
-      <c r="E61" s="64"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="65"/>
       <c r="F61" s="58"/>
       <c r="G61" s="56"/>
       <c r="H61" s="56"/>
       <c r="I61" s="56"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="65"/>
+      <c r="A62" s="66"/>
       <c r="B62" s="5" t="s">
         <v>1217</v>
       </c>
-      <c r="C62" s="64" t="s">
+      <c r="C62" s="65" t="s">
         <v>1218</v>
       </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
       <c r="F62" s="58"/>
       <c r="G62" s="56"/>
       <c r="H62" s="56"/>
       <c r="I62" s="56"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="65"/>
+      <c r="A63" s="66"/>
       <c r="B63" s="5" t="s">
         <v>1219</v>
       </c>
-      <c r="C63" s="64" t="s">
+      <c r="C63" s="65" t="s">
         <v>1220</v>
       </c>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
       <c r="F63" s="58"/>
       <c r="G63" s="56"/>
       <c r="H63" s="56"/>
       <c r="I63" s="56"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="65"/>
+      <c r="A64" s="66"/>
       <c r="B64" s="5" t="s">
         <v>1221</v>
       </c>
-      <c r="C64" s="64" t="s">
+      <c r="C64" s="65" t="s">
         <v>1222</v>
       </c>
-      <c r="D64" s="64"/>
-      <c r="E64" s="64"/>
+      <c r="D64" s="65"/>
+      <c r="E64" s="65"/>
       <c r="F64" s="58"/>
       <c r="G64" s="56"/>
       <c r="H64" s="56"/>
@@ -24401,30 +24401,72 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
@@ -24449,72 +24491,30 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -25850,13 +25850,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -25869,6 +25862,13 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26239,6 +26239,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
@@ -26246,18 +26258,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -26724,6 +26724,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -26737,19 +26750,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -27634,33 +27634,19 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:I23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="C24:D24"/>
@@ -27674,19 +27660,33 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28171,6 +28171,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -28181,13 +28188,6 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -28595,11 +28595,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -28612,6 +28607,11 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -28643,15 +28643,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -28880,6 +28871,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -28892,14 +28892,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28914,6 +28906,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
:memo: update CDM excel
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\db\dt4h\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FC43FCF-1579-4A22-982E-D8701F9C9113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E4262E-FA82-488D-8FE6-02DF78AB64CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" tabRatio="901" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" tabRatio="901" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,6 @@
     <sheet name="AllergyIntolerance" sheetId="31" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -860,7 +859,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4029" uniqueCount="1828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4033" uniqueCount="1830">
   <si>
     <t>Required</t>
   </si>
@@ -6359,6 +6358,12 @@
   </si>
   <si>
     <t>encounter-service-types</t>
+  </si>
+  <si>
+    <t>18049-7</t>
+  </si>
+  <si>
+    <t>Left ventricular Ejection fraction by US.M-mode+Calculated by Teichholz method</t>
   </si>
 </sst>
 </file>
@@ -11090,7 +11095,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A15" sqref="A15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14623,10 +14628,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF00AD05-AD0A-4301-B0FD-56AA1951174D}">
-  <dimension ref="A1:K149"/>
+  <dimension ref="A1:K150"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15114,7 +15119,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>1390</v>
+        <v>1828</v>
       </c>
       <c r="D25" t="s">
         <v>345</v>
@@ -15123,7 +15128,7 @@
         <v>671</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>1391</v>
+        <v>1829</v>
       </c>
       <c r="H25" s="46"/>
       <c r="I25" s="10"/>
@@ -15131,32 +15136,32 @@
       <c r="K25" s="10"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>1396</v>
-      </c>
       <c r="B26" t="s">
-        <v>1397</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1398</v>
+        <v>1390</v>
       </c>
       <c r="D26" t="s">
         <v>345</v>
       </c>
       <c r="E26" t="s">
-        <v>1399</v>
+        <v>671</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>1400</v>
-      </c>
-      <c r="H26" s="64"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
+        <v>1391</v>
+      </c>
+      <c r="H26" s="46"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1396</v>
+      </c>
       <c r="B27" t="s">
-        <v>1401</v>
+        <v>1397</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1398</v>
       </c>
       <c r="D27" t="s">
         <v>345</v>
@@ -15165,16 +15170,16 @@
         <v>1399</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>1402</v>
-      </c>
-      <c r="H27" s="46"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+        <v>1400</v>
+      </c>
+      <c r="H27" s="64"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="D28" t="s">
         <v>345</v>
@@ -15183,7 +15188,7 @@
         <v>1399</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="H28" s="46"/>
       <c r="I28" s="10"/>
@@ -15192,7 +15197,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="D29" t="s">
         <v>345</v>
@@ -15201,7 +15206,7 @@
         <v>1399</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="H29" s="46"/>
       <c r="I29" s="10"/>
@@ -15210,7 +15215,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="D30" t="s">
         <v>345</v>
@@ -15219,7 +15224,7 @@
         <v>1399</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="H30" s="46"/>
       <c r="I30" s="10"/>
@@ -15228,7 +15233,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="D31" t="s">
         <v>345</v>
@@ -15237,7 +15242,7 @@
         <v>1399</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="H31" s="46"/>
       <c r="I31" s="10"/>
@@ -15246,7 +15251,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D32" t="s">
         <v>345</v>
@@ -15255,7 +15260,7 @@
         <v>1399</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="H32" s="46"/>
       <c r="I32" s="10"/>
@@ -15264,7 +15269,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="D33" t="s">
         <v>345</v>
@@ -15273,7 +15278,7 @@
         <v>1399</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="H33" s="46"/>
       <c r="I33" s="10"/>
@@ -15282,7 +15287,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="D34" t="s">
         <v>345</v>
@@ -15291,7 +15296,7 @@
         <v>1399</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="H34" s="46"/>
       <c r="I34" s="10"/>
@@ -15299,11 +15304,8 @@
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>1417</v>
-      </c>
       <c r="B35" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="D35" t="s">
         <v>345</v>
@@ -15312,16 +15314,19 @@
         <v>1399</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>1419</v>
-      </c>
-      <c r="H35" s="64"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
+        <v>1416</v>
+      </c>
+      <c r="H35" s="46"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>1417</v>
+      </c>
       <c r="B36" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D36" t="s">
         <v>345</v>
@@ -15330,7 +15335,7 @@
         <v>1399</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="H36" s="64"/>
       <c r="I36" s="62"/>
@@ -15339,7 +15344,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="D37" t="s">
         <v>345</v>
@@ -15348,7 +15353,7 @@
         <v>1399</v>
       </c>
       <c r="F37" s="33" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="H37" s="64"/>
       <c r="I37" s="62"/>
@@ -15357,7 +15362,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="D38" t="s">
         <v>345</v>
@@ -15366,7 +15371,7 @@
         <v>1399</v>
       </c>
       <c r="F38" s="33" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="H38" s="64"/>
       <c r="I38" s="62"/>
@@ -15375,7 +15380,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="D39" t="s">
         <v>345</v>
@@ -15384,7 +15389,7 @@
         <v>1399</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="H39" s="64"/>
       <c r="I39" s="62"/>
@@ -15393,7 +15398,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="D40" t="s">
         <v>345</v>
@@ -15402,7 +15407,7 @@
         <v>1399</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="H40" s="64"/>
       <c r="I40" s="62"/>
@@ -15411,7 +15416,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="D41" t="s">
         <v>345</v>
@@ -15420,7 +15425,7 @@
         <v>1399</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="H41" s="64"/>
       <c r="I41" s="62"/>
@@ -15429,7 +15434,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="D42" t="s">
         <v>345</v>
@@ -15438,7 +15443,7 @@
         <v>1399</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="H42" s="64"/>
       <c r="I42" s="62"/>
@@ -15447,7 +15452,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="D43" t="s">
         <v>345</v>
@@ -15456,7 +15461,7 @@
         <v>1399</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="H43" s="64"/>
       <c r="I43" s="62"/>
@@ -15464,23 +15469,17 @@
       <c r="K43" s="62"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>1436</v>
-      </c>
       <c r="B44" t="s">
-        <v>1437</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1438</v>
+        <v>1434</v>
       </c>
       <c r="D44" t="s">
         <v>345</v>
       </c>
       <c r="E44" t="s">
-        <v>657</v>
+        <v>1399</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>1439</v>
+        <v>1435</v>
       </c>
       <c r="H44" s="64"/>
       <c r="I44" s="62"/>
@@ -15488,8 +15487,14 @@
       <c r="K44" s="62"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>1436</v>
+      </c>
       <c r="B45" t="s">
-        <v>1440</v>
+        <v>1437</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1438</v>
       </c>
       <c r="D45" t="s">
         <v>345</v>
@@ -15498,22 +15503,16 @@
         <v>657</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>1441</v>
-      </c>
-      <c r="H45" s="46"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
+        <v>1439</v>
+      </c>
+      <c r="H45" s="64"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>1442</v>
-      </c>
       <c r="B46" t="s">
-        <v>1443</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1444</v>
+        <v>1440</v>
       </c>
       <c r="D46" t="s">
         <v>345</v>
@@ -15522,16 +15521,22 @@
         <v>657</v>
       </c>
       <c r="F46" s="33" t="s">
-        <v>1445</v>
-      </c>
-      <c r="H46" s="64"/>
-      <c r="I46" s="62"/>
-      <c r="J46" s="62"/>
-      <c r="K46" s="62"/>
+        <v>1441</v>
+      </c>
+      <c r="H46" s="46"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>1442</v>
+      </c>
       <c r="B47" t="s">
-        <v>1446</v>
+        <v>1443</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1444</v>
       </c>
       <c r="D47" t="s">
         <v>345</v>
@@ -15540,28 +15545,25 @@
         <v>657</v>
       </c>
       <c r="F47" s="33" t="s">
+        <v>1445</v>
+      </c>
+      <c r="H47" s="64"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="62"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D48" t="s">
+        <v>345</v>
+      </c>
+      <c r="E48" t="s">
+        <v>657</v>
+      </c>
+      <c r="F48" s="33" t="s">
         <v>1447</v>
-      </c>
-      <c r="H47" s="46"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>1448</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1448</v>
-      </c>
-      <c r="D48" t="s">
-        <v>1449</v>
-      </c>
-      <c r="E48" t="s">
-        <v>1450</v>
-      </c>
-      <c r="F48" s="33" t="s">
-        <v>1451</v>
       </c>
       <c r="H48" s="46"/>
       <c r="I48" s="10"/>
@@ -15570,10 +15572,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="B49" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
       <c r="D49" t="s">
         <v>1449</v>
@@ -15582,28 +15584,28 @@
         <v>1450</v>
       </c>
       <c r="F49" s="33" t="s">
-        <v>1453</v>
-      </c>
-      <c r="H49" s="64"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="62"/>
-      <c r="K49" s="62"/>
+        <v>1451</v>
+      </c>
+      <c r="H49" s="46"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B50" t="s">
-        <v>1455</v>
+        <v>1452</v>
       </c>
       <c r="D50" t="s">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E50" t="s">
-        <v>671</v>
+        <v>1450</v>
       </c>
       <c r="F50" s="33" t="s">
-        <v>1456</v>
+        <v>1453</v>
       </c>
       <c r="H50" s="64"/>
       <c r="I50" s="62"/>
@@ -15612,19 +15614,19 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
       <c r="B51" t="s">
-        <v>1458</v>
+        <v>1455</v>
       </c>
       <c r="D51" t="s">
         <v>345</v>
       </c>
       <c r="E51" t="s">
-        <v>657</v>
+        <v>671</v>
       </c>
       <c r="F51" s="33" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="H51" s="64"/>
       <c r="I51" s="62"/>
@@ -15633,10 +15635,10 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="B52" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="D52" t="s">
         <v>345</v>
@@ -15645,7 +15647,7 @@
         <v>657</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>1462</v>
+        <v>1459</v>
       </c>
       <c r="H52" s="64"/>
       <c r="I52" s="62"/>
@@ -15654,10 +15656,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="B53" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="D53" t="s">
         <v>345</v>
@@ -15666,7 +15668,7 @@
         <v>657</v>
       </c>
       <c r="F53" s="33" t="s">
-        <v>1465</v>
+        <v>1462</v>
       </c>
       <c r="H53" s="64"/>
       <c r="I53" s="62"/>
@@ -15675,10 +15677,10 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1466</v>
+        <v>1463</v>
       </c>
       <c r="B54" t="s">
-        <v>1467</v>
+        <v>1464</v>
       </c>
       <c r="D54" t="s">
         <v>345</v>
@@ -15687,7 +15689,7 @@
         <v>657</v>
       </c>
       <c r="F54" s="33" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
       <c r="H54" s="64"/>
       <c r="I54" s="62"/>
@@ -15695,8 +15697,11 @@
       <c r="K54" s="62"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>1466</v>
+      </c>
       <c r="B55" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="D55" t="s">
         <v>345</v>
@@ -15705,19 +15710,16 @@
         <v>657</v>
       </c>
       <c r="F55" s="33" t="s">
-        <v>1470</v>
-      </c>
-      <c r="H55" s="46"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
+        <v>1468</v>
+      </c>
+      <c r="H55" s="64"/>
+      <c r="I55" s="62"/>
+      <c r="J55" s="62"/>
+      <c r="K55" s="62"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>1471</v>
-      </c>
       <c r="B56" t="s">
-        <v>1472</v>
+        <v>1469</v>
       </c>
       <c r="D56" t="s">
         <v>345</v>
@@ -15726,16 +15728,19 @@
         <v>657</v>
       </c>
       <c r="F56" s="33" t="s">
-        <v>1473</v>
-      </c>
-      <c r="H56" s="64"/>
-      <c r="I56" s="62"/>
-      <c r="J56" s="62"/>
-      <c r="K56" s="62"/>
+        <v>1470</v>
+      </c>
+      <c r="H56" s="46"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>1471</v>
+      </c>
       <c r="B57" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="D57" t="s">
         <v>345</v>
@@ -15744,37 +15749,37 @@
         <v>657</v>
       </c>
       <c r="F57" s="33" t="s">
-        <v>1475</v>
-      </c>
-      <c r="H57" s="46"/>
-      <c r="I57" s="10"/>
-      <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
+        <v>1473</v>
+      </c>
+      <c r="H57" s="64"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="62"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>1476</v>
-      </c>
       <c r="B58" t="s">
-        <v>1477</v>
+        <v>1474</v>
       </c>
       <c r="D58" t="s">
         <v>345</v>
       </c>
       <c r="E58" t="s">
-        <v>1478</v>
+        <v>657</v>
       </c>
       <c r="F58" s="33" t="s">
-        <v>1479</v>
-      </c>
-      <c r="H58" s="64"/>
-      <c r="I58" s="62"/>
-      <c r="J58" s="62"/>
-      <c r="K58" s="62"/>
+        <v>1475</v>
+      </c>
+      <c r="H58" s="46"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>1476</v>
+      </c>
       <c r="B59" t="s">
-        <v>1480</v>
+        <v>1477</v>
       </c>
       <c r="D59" t="s">
         <v>345</v>
@@ -15783,7 +15788,7 @@
         <v>1478</v>
       </c>
       <c r="F59" s="33" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="H59" s="64"/>
       <c r="I59" s="62"/>
@@ -15791,20 +15796,17 @@
       <c r="K59" s="62"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>1482</v>
-      </c>
       <c r="B60" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="D60" t="s">
-        <v>1449</v>
+        <v>345</v>
       </c>
       <c r="E60" t="s">
-        <v>1343</v>
+        <v>1478</v>
       </c>
       <c r="F60" s="33" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="H60" s="64"/>
       <c r="I60" s="62"/>
@@ -15813,10 +15815,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="B61" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="D61" t="s">
         <v>1449</v>
@@ -15825,7 +15827,7 @@
         <v>1343</v>
       </c>
       <c r="F61" s="33" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="H61" s="64"/>
       <c r="I61" s="62"/>
@@ -15834,19 +15836,19 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="B62" t="s">
-        <v>1487</v>
+        <v>1484</v>
       </c>
       <c r="D62" t="s">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E62" t="s">
-        <v>1488</v>
+        <v>1343</v>
       </c>
       <c r="F62" s="33" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="H62" s="64"/>
       <c r="I62" s="62"/>
@@ -15855,10 +15857,10 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
       <c r="B63" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="D63" t="s">
         <v>345</v>
@@ -15867,7 +15869,7 @@
         <v>1488</v>
       </c>
       <c r="F63" s="33" t="s">
-        <v>1492</v>
+        <v>1489</v>
       </c>
       <c r="H63" s="64"/>
       <c r="I63" s="62"/>
@@ -15876,19 +15878,19 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1493</v>
+        <v>1490</v>
       </c>
       <c r="B64" t="s">
-        <v>1494</v>
+        <v>1491</v>
       </c>
       <c r="D64" t="s">
         <v>345</v>
       </c>
       <c r="E64" t="s">
-        <v>1478</v>
+        <v>1488</v>
       </c>
       <c r="F64" s="33" t="s">
-        <v>1495</v>
+        <v>1492</v>
       </c>
       <c r="H64" s="64"/>
       <c r="I64" s="62"/>
@@ -15897,52 +15899,52 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1496</v>
+        <v>1493</v>
       </c>
       <c r="B65" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="D65" t="s">
         <v>345</v>
       </c>
       <c r="E65" t="s">
-        <v>1488</v>
+        <v>1478</v>
       </c>
       <c r="F65" s="33" t="s">
-        <v>1498</v>
-      </c>
-      <c r="H65" s="46"/>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
+        <v>1495</v>
+      </c>
+      <c r="H65" s="64"/>
+      <c r="I65" s="62"/>
+      <c r="J65" s="62"/>
+      <c r="K65" s="62"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1499</v>
+        <v>1496</v>
       </c>
       <c r="B66" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="D66" t="s">
-        <v>1449</v>
+        <v>345</v>
       </c>
       <c r="E66" t="s">
         <v>1488</v>
       </c>
       <c r="F66" s="33" t="s">
-        <v>1500</v>
-      </c>
-      <c r="H66" s="64"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="62"/>
-      <c r="K66" s="62"/>
+        <v>1498</v>
+      </c>
+      <c r="H66" s="46"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="B67" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="D67" t="s">
         <v>1449</v>
@@ -15951,7 +15953,7 @@
         <v>1488</v>
       </c>
       <c r="F67" s="33" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="H67" s="64"/>
       <c r="I67" s="62"/>
@@ -15960,19 +15962,19 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="B68" t="s">
-        <v>1504</v>
+        <v>1501</v>
       </c>
       <c r="D68" t="s">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E68" t="s">
-        <v>1478</v>
+        <v>1488</v>
       </c>
       <c r="F68" s="33" t="s">
-        <v>1505</v>
+        <v>1502</v>
       </c>
       <c r="H68" s="64"/>
       <c r="I68" s="62"/>
@@ -15981,58 +15983,58 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1506</v>
+        <v>1503</v>
       </c>
       <c r="B69" t="s">
-        <v>1507</v>
+        <v>1504</v>
       </c>
       <c r="D69" t="s">
         <v>345</v>
       </c>
+      <c r="E69" t="s">
+        <v>1478</v>
+      </c>
       <c r="F69" s="33" t="s">
-        <v>1508</v>
-      </c>
-      <c r="H69" s="46"/>
-      <c r="I69" s="10"/>
-      <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
+        <v>1505</v>
+      </c>
+      <c r="H69" s="64"/>
+      <c r="I69" s="62"/>
+      <c r="J69" s="62"/>
+      <c r="K69" s="62"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1509</v>
+        <v>1506</v>
       </c>
       <c r="B70" t="s">
-        <v>1510</v>
+        <v>1507</v>
       </c>
       <c r="D70" t="s">
         <v>345</v>
       </c>
-      <c r="E70" t="s">
-        <v>1511</v>
-      </c>
       <c r="F70" s="33" t="s">
-        <v>1512</v>
-      </c>
-      <c r="H70" s="64"/>
-      <c r="I70" s="62"/>
-      <c r="J70" s="62"/>
-      <c r="K70" s="62"/>
+        <v>1508</v>
+      </c>
+      <c r="H70" s="46"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1513</v>
+        <v>1509</v>
       </c>
       <c r="B71" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="D71" t="s">
         <v>345</v>
       </c>
       <c r="E71" t="s">
-        <v>1488</v>
+        <v>1511</v>
       </c>
       <c r="F71" s="33" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
       <c r="H71" s="64"/>
       <c r="I71" s="62"/>
@@ -16041,10 +16043,10 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1516</v>
+        <v>1513</v>
       </c>
       <c r="B72" t="s">
-        <v>1517</v>
+        <v>1514</v>
       </c>
       <c r="D72" t="s">
         <v>345</v>
@@ -16053,46 +16055,46 @@
         <v>1488</v>
       </c>
       <c r="F72" s="33" t="s">
-        <v>1518</v>
-      </c>
-      <c r="H72" s="46"/>
-      <c r="I72" s="10"/>
-      <c r="J72" s="10"/>
-      <c r="K72" s="10"/>
+        <v>1515</v>
+      </c>
+      <c r="H72" s="64"/>
+      <c r="I72" s="62"/>
+      <c r="J72" s="62"/>
+      <c r="K72" s="62"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1519</v>
+        <v>1516</v>
       </c>
       <c r="B73" t="s">
-        <v>1520</v>
+        <v>1517</v>
       </c>
       <c r="D73" t="s">
         <v>345</v>
       </c>
+      <c r="E73" t="s">
+        <v>1488</v>
+      </c>
       <c r="F73" s="33" t="s">
-        <v>1521</v>
-      </c>
-      <c r="H73" s="64"/>
-      <c r="I73" s="62"/>
-      <c r="J73" s="62"/>
-      <c r="K73" s="62"/>
+        <v>1518</v>
+      </c>
+      <c r="H73" s="46"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1522</v>
+        <v>1519</v>
       </c>
       <c r="B74" t="s">
-        <v>1523</v>
+        <v>1520</v>
       </c>
       <c r="D74" t="s">
         <v>345</v>
       </c>
-      <c r="E74" t="s">
-        <v>657</v>
-      </c>
       <c r="F74" s="33" t="s">
-        <v>1524</v>
+        <v>1521</v>
       </c>
       <c r="H74" s="64"/>
       <c r="I74" s="62"/>
@@ -16101,22 +16103,19 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>1525</v>
+        <v>1522</v>
       </c>
       <c r="B75" t="s">
-        <v>1526</v>
+        <v>1523</v>
       </c>
       <c r="D75" t="s">
         <v>345</v>
       </c>
       <c r="E75" t="s">
-        <v>1488</v>
+        <v>657</v>
       </c>
       <c r="F75" s="33" t="s">
-        <v>1527</v>
-      </c>
-      <c r="G75" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
       <c r="H75" s="64"/>
       <c r="I75" s="62"/>
@@ -16125,19 +16124,22 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>1529</v>
+        <v>1525</v>
       </c>
       <c r="B76" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="D76" t="s">
-        <v>1449</v>
+        <v>345</v>
       </c>
       <c r="E76" t="s">
-        <v>1450</v>
+        <v>1488</v>
       </c>
       <c r="F76" s="33" t="s">
-        <v>1530</v>
+        <v>1527</v>
+      </c>
+      <c r="G76" t="s">
+        <v>1528</v>
       </c>
       <c r="H76" s="64"/>
       <c r="I76" s="62"/>
@@ -16146,10 +16148,10 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="B77" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="D77" t="s">
         <v>1449</v>
@@ -16158,7 +16160,7 @@
         <v>1450</v>
       </c>
       <c r="F77" s="33" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="H77" s="64"/>
       <c r="I77" s="62"/>
@@ -16167,10 +16169,10 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="B78" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="D78" t="s">
         <v>1449</v>
@@ -16179,7 +16181,7 @@
         <v>1450</v>
       </c>
       <c r="F78" s="33" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="H78" s="64"/>
       <c r="I78" s="62"/>
@@ -16188,10 +16190,10 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="B79" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="D79" t="s">
         <v>1449</v>
@@ -16200,7 +16202,7 @@
         <v>1450</v>
       </c>
       <c r="F79" s="33" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="H79" s="64"/>
       <c r="I79" s="62"/>
@@ -16208,17 +16210,20 @@
       <c r="K79" s="62"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>1535</v>
+      </c>
       <c r="B80" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="D80" t="s">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E80" t="s">
-        <v>657</v>
+        <v>1450</v>
       </c>
       <c r="F80" s="33" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="H80" s="64"/>
       <c r="I80" s="62"/>
@@ -16227,7 +16232,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="D81" t="s">
         <v>345</v>
@@ -16236,7 +16241,7 @@
         <v>657</v>
       </c>
       <c r="F81" s="33" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="H81" s="64"/>
       <c r="I81" s="62"/>
@@ -16245,7 +16250,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="D82" t="s">
         <v>345</v>
@@ -16254,7 +16259,7 @@
         <v>657</v>
       </c>
       <c r="F82" s="33" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="H82" s="64"/>
       <c r="I82" s="62"/>
@@ -16262,20 +16267,17 @@
       <c r="K82" s="62"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>1543</v>
-      </c>
       <c r="B83" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="D83" t="s">
-        <v>1449</v>
+        <v>345</v>
       </c>
       <c r="E83" t="s">
-        <v>1399</v>
+        <v>657</v>
       </c>
       <c r="F83" s="33" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="H83" s="64"/>
       <c r="I83" s="62"/>
@@ -16284,10 +16286,10 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="B84" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="D84" t="s">
         <v>1449</v>
@@ -16296,7 +16298,7 @@
         <v>1399</v>
       </c>
       <c r="F84" s="33" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="H84" s="64"/>
       <c r="I84" s="62"/>
@@ -16305,10 +16307,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="B85" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="D85" t="s">
         <v>1449</v>
@@ -16317,7 +16319,7 @@
         <v>1399</v>
       </c>
       <c r="F85" s="33" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="H85" s="64"/>
       <c r="I85" s="62"/>
@@ -16326,19 +16328,19 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="B86" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="D86" t="s">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E86" t="s">
-        <v>1551</v>
+        <v>1399</v>
       </c>
       <c r="F86" s="33" t="s">
-        <v>1552</v>
+        <v>1548</v>
       </c>
       <c r="H86" s="64"/>
       <c r="I86" s="62"/>
@@ -16346,8 +16348,11 @@
       <c r="K86" s="62"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>1549</v>
+      </c>
       <c r="B87" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="D87" t="s">
         <v>345</v>
@@ -16356,7 +16361,7 @@
         <v>1551</v>
       </c>
       <c r="F87" s="33" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="H87" s="64"/>
       <c r="I87" s="62"/>
@@ -16365,7 +16370,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="D88" t="s">
         <v>345</v>
@@ -16374,7 +16379,7 @@
         <v>1551</v>
       </c>
       <c r="F88" s="33" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="H88" s="64"/>
       <c r="I88" s="62"/>
@@ -16382,20 +16387,17 @@
       <c r="K88" s="62"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>1557</v>
-      </c>
       <c r="B89" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
       <c r="D89" t="s">
         <v>345</v>
       </c>
       <c r="E89" t="s">
-        <v>1450</v>
+        <v>1551</v>
       </c>
       <c r="F89" s="33" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
       <c r="H89" s="64"/>
       <c r="I89" s="62"/>
@@ -16404,19 +16406,19 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1560</v>
+        <v>1557</v>
       </c>
       <c r="B90" t="s">
-        <v>1561</v>
+        <v>1558</v>
       </c>
       <c r="D90" t="s">
         <v>345</v>
       </c>
       <c r="E90" t="s">
-        <v>657</v>
+        <v>1450</v>
       </c>
       <c r="F90" s="33" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="H90" s="64"/>
       <c r="I90" s="62"/>
@@ -16425,10 +16427,10 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="B91" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="D91" t="s">
         <v>345</v>
@@ -16437,7 +16439,7 @@
         <v>657</v>
       </c>
       <c r="F91" s="33" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
       <c r="H91" s="64"/>
       <c r="I91" s="62"/>
@@ -16446,10 +16448,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="B92" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="D92" t="s">
         <v>345</v>
@@ -16458,7 +16460,7 @@
         <v>657</v>
       </c>
       <c r="F92" s="33" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="H92" s="64"/>
       <c r="I92" s="62"/>
@@ -16467,19 +16469,19 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="B93" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="D93" t="s">
         <v>345</v>
       </c>
       <c r="E93" t="s">
-        <v>1450</v>
+        <v>657</v>
       </c>
       <c r="F93" s="33" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="H93" s="64"/>
       <c r="I93" s="62"/>
@@ -16488,19 +16490,19 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="B94" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="D94" t="s">
-        <v>1449</v>
+        <v>345</v>
       </c>
       <c r="E94" t="s">
-        <v>657</v>
+        <v>1450</v>
       </c>
       <c r="F94" s="33" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="H94" s="64"/>
       <c r="I94" s="62"/>
@@ -16509,19 +16511,19 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="B95" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="D95" t="s">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E95" t="s">
         <v>657</v>
       </c>
       <c r="F95" s="33" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="H95" s="64"/>
       <c r="I95" s="62"/>
@@ -16530,19 +16532,19 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="B96" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="D96" t="s">
-        <v>1449</v>
+        <v>345</v>
       </c>
       <c r="E96" t="s">
-        <v>1361</v>
+        <v>657</v>
       </c>
       <c r="F96" s="33" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="H96" s="64"/>
       <c r="I96" s="62"/>
@@ -16551,19 +16553,19 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="B97" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="D97" t="s">
-        <v>345</v>
+        <v>1449</v>
       </c>
       <c r="E97" t="s">
         <v>1361</v>
       </c>
       <c r="F97" s="33" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="H97" s="64"/>
       <c r="I97" s="62"/>
@@ -16572,19 +16574,19 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="B98" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="D98" t="s">
         <v>345</v>
       </c>
       <c r="E98" t="s">
-        <v>1399</v>
+        <v>1361</v>
       </c>
       <c r="F98" s="33" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="H98" s="64"/>
       <c r="I98" s="62"/>
@@ -16592,11 +16594,11 @@
       <c r="K98" s="62"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>1582</v>
+      </c>
       <c r="B99" t="s">
-        <v>1585</v>
-      </c>
-      <c r="C99" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="D99" t="s">
         <v>345</v>
@@ -16605,7 +16607,7 @@
         <v>1399</v>
       </c>
       <c r="F99" s="33" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="H99" s="64"/>
       <c r="I99" s="62"/>
@@ -16614,7 +16616,10 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>1588</v>
+        <v>1585</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1586</v>
       </c>
       <c r="D100" t="s">
         <v>345</v>
@@ -16623,7 +16628,7 @@
         <v>1399</v>
       </c>
       <c r="F100" s="33" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="H100" s="64"/>
       <c r="I100" s="62"/>
@@ -16632,7 +16637,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="D101" t="s">
         <v>345</v>
@@ -16641,7 +16646,7 @@
         <v>1399</v>
       </c>
       <c r="F101" s="33" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="H101" s="64"/>
       <c r="I101" s="62"/>
@@ -16649,20 +16654,17 @@
       <c r="K101" s="62"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>1592</v>
-      </c>
       <c r="B102" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="D102" t="s">
         <v>345</v>
       </c>
       <c r="E102" t="s">
-        <v>1551</v>
+        <v>1399</v>
       </c>
       <c r="F102" s="33" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="H102" s="64"/>
       <c r="I102" s="62"/>
@@ -16671,19 +16673,19 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="B103" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
       <c r="D103" t="s">
         <v>345</v>
       </c>
       <c r="E103" t="s">
-        <v>1399</v>
+        <v>1551</v>
       </c>
       <c r="F103" s="33" t="s">
-        <v>1300</v>
+        <v>1594</v>
       </c>
       <c r="H103" s="64"/>
       <c r="I103" s="62"/>
@@ -16691,25 +16693,28 @@
       <c r="K103" s="62"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F104" s="33"/>
+      <c r="A104" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D104" t="s">
+        <v>345</v>
+      </c>
+      <c r="E104" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F104" s="33" t="s">
+        <v>1300</v>
+      </c>
       <c r="H104" s="64"/>
       <c r="I104" s="62"/>
       <c r="J104" s="62"/>
       <c r="K104" s="62"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B105" s="49" t="s">
-        <v>1597</v>
-      </c>
-      <c r="D105" t="s">
-        <v>345</v>
-      </c>
-      <c r="E105" s="49" t="s">
-        <v>657</v>
-      </c>
-      <c r="F105" s="50" t="s">
-        <v>1598</v>
-      </c>
+      <c r="F105" s="33"/>
       <c r="H105" s="64"/>
       <c r="I105" s="62"/>
       <c r="J105" s="62"/>
@@ -16717,16 +16722,16 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B106" s="49" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="D106" t="s">
         <v>345</v>
       </c>
       <c r="E106" s="49" t="s">
-        <v>1399</v>
+        <v>657</v>
       </c>
       <c r="F106" s="50" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="H106" s="64"/>
       <c r="I106" s="62"/>
@@ -16735,16 +16740,16 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B107" s="49" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="D107" t="s">
         <v>345</v>
       </c>
       <c r="E107" s="49" t="s">
-        <v>1602</v>
+        <v>1399</v>
       </c>
       <c r="F107" s="50" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="H107" s="64"/>
       <c r="I107" s="62"/>
@@ -16753,16 +16758,16 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B108" s="49" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
       <c r="D108" t="s">
         <v>345</v>
       </c>
       <c r="E108" s="49" t="s">
-        <v>1399</v>
+        <v>1602</v>
       </c>
       <c r="F108" s="50" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="H108" s="64"/>
       <c r="I108" s="62"/>
@@ -16771,7 +16776,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B109" s="49" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="D109" t="s">
         <v>345</v>
@@ -16780,7 +16785,7 @@
         <v>1399</v>
       </c>
       <c r="F109" s="50" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="H109" s="64"/>
       <c r="I109" s="62"/>
@@ -16789,16 +16794,16 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B110" s="49" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="D110" t="s">
         <v>345</v>
       </c>
       <c r="E110" s="49" t="s">
-        <v>1488</v>
+        <v>1399</v>
       </c>
       <c r="F110" s="50" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="H110" s="64"/>
       <c r="I110" s="62"/>
@@ -16807,16 +16812,16 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B111" s="49" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="D111" t="s">
         <v>345</v>
       </c>
       <c r="E111" s="49" t="s">
-        <v>1511</v>
+        <v>1488</v>
       </c>
       <c r="F111" s="50" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="H111" s="64"/>
       <c r="I111" s="62"/>
@@ -16825,14 +16830,16 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B112" s="49" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="D112" t="s">
         <v>345</v>
       </c>
-      <c r="E112" s="49"/>
+      <c r="E112" s="49" t="s">
+        <v>1511</v>
+      </c>
       <c r="F112" s="50" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="H112" s="64"/>
       <c r="I112" s="62"/>
@@ -16841,16 +16848,14 @@
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B113" s="49" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="D113" t="s">
         <v>345</v>
       </c>
-      <c r="E113" s="49" t="s">
-        <v>1488</v>
-      </c>
+      <c r="E113" s="49"/>
       <c r="F113" s="50" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="H113" s="64"/>
       <c r="I113" s="62"/>
@@ -16859,7 +16864,7 @@
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B114" s="49" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="D114" t="s">
         <v>345</v>
@@ -16868,7 +16873,7 @@
         <v>1488</v>
       </c>
       <c r="F114" s="50" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="H114" s="64"/>
       <c r="I114" s="62"/>
@@ -16877,7 +16882,7 @@
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B115" s="49" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="D115" t="s">
         <v>345</v>
@@ -16886,7 +16891,7 @@
         <v>1488</v>
       </c>
       <c r="F115" s="50" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="H115" s="64"/>
       <c r="I115" s="62"/>
@@ -16895,7 +16900,7 @@
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B116" s="49" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="D116" t="s">
         <v>345</v>
@@ -16904,7 +16909,7 @@
         <v>1488</v>
       </c>
       <c r="F116" s="50" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="H116" s="64"/>
       <c r="I116" s="62"/>
@@ -16913,16 +16918,16 @@
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B117" s="49" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="D117" t="s">
         <v>345</v>
       </c>
       <c r="E117" s="49" t="s">
-        <v>1623</v>
+        <v>1488</v>
       </c>
       <c r="F117" s="50" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
       <c r="H117" s="64"/>
       <c r="I117" s="62"/>
@@ -16931,16 +16936,16 @@
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B118" s="49" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="D118" t="s">
         <v>345</v>
       </c>
       <c r="E118" s="49" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="F118" s="50" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="H118" s="64"/>
       <c r="I118" s="62"/>
@@ -16949,14 +16954,16 @@
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B119" s="49" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="D119" t="s">
         <v>345</v>
       </c>
-      <c r="E119" s="49"/>
+      <c r="E119" s="49" t="s">
+        <v>1626</v>
+      </c>
       <c r="F119" s="50" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="H119" s="64"/>
       <c r="I119" s="62"/>
@@ -16965,16 +16972,14 @@
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B120" s="49" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="D120" t="s">
         <v>345</v>
       </c>
-      <c r="E120" s="49" t="s">
-        <v>1631</v>
-      </c>
+      <c r="E120" s="49"/>
       <c r="F120" s="50" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
       <c r="H120" s="64"/>
       <c r="I120" s="62"/>
@@ -16983,16 +16988,16 @@
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B121" s="49" t="s">
-        <v>1633</v>
+        <v>1630</v>
       </c>
       <c r="D121" t="s">
         <v>345</v>
       </c>
       <c r="E121" s="49" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
       <c r="F121" s="50" t="s">
-        <v>1635</v>
+        <v>1632</v>
       </c>
       <c r="H121" s="64"/>
       <c r="I121" s="62"/>
@@ -17001,16 +17006,16 @@
     </row>
     <row r="122" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B122" s="49" t="s">
-        <v>1636</v>
+        <v>1633</v>
       </c>
       <c r="D122" t="s">
         <v>345</v>
       </c>
       <c r="E122" s="49" t="s">
-        <v>657</v>
+        <v>1634</v>
       </c>
       <c r="F122" s="50" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="H122" s="64"/>
       <c r="I122" s="62"/>
@@ -17019,16 +17024,16 @@
     </row>
     <row r="123" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B123" s="49" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="D123" t="s">
         <v>345</v>
       </c>
       <c r="E123" s="49" t="s">
-        <v>1631</v>
+        <v>657</v>
       </c>
       <c r="F123" s="50" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="H123" s="64"/>
       <c r="I123" s="62"/>
@@ -17037,16 +17042,16 @@
     </row>
     <row r="124" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B124" s="49" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="D124" t="s">
         <v>345</v>
       </c>
       <c r="E124" s="49" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
       <c r="F124" s="50" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="H124" s="64"/>
       <c r="I124" s="62"/>
@@ -17055,16 +17060,16 @@
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B125" s="49" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="D125" t="s">
         <v>345</v>
       </c>
       <c r="E125" s="49" t="s">
-        <v>1631</v>
+        <v>1634</v>
       </c>
       <c r="F125" s="50" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="H125" s="64"/>
       <c r="I125" s="62"/>
@@ -17073,16 +17078,16 @@
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B126" s="49" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="D126" t="s">
         <v>345</v>
       </c>
       <c r="E126" s="49" t="s">
-        <v>1488</v>
+        <v>1631</v>
       </c>
       <c r="F126" s="50" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="H126" s="64"/>
       <c r="I126" s="62"/>
@@ -17091,16 +17096,16 @@
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B127" s="49" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="D127" t="s">
         <v>345</v>
       </c>
       <c r="E127" s="49" t="s">
-        <v>1551</v>
+        <v>1488</v>
       </c>
       <c r="F127" s="50" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="H127" s="64"/>
       <c r="I127" s="62"/>
@@ -17109,7 +17114,7 @@
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B128" s="49" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="D128" t="s">
         <v>345</v>
@@ -17118,7 +17123,7 @@
         <v>1551</v>
       </c>
       <c r="F128" s="50" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="H128" s="64"/>
       <c r="I128" s="62"/>
@@ -17127,16 +17132,16 @@
     </row>
     <row r="129" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B129" s="49" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="D129" t="s">
         <v>345</v>
       </c>
       <c r="E129" s="49" t="s">
-        <v>1651</v>
+        <v>1551</v>
       </c>
       <c r="F129" s="50" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
       <c r="H129" s="64"/>
       <c r="I129" s="62"/>
@@ -17145,16 +17150,16 @@
     </row>
     <row r="130" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B130" s="49" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
       <c r="D130" t="s">
         <v>345</v>
       </c>
       <c r="E130" s="49" t="s">
-        <v>1488</v>
+        <v>1651</v>
       </c>
       <c r="F130" s="50" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="H130" s="64"/>
       <c r="I130" s="62"/>
@@ -17163,16 +17168,16 @@
     </row>
     <row r="131" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B131" s="49" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="D131" t="s">
         <v>345</v>
       </c>
       <c r="E131" s="49" t="s">
-        <v>1656</v>
+        <v>1488</v>
       </c>
       <c r="F131" s="50" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="H131" s="64"/>
       <c r="I131" s="62"/>
@@ -17181,16 +17186,16 @@
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B132" s="49" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
       <c r="D132" t="s">
         <v>345</v>
       </c>
       <c r="E132" s="49" t="s">
-        <v>1626</v>
+        <v>1656</v>
       </c>
       <c r="F132" s="50" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="H132" s="64"/>
       <c r="I132" s="62"/>
@@ -17199,16 +17204,16 @@
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B133" s="49" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="D133" t="s">
         <v>345</v>
       </c>
       <c r="E133" s="49" t="s">
-        <v>657</v>
+        <v>1626</v>
       </c>
       <c r="F133" s="50" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="H133" s="64"/>
       <c r="I133" s="62"/>
@@ -17217,7 +17222,7 @@
     </row>
     <row r="134" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B134" s="49" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="D134" t="s">
         <v>345</v>
@@ -17226,7 +17231,7 @@
         <v>657</v>
       </c>
       <c r="F134" s="50" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="H134" s="64"/>
       <c r="I134" s="62"/>
@@ -17235,16 +17240,16 @@
     </row>
     <row r="135" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B135" s="49" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="D135" t="s">
         <v>345</v>
       </c>
       <c r="E135" s="49" t="s">
-        <v>1631</v>
+        <v>657</v>
       </c>
       <c r="F135" s="50" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="H135" s="64"/>
       <c r="I135" s="62"/>
@@ -17253,16 +17258,16 @@
     </row>
     <row r="136" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B136" s="49" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="D136" t="s">
         <v>345</v>
       </c>
       <c r="E136" s="49" t="s">
-        <v>1488</v>
+        <v>1631</v>
       </c>
       <c r="F136" s="50" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="H136" s="64"/>
       <c r="I136" s="62"/>
@@ -17271,14 +17276,16 @@
     </row>
     <row r="137" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B137" s="49" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="D137" t="s">
         <v>345</v>
       </c>
-      <c r="E137" s="49"/>
+      <c r="E137" s="49" t="s">
+        <v>1488</v>
+      </c>
       <c r="F137" s="50" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
       <c r="H137" s="64"/>
       <c r="I137" s="62"/>
@@ -17287,14 +17294,14 @@
     </row>
     <row r="138" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B138" s="49" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="D138" t="s">
         <v>345</v>
       </c>
       <c r="E138" s="49"/>
       <c r="F138" s="50" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="H138" s="64"/>
       <c r="I138" s="62"/>
@@ -17303,19 +17310,14 @@
     </row>
     <row r="139" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B139" s="49" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="D139" t="s">
         <v>345</v>
       </c>
-      <c r="E139" s="49" t="s">
-        <v>1528</v>
-      </c>
+      <c r="E139" s="49"/>
       <c r="F139" s="50" t="s">
-        <v>1673</v>
-      </c>
-      <c r="G139" s="49" t="s">
-        <v>1528</v>
+        <v>1671</v>
       </c>
       <c r="H139" s="64"/>
       <c r="I139" s="62"/>
@@ -17324,16 +17326,19 @@
     </row>
     <row r="140" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B140" s="49" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="D140" t="s">
         <v>345</v>
       </c>
       <c r="E140" s="49" t="s">
-        <v>1626</v>
+        <v>1528</v>
       </c>
       <c r="F140" s="50" t="s">
-        <v>1675</v>
+        <v>1673</v>
+      </c>
+      <c r="G140" s="49" t="s">
+        <v>1528</v>
       </c>
       <c r="H140" s="64"/>
       <c r="I140" s="62"/>
@@ -17342,16 +17347,16 @@
     </row>
     <row r="141" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B141" s="49" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="D141" t="s">
         <v>345</v>
       </c>
       <c r="E141" s="49" t="s">
-        <v>1634</v>
+        <v>1626</v>
       </c>
       <c r="F141" s="50" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
       <c r="H141" s="64"/>
       <c r="I141" s="62"/>
@@ -17360,16 +17365,16 @@
     </row>
     <row r="142" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B142" s="49" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="D142" t="s">
         <v>345</v>
       </c>
       <c r="E142" s="49" t="s">
-        <v>1626</v>
+        <v>1634</v>
       </c>
       <c r="F142" s="50" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="H142" s="64"/>
       <c r="I142" s="62"/>
@@ -17378,16 +17383,16 @@
     </row>
     <row r="143" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B143" s="49" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="D143" t="s">
         <v>345</v>
       </c>
       <c r="E143" s="49" t="s">
-        <v>1634</v>
+        <v>1626</v>
       </c>
       <c r="F143" s="50" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="H143" s="64"/>
       <c r="I143" s="62"/>
@@ -17396,16 +17401,16 @@
     </row>
     <row r="144" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B144" s="49" t="s">
-        <v>1398</v>
+        <v>1680</v>
       </c>
       <c r="D144" t="s">
         <v>345</v>
       </c>
       <c r="E144" s="49" t="s">
-        <v>1602</v>
+        <v>1634</v>
       </c>
       <c r="F144" s="50" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="H144" s="64"/>
       <c r="I144" s="62"/>
@@ -17414,7 +17419,7 @@
     </row>
     <row r="145" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B145" s="49" t="s">
-        <v>1683</v>
+        <v>1398</v>
       </c>
       <c r="D145" t="s">
         <v>345</v>
@@ -17423,7 +17428,7 @@
         <v>1602</v>
       </c>
       <c r="F145" s="50" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="H145" s="64"/>
       <c r="I145" s="62"/>
@@ -17432,16 +17437,16 @@
     </row>
     <row r="146" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B146" s="49" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="D146" t="s">
         <v>345</v>
       </c>
       <c r="E146" s="49" t="s">
-        <v>657</v>
+        <v>1602</v>
       </c>
       <c r="F146" s="50" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="H146" s="64"/>
       <c r="I146" s="62"/>
@@ -17450,7 +17455,7 @@
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B147" s="49" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="D147" t="s">
         <v>345</v>
@@ -17459,7 +17464,7 @@
         <v>657</v>
       </c>
       <c r="F147" s="50" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="H147" s="64"/>
       <c r="I147" s="62"/>
@@ -17468,14 +17473,16 @@
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B148" s="49" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="D148" t="s">
         <v>345</v>
       </c>
-      <c r="E148" s="49"/>
+      <c r="E148" s="49" t="s">
+        <v>657</v>
+      </c>
       <c r="F148" s="50" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="H148" s="64"/>
       <c r="I148" s="62"/>
@@ -17484,24 +17491,40 @@
     </row>
     <row r="149" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B149" s="49" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="D149" t="s">
         <v>345</v>
       </c>
-      <c r="E149" s="49" t="s">
-        <v>1528</v>
-      </c>
+      <c r="E149" s="49"/>
       <c r="F149" s="50" t="s">
-        <v>1692</v>
-      </c>
-      <c r="G149" s="49" t="s">
-        <v>1528</v>
+        <v>1690</v>
       </c>
       <c r="H149" s="64"/>
       <c r="I149" s="62"/>
       <c r="J149" s="62"/>
       <c r="K149" s="62"/>
+    </row>
+    <row r="150" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B150" s="49" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D150" t="s">
+        <v>345</v>
+      </c>
+      <c r="E150" s="49" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F150" s="50" t="s">
+        <v>1692</v>
+      </c>
+      <c r="G150" s="49" t="s">
+        <v>1528</v>
+      </c>
+      <c r="H150" s="64"/>
+      <c r="I150" s="62"/>
+      <c r="J150" s="62"/>
+      <c r="K150" s="62"/>
     </row>
   </sheetData>
   <dataConsolidate link="1"/>
@@ -17509,114 +17532,114 @@
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H27:K27"/>
     <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H37:K37"/>
     <mergeCell ref="H44:K44"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H47:K47"/>
     <mergeCell ref="H50:K50"/>
     <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H52:K52"/>
     <mergeCell ref="H38:K38"/>
     <mergeCell ref="H39:K39"/>
     <mergeCell ref="H40:K40"/>
     <mergeCell ref="H41:K41"/>
     <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="H43:K43"/>
     <mergeCell ref="H61:K61"/>
     <mergeCell ref="H62:K62"/>
     <mergeCell ref="H63:K63"/>
     <mergeCell ref="H64:K64"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="H67:K67"/>
     <mergeCell ref="H53:K53"/>
     <mergeCell ref="H54:K54"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H57:K57"/>
     <mergeCell ref="H59:K59"/>
-    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H60:K60"/>
     <mergeCell ref="H76:K76"/>
     <mergeCell ref="H77:K77"/>
     <mergeCell ref="H78:K78"/>
     <mergeCell ref="H79:K79"/>
     <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H67:K67"/>
+    <mergeCell ref="H81:K81"/>
     <mergeCell ref="H68:K68"/>
-    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H69:K69"/>
     <mergeCell ref="H71:K71"/>
-    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="H72:K72"/>
     <mergeCell ref="H74:K74"/>
-    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H75:K75"/>
     <mergeCell ref="H88:K88"/>
     <mergeCell ref="H89:K89"/>
     <mergeCell ref="H90:K90"/>
     <mergeCell ref="H91:K91"/>
     <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H93:K93"/>
     <mergeCell ref="H82:K82"/>
     <mergeCell ref="H83:K83"/>
     <mergeCell ref="H84:K84"/>
     <mergeCell ref="H85:K85"/>
     <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H87:K87"/>
     <mergeCell ref="H100:K100"/>
     <mergeCell ref="H101:K101"/>
     <mergeCell ref="H102:K102"/>
     <mergeCell ref="H103:K103"/>
     <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H105:K105"/>
     <mergeCell ref="H94:K94"/>
     <mergeCell ref="H95:K95"/>
     <mergeCell ref="H96:K96"/>
     <mergeCell ref="H97:K97"/>
     <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H99:K99"/>
     <mergeCell ref="H112:K112"/>
     <mergeCell ref="H113:K113"/>
     <mergeCell ref="H114:K114"/>
     <mergeCell ref="H115:K115"/>
     <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="H117:K117"/>
     <mergeCell ref="H106:K106"/>
     <mergeCell ref="H107:K107"/>
     <mergeCell ref="H108:K108"/>
     <mergeCell ref="H109:K109"/>
     <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H111:K111"/>
     <mergeCell ref="H124:K124"/>
     <mergeCell ref="H125:K125"/>
     <mergeCell ref="H126:K126"/>
     <mergeCell ref="H127:K127"/>
     <mergeCell ref="H128:K128"/>
-    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H129:K129"/>
     <mergeCell ref="H118:K118"/>
     <mergeCell ref="H119:K119"/>
     <mergeCell ref="H120:K120"/>
     <mergeCell ref="H121:K121"/>
     <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="H123:K123"/>
     <mergeCell ref="H136:K136"/>
     <mergeCell ref="H137:K137"/>
     <mergeCell ref="H138:K138"/>
     <mergeCell ref="H139:K139"/>
     <mergeCell ref="H140:K140"/>
-    <mergeCell ref="H129:K129"/>
+    <mergeCell ref="H141:K141"/>
     <mergeCell ref="H130:K130"/>
     <mergeCell ref="H131:K131"/>
     <mergeCell ref="H132:K132"/>
     <mergeCell ref="H133:K133"/>
     <mergeCell ref="H134:K134"/>
-    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H135:K135"/>
     <mergeCell ref="H148:K148"/>
     <mergeCell ref="H149:K149"/>
-    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="H150:K150"/>
     <mergeCell ref="H142:K142"/>
     <mergeCell ref="H143:K143"/>
     <mergeCell ref="H144:K144"/>
     <mergeCell ref="H145:K145"/>
     <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26043,8 +26066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63947D01-B4BD-4B2C-8904-F72EDA2AD99B}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28005,17 +28028,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -28024,7 +28036,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -28253,24 +28265,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -28278,7 +28284,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28295,4 +28301,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:sparkles: Extend echo-parameters code system with new ones and add heartRate slice to HFR_Electrocardiograph profile
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\db\dt4h\common-data-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77D0F0B-62E2-4566-B13A-664051366095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66366D1F-6ED6-4A63-884D-F80720BB7256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" tabRatio="901" firstSheet="11" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="901" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -860,7 +860,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4335" uniqueCount="1955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="1957">
   <si>
     <t>Required</t>
   </si>
@@ -6745,6 +6745,12 @@
   </si>
   <si>
     <t>dyn·sec/cm5</t>
+  </si>
+  <si>
+    <t>RADi</t>
+  </si>
+  <si>
+    <t>RAAi</t>
   </si>
 </sst>
 </file>
@@ -6996,7 +7002,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -7102,14 +7108,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7117,12 +7126,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -8500,6 +8503,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -8510,13 +8520,6 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9216,7 +9219,7 @@
         <v>462</v>
       </c>
       <c r="D39" s="63"/>
-      <c r="E39" s="65"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="68" t="s">
         <v>463</v>
       </c>
@@ -9231,11 +9234,11 @@
       <c r="B40" s="42" t="s">
         <v>465</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="65" t="s">
         <v>466</v>
       </c>
-      <c r="D40" s="66"/>
-      <c r="E40" s="67"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="66"/>
       <c r="F40" s="64"/>
       <c r="G40" s="62"/>
       <c r="H40" s="62"/>
@@ -9248,11 +9251,11 @@
       <c r="B41" s="42" t="s">
         <v>468</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="65" t="s">
         <v>469</v>
       </c>
-      <c r="D41" s="66"/>
-      <c r="E41" s="67"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="66"/>
       <c r="F41" s="64"/>
       <c r="G41" s="62"/>
       <c r="H41" s="62"/>
@@ -9265,11 +9268,11 @@
       <c r="B42" s="42" t="s">
         <v>471</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="65" t="s">
         <v>472</v>
       </c>
-      <c r="D42" s="66"/>
-      <c r="E42" s="67"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="66"/>
       <c r="F42" s="64"/>
       <c r="G42" s="62"/>
       <c r="H42" s="62"/>
@@ -9282,11 +9285,11 @@
       <c r="B43" s="42" t="s">
         <v>474</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="65" t="s">
         <v>1297</v>
       </c>
-      <c r="D43" s="66"/>
-      <c r="E43" s="67"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="66"/>
       <c r="F43" s="64"/>
       <c r="G43" s="62"/>
       <c r="H43" s="62"/>
@@ -9299,11 +9302,11 @@
       <c r="B44" s="42" t="s">
         <v>476</v>
       </c>
-      <c r="C44" s="66" t="s">
+      <c r="C44" s="65" t="s">
         <v>477</v>
       </c>
-      <c r="D44" s="66"/>
-      <c r="E44" s="67"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="66"/>
       <c r="F44" s="64"/>
       <c r="G44" s="62"/>
       <c r="H44" s="62"/>
@@ -9316,11 +9319,11 @@
       <c r="B45" s="42" t="s">
         <v>479</v>
       </c>
-      <c r="C45" s="66" t="s">
+      <c r="C45" s="65" t="s">
         <v>480</v>
       </c>
-      <c r="D45" s="66"/>
-      <c r="E45" s="67"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="66"/>
       <c r="F45" s="64"/>
       <c r="G45" s="62"/>
       <c r="H45" s="62"/>
@@ -9333,11 +9336,11 @@
       <c r="B46" s="42" t="s">
         <v>482</v>
       </c>
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="65" t="s">
         <v>483</v>
       </c>
-      <c r="D46" s="66"/>
-      <c r="E46" s="67"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="66"/>
       <c r="F46" s="64"/>
       <c r="G46" s="62"/>
       <c r="H46" s="62"/>
@@ -9350,11 +9353,11 @@
       <c r="B47" s="42" t="s">
         <v>485</v>
       </c>
-      <c r="C47" s="66" t="s">
+      <c r="C47" s="65" t="s">
         <v>486</v>
       </c>
-      <c r="D47" s="66"/>
-      <c r="E47" s="67"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="66"/>
       <c r="F47" s="64"/>
       <c r="G47" s="62"/>
       <c r="H47" s="62"/>
@@ -9367,11 +9370,11 @@
       <c r="B48" s="42" t="s">
         <v>488</v>
       </c>
-      <c r="C48" s="66" t="s">
+      <c r="C48" s="65" t="s">
         <v>489</v>
       </c>
-      <c r="D48" s="66"/>
-      <c r="E48" s="67"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="66"/>
       <c r="F48" s="64"/>
       <c r="G48" s="62"/>
       <c r="H48" s="62"/>
@@ -9384,11 +9387,11 @@
       <c r="B49" s="42" t="s">
         <v>491</v>
       </c>
-      <c r="C49" s="66" t="s">
+      <c r="C49" s="65" t="s">
         <v>492</v>
       </c>
-      <c r="D49" s="66"/>
-      <c r="E49" s="67"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="66"/>
       <c r="F49" s="64"/>
       <c r="G49" s="62"/>
       <c r="H49" s="62"/>
@@ -9401,11 +9404,11 @@
       <c r="B50" s="42" t="s">
         <v>494</v>
       </c>
-      <c r="C50" s="66" t="s">
+      <c r="C50" s="65" t="s">
         <v>495</v>
       </c>
-      <c r="D50" s="66"/>
-      <c r="E50" s="67"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="66"/>
       <c r="F50" s="64"/>
       <c r="G50" s="62"/>
       <c r="H50" s="62"/>
@@ -9418,11 +9421,11 @@
       <c r="B51" s="42" t="s">
         <v>497</v>
       </c>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="65" t="s">
         <v>498</v>
       </c>
-      <c r="D51" s="66"/>
-      <c r="E51" s="67"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="66"/>
       <c r="F51" s="64"/>
       <c r="G51" s="62"/>
       <c r="H51" s="62"/>
@@ -9435,11 +9438,11 @@
       <c r="B52" s="42" t="s">
         <v>500</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="65" t="s">
         <v>501</v>
       </c>
-      <c r="D52" s="66"/>
-      <c r="E52" s="67"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="66"/>
       <c r="F52" s="64"/>
       <c r="G52" s="62"/>
       <c r="H52" s="62"/>
@@ -9452,11 +9455,11 @@
       <c r="B53" s="42" t="s">
         <v>503</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C53" s="65" t="s">
         <v>504</v>
       </c>
-      <c r="D53" s="66"/>
-      <c r="E53" s="67"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="66"/>
       <c r="F53" s="64"/>
       <c r="G53" s="62"/>
       <c r="H53" s="62"/>
@@ -9469,11 +9472,11 @@
       <c r="B54" s="42" t="s">
         <v>506</v>
       </c>
-      <c r="C54" s="66" t="s">
+      <c r="C54" s="65" t="s">
         <v>507</v>
       </c>
-      <c r="D54" s="66"/>
-      <c r="E54" s="67"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="66"/>
       <c r="F54" s="64"/>
       <c r="G54" s="62"/>
       <c r="H54" s="62"/>
@@ -9486,11 +9489,11 @@
       <c r="B55" s="42" t="s">
         <v>509</v>
       </c>
-      <c r="C55" s="66" t="s">
+      <c r="C55" s="65" t="s">
         <v>510</v>
       </c>
-      <c r="D55" s="66"/>
-      <c r="E55" s="67"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="66"/>
       <c r="F55" s="64"/>
       <c r="G55" s="62"/>
       <c r="H55" s="62"/>
@@ -9503,11 +9506,11 @@
       <c r="B56" s="42" t="s">
         <v>512</v>
       </c>
-      <c r="C56" s="66" t="s">
+      <c r="C56" s="65" t="s">
         <v>513</v>
       </c>
-      <c r="D56" s="66"/>
-      <c r="E56" s="67"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="66"/>
       <c r="F56" s="64"/>
       <c r="G56" s="62"/>
       <c r="H56" s="62"/>
@@ -9520,11 +9523,11 @@
       <c r="B57" s="42" t="s">
         <v>515</v>
       </c>
-      <c r="C57" s="66" t="s">
+      <c r="C57" s="65" t="s">
         <v>516</v>
       </c>
-      <c r="D57" s="66"/>
-      <c r="E57" s="67"/>
+      <c r="D57" s="65"/>
+      <c r="E57" s="66"/>
       <c r="F57" s="64"/>
       <c r="G57" s="62"/>
       <c r="H57" s="62"/>
@@ -9537,11 +9540,11 @@
       <c r="B58" s="42" t="s">
         <v>518</v>
       </c>
-      <c r="C58" s="66" t="s">
+      <c r="C58" s="65" t="s">
         <v>519</v>
       </c>
-      <c r="D58" s="66"/>
-      <c r="E58" s="67"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="66"/>
       <c r="F58" s="64"/>
       <c r="G58" s="62"/>
       <c r="H58" s="62"/>
@@ -9554,11 +9557,11 @@
       <c r="B59" s="42" t="s">
         <v>521</v>
       </c>
-      <c r="C59" s="66" t="s">
+      <c r="C59" s="65" t="s">
         <v>522</v>
       </c>
-      <c r="D59" s="66"/>
-      <c r="E59" s="67"/>
+      <c r="D59" s="65"/>
+      <c r="E59" s="66"/>
       <c r="F59" s="64"/>
       <c r="G59" s="62"/>
       <c r="H59" s="62"/>
@@ -9571,11 +9574,11 @@
       <c r="B60" s="42" t="s">
         <v>524</v>
       </c>
-      <c r="C60" s="66" t="s">
+      <c r="C60" s="65" t="s">
         <v>525</v>
       </c>
-      <c r="D60" s="66"/>
-      <c r="E60" s="67"/>
+      <c r="D60" s="65"/>
+      <c r="E60" s="66"/>
       <c r="F60" s="64"/>
       <c r="G60" s="62"/>
       <c r="H60" s="62"/>
@@ -9588,11 +9591,11 @@
       <c r="B61" s="42" t="s">
         <v>527</v>
       </c>
-      <c r="C61" s="66" t="s">
+      <c r="C61" s="65" t="s">
         <v>528</v>
       </c>
-      <c r="D61" s="66"/>
-      <c r="E61" s="67"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="66"/>
       <c r="F61" s="64"/>
       <c r="G61" s="62"/>
       <c r="H61" s="62"/>
@@ -9605,11 +9608,11 @@
       <c r="B62" s="42" t="s">
         <v>530</v>
       </c>
-      <c r="C62" s="66" t="s">
+      <c r="C62" s="65" t="s">
         <v>531</v>
       </c>
-      <c r="D62" s="66"/>
-      <c r="E62" s="67"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="66"/>
       <c r="F62" s="64"/>
       <c r="G62" s="62"/>
       <c r="H62" s="62"/>
@@ -9622,11 +9625,11 @@
       <c r="B63" s="42" t="s">
         <v>533</v>
       </c>
-      <c r="C63" s="66" t="s">
+      <c r="C63" s="65" t="s">
         <v>534</v>
       </c>
-      <c r="D63" s="66"/>
-      <c r="E63" s="67"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="66"/>
       <c r="F63" s="64"/>
       <c r="G63" s="62"/>
       <c r="H63" s="62"/>
@@ -9639,11 +9642,11 @@
       <c r="B64" s="42" t="s">
         <v>535</v>
       </c>
-      <c r="C64" s="66" t="s">
+      <c r="C64" s="65" t="s">
         <v>536</v>
       </c>
-      <c r="D64" s="66"/>
-      <c r="E64" s="67"/>
+      <c r="D64" s="65"/>
+      <c r="E64" s="66"/>
       <c r="F64" s="64"/>
       <c r="G64" s="62"/>
       <c r="H64" s="62"/>
@@ -9656,11 +9659,11 @@
       <c r="B65" s="42" t="s">
         <v>538</v>
       </c>
-      <c r="C65" s="66" t="s">
+      <c r="C65" s="65" t="s">
         <v>539</v>
       </c>
-      <c r="D65" s="66"/>
-      <c r="E65" s="67"/>
+      <c r="D65" s="65"/>
+      <c r="E65" s="66"/>
       <c r="F65" s="64"/>
       <c r="G65" s="62"/>
       <c r="H65" s="62"/>
@@ -9673,11 +9676,11 @@
       <c r="B66" s="42" t="s">
         <v>541</v>
       </c>
-      <c r="C66" s="66" t="s">
+      <c r="C66" s="65" t="s">
         <v>542</v>
       </c>
-      <c r="D66" s="66"/>
-      <c r="E66" s="67"/>
+      <c r="D66" s="65"/>
+      <c r="E66" s="66"/>
       <c r="F66" s="64"/>
       <c r="G66" s="62"/>
       <c r="H66" s="62"/>
@@ -9690,11 +9693,11 @@
       <c r="B67" s="42" t="s">
         <v>544</v>
       </c>
-      <c r="C67" s="66" t="s">
+      <c r="C67" s="65" t="s">
         <v>545</v>
       </c>
-      <c r="D67" s="66"/>
-      <c r="E67" s="67"/>
+      <c r="D67" s="65"/>
+      <c r="E67" s="66"/>
       <c r="F67" s="64"/>
       <c r="G67" s="62"/>
       <c r="H67" s="62"/>
@@ -9707,11 +9710,11 @@
       <c r="B68" s="42" t="s">
         <v>547</v>
       </c>
-      <c r="C68" s="66" t="s">
+      <c r="C68" s="65" t="s">
         <v>548</v>
       </c>
-      <c r="D68" s="66"/>
-      <c r="E68" s="67"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="66"/>
       <c r="F68" s="64"/>
       <c r="G68" s="62"/>
       <c r="H68" s="62"/>
@@ -9724,11 +9727,11 @@
       <c r="B69" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="C69" s="66" t="s">
+      <c r="C69" s="65" t="s">
         <v>551</v>
       </c>
-      <c r="D69" s="66"/>
-      <c r="E69" s="67"/>
+      <c r="D69" s="65"/>
+      <c r="E69" s="66"/>
       <c r="F69" s="64"/>
       <c r="G69" s="62"/>
       <c r="H69" s="62"/>
@@ -9741,11 +9744,11 @@
       <c r="B70" s="42" t="s">
         <v>553</v>
       </c>
-      <c r="C70" s="66" t="s">
+      <c r="C70" s="65" t="s">
         <v>554</v>
       </c>
-      <c r="D70" s="66"/>
-      <c r="E70" s="67"/>
+      <c r="D70" s="65"/>
+      <c r="E70" s="66"/>
       <c r="F70" s="64"/>
       <c r="G70" s="62"/>
       <c r="H70" s="62"/>
@@ -9758,11 +9761,11 @@
       <c r="B71" s="42" t="s">
         <v>556</v>
       </c>
-      <c r="C71" s="66" t="s">
+      <c r="C71" s="65" t="s">
         <v>557</v>
       </c>
-      <c r="D71" s="66"/>
-      <c r="E71" s="67"/>
+      <c r="D71" s="65"/>
+      <c r="E71" s="66"/>
       <c r="F71" s="64"/>
       <c r="G71" s="62"/>
       <c r="H71" s="62"/>
@@ -9775,11 +9778,11 @@
       <c r="B72" s="42" t="s">
         <v>559</v>
       </c>
-      <c r="C72" s="66" t="s">
+      <c r="C72" s="65" t="s">
         <v>560</v>
       </c>
-      <c r="D72" s="66"/>
-      <c r="E72" s="67"/>
+      <c r="D72" s="65"/>
+      <c r="E72" s="66"/>
       <c r="F72" s="64"/>
       <c r="G72" s="62"/>
       <c r="H72" s="62"/>
@@ -9792,11 +9795,11 @@
       <c r="B73" s="42" t="s">
         <v>562</v>
       </c>
-      <c r="C73" s="66" t="s">
+      <c r="C73" s="65" t="s">
         <v>563</v>
       </c>
-      <c r="D73" s="66"/>
-      <c r="E73" s="67"/>
+      <c r="D73" s="65"/>
+      <c r="E73" s="66"/>
       <c r="F73" s="64"/>
       <c r="G73" s="62"/>
       <c r="H73" s="62"/>
@@ -9809,11 +9812,11 @@
       <c r="B74" s="42" t="s">
         <v>565</v>
       </c>
-      <c r="C74" s="66" t="s">
+      <c r="C74" s="65" t="s">
         <v>566</v>
       </c>
-      <c r="D74" s="66"/>
-      <c r="E74" s="67"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="66"/>
       <c r="F74" s="64"/>
       <c r="G74" s="62"/>
       <c r="H74" s="62"/>
@@ -9826,11 +9829,11 @@
       <c r="B75" s="42" t="s">
         <v>568</v>
       </c>
-      <c r="C75" s="66" t="s">
+      <c r="C75" s="65" t="s">
         <v>569</v>
       </c>
-      <c r="D75" s="66"/>
-      <c r="E75" s="67"/>
+      <c r="D75" s="65"/>
+      <c r="E75" s="66"/>
       <c r="F75" s="64"/>
       <c r="G75" s="62"/>
       <c r="H75" s="62"/>
@@ -9843,11 +9846,11 @@
       <c r="B76" s="42" t="s">
         <v>571</v>
       </c>
-      <c r="C76" s="66" t="s">
+      <c r="C76" s="65" t="s">
         <v>572</v>
       </c>
-      <c r="D76" s="66"/>
-      <c r="E76" s="67"/>
+      <c r="D76" s="65"/>
+      <c r="E76" s="66"/>
       <c r="F76" s="64"/>
       <c r="G76" s="62"/>
       <c r="H76" s="62"/>
@@ -9860,11 +9863,11 @@
       <c r="B77" s="42" t="s">
         <v>574</v>
       </c>
-      <c r="C77" s="66" t="s">
+      <c r="C77" s="65" t="s">
         <v>575</v>
       </c>
-      <c r="D77" s="66"/>
-      <c r="E77" s="67"/>
+      <c r="D77" s="65"/>
+      <c r="E77" s="66"/>
       <c r="F77" s="64"/>
       <c r="G77" s="62"/>
       <c r="H77" s="62"/>
@@ -9877,11 +9880,11 @@
       <c r="B78" s="42" t="s">
         <v>577</v>
       </c>
-      <c r="C78" s="66" t="s">
+      <c r="C78" s="65" t="s">
         <v>578</v>
       </c>
-      <c r="D78" s="66"/>
-      <c r="E78" s="67"/>
+      <c r="D78" s="65"/>
+      <c r="E78" s="66"/>
       <c r="F78" s="64"/>
       <c r="G78" s="62"/>
       <c r="H78" s="62"/>
@@ -9894,11 +9897,11 @@
       <c r="B79" s="42" t="s">
         <v>580</v>
       </c>
-      <c r="C79" s="66" t="s">
+      <c r="C79" s="65" t="s">
         <v>581</v>
       </c>
-      <c r="D79" s="66"/>
-      <c r="E79" s="67"/>
+      <c r="D79" s="65"/>
+      <c r="E79" s="66"/>
       <c r="F79" s="64"/>
       <c r="G79" s="62"/>
       <c r="H79" s="62"/>
@@ -9911,11 +9914,11 @@
       <c r="B80" s="42" t="s">
         <v>583</v>
       </c>
-      <c r="C80" s="66" t="s">
+      <c r="C80" s="65" t="s">
         <v>584</v>
       </c>
-      <c r="D80" s="66"/>
-      <c r="E80" s="67"/>
+      <c r="D80" s="65"/>
+      <c r="E80" s="66"/>
       <c r="F80" s="64"/>
       <c r="G80" s="62"/>
       <c r="H80" s="62"/>
@@ -9928,11 +9931,11 @@
       <c r="B81" s="42" t="s">
         <v>586</v>
       </c>
-      <c r="C81" s="66" t="s">
+      <c r="C81" s="65" t="s">
         <v>587</v>
       </c>
-      <c r="D81" s="66"/>
-      <c r="E81" s="67"/>
+      <c r="D81" s="65"/>
+      <c r="E81" s="66"/>
       <c r="F81" s="64"/>
       <c r="G81" s="62"/>
       <c r="H81" s="62"/>
@@ -9940,36 +9943,69 @@
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="F48:I48"/>
     <mergeCell ref="F49:I49"/>
@@ -9994,69 +10030,36 @@
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="F55:I55"/>
     <mergeCell ref="F56:I56"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10920,14 +10923,41 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -10944,41 +10974,14 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -12136,7 +12139,7 @@
       <c r="I34" s="62"/>
       <c r="J34" s="62"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A35" s="49" t="s">
         <v>1784</v>
       </c>
@@ -12190,29 +12193,19 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
     <mergeCell ref="G32:J32"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
@@ -12225,19 +12218,29 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="G31:J31"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:F21" xr:uid="{7FAB08B6-9907-44B4-A82A-4A3E200D36A8}">
@@ -13549,25 +13552,23 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F30:I30"/>
     <mergeCell ref="F55:I55"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="F35:I35"/>
@@ -13581,23 +13582,25 @@
     <mergeCell ref="F49:I49"/>
     <mergeCell ref="F50:I50"/>
     <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F61:I61"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -15166,8 +15169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF00AD05-AD0A-4301-B0FD-56AA1951174D}">
   <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17094,6 +17097,9 @@
       <c r="B95" t="s">
         <v>1567</v>
       </c>
+      <c r="C95" t="s">
+        <v>1955</v>
+      </c>
       <c r="D95" t="s">
         <v>1444</v>
       </c>
@@ -17255,6 +17261,9 @@
       </c>
       <c r="B103" t="s">
         <v>1588</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1956</v>
       </c>
       <c r="D103" t="s">
         <v>345</v>
@@ -18128,24 +18137,87 @@
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="111">
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H149:K149"/>
+    <mergeCell ref="H150:K150"/>
+    <mergeCell ref="H151:K151"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="H138:K138"/>
+    <mergeCell ref="H139:K139"/>
+    <mergeCell ref="H140:K140"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H131:K131"/>
+    <mergeCell ref="H132:K132"/>
+    <mergeCell ref="H133:K133"/>
+    <mergeCell ref="H134:K134"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="H136:K136"/>
+    <mergeCell ref="H125:K125"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="H128:K128"/>
+    <mergeCell ref="H129:K129"/>
+    <mergeCell ref="H130:K130"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="H121:K121"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="H106:K106"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H68:K68"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="H71:K71"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="H75:K75"/>
     <mergeCell ref="H61:K61"/>
     <mergeCell ref="H62:K62"/>
     <mergeCell ref="H63:K63"/>
@@ -18158,87 +18230,24 @@
     <mergeCell ref="H57:K57"/>
     <mergeCell ref="H59:K59"/>
     <mergeCell ref="H60:K60"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H68:K68"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="H71:K71"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H106:K106"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="H128:K128"/>
-    <mergeCell ref="H129:K129"/>
-    <mergeCell ref="H130:K130"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="H138:K138"/>
-    <mergeCell ref="H139:K139"/>
-    <mergeCell ref="H140:K140"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H131:K131"/>
-    <mergeCell ref="H132:K132"/>
-    <mergeCell ref="H133:K133"/>
-    <mergeCell ref="H134:K134"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="H136:K136"/>
-    <mergeCell ref="H149:K149"/>
-    <mergeCell ref="H150:K150"/>
-    <mergeCell ref="H151:K151"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H47:K47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20923,13 +20932,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F118:I118"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="F114:I114"/>
+    <mergeCell ref="F115:I115"/>
+    <mergeCell ref="F116:I116"/>
+    <mergeCell ref="F117:I117"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
     <mergeCell ref="C131:D131"/>
     <mergeCell ref="C124:D124"/>
     <mergeCell ref="C125:D125"/>
@@ -20938,14 +20948,13 @@
     <mergeCell ref="C128:D128"/>
     <mergeCell ref="C129:D129"/>
     <mergeCell ref="C130:D130"/>
-    <mergeCell ref="F114:I114"/>
-    <mergeCell ref="F115:I115"/>
-    <mergeCell ref="F116:I116"/>
-    <mergeCell ref="F117:I117"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="F118:I118"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -20978,9 +20987,9 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C8D262-C29E-46BC-91E9-5E2FD0F3F367}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -21640,344 +21649,122 @@
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F32" s="75"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-    </row>
-    <row r="33" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F33" s="75"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="73"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="73"/>
-    </row>
-    <row r="34" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F34" s="75"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-    </row>
-    <row r="35" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F35" s="75"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-    </row>
-    <row r="36" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F36" s="75"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-    </row>
-    <row r="37" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F37" s="75"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-    </row>
-    <row r="38" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F38" s="75"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-    </row>
-    <row r="39" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F39" s="75"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="74"/>
-      <c r="K39" s="74"/>
-    </row>
-    <row r="40" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F40" s="75"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="74"/>
-      <c r="K40" s="74"/>
-    </row>
-    <row r="41" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F41" s="75"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="74"/>
-    </row>
-    <row r="42" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F42" s="75"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="74"/>
-    </row>
-    <row r="43" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F43" s="75"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="74"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="74"/>
-    </row>
-    <row r="44" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F44" s="75"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
-      <c r="J44" s="74"/>
-      <c r="K44" s="74"/>
-    </row>
-    <row r="45" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F45" s="75"/>
-      <c r="G45" s="73"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-    </row>
-    <row r="46" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F46" s="75"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="73"/>
-    </row>
-    <row r="47" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F47" s="75"/>
-      <c r="G47" s="73"/>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="74"/>
-      <c r="K47" s="74"/>
-    </row>
-    <row r="48" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F48" s="75"/>
-      <c r="G48" s="73"/>
-      <c r="H48" s="73"/>
-      <c r="I48" s="73"/>
-      <c r="J48" s="73"/>
-      <c r="K48" s="73"/>
-    </row>
-    <row r="49" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F49" s="75"/>
-      <c r="G49" s="73"/>
-      <c r="H49" s="73"/>
-      <c r="I49" s="73"/>
-      <c r="J49" s="73"/>
-      <c r="K49" s="73"/>
-    </row>
-    <row r="50" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F50" s="75"/>
-      <c r="G50" s="73"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
-    </row>
-    <row r="51" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F51" s="75"/>
-      <c r="G51" s="73"/>
-      <c r="H51" s="74"/>
-      <c r="I51" s="74"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="74"/>
-    </row>
-    <row r="52" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F52" s="75"/>
-      <c r="G52" s="73"/>
-      <c r="H52" s="74"/>
-      <c r="I52" s="74"/>
-      <c r="J52" s="74"/>
-      <c r="K52" s="74"/>
-    </row>
-    <row r="53" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F53" s="75"/>
-      <c r="G53" s="73"/>
-      <c r="H53" s="74"/>
-      <c r="I53" s="74"/>
-      <c r="J53" s="74"/>
-      <c r="K53" s="74"/>
-    </row>
-    <row r="54" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F54" s="75"/>
-      <c r="G54" s="73"/>
-      <c r="H54" s="74"/>
-      <c r="I54" s="74"/>
-      <c r="J54" s="74"/>
-      <c r="K54" s="74"/>
-    </row>
-    <row r="55" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F55" s="75"/>
-      <c r="G55" s="73"/>
-      <c r="H55" s="74"/>
-      <c r="I55" s="74"/>
-      <c r="J55" s="74"/>
-      <c r="K55" s="74"/>
-    </row>
-    <row r="56" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F56" s="75"/>
-      <c r="G56" s="73"/>
-      <c r="H56" s="73"/>
-      <c r="I56" s="73"/>
-      <c r="J56" s="73"/>
-      <c r="K56" s="73"/>
-    </row>
-    <row r="57" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F57" s="75"/>
-      <c r="G57" s="73"/>
-      <c r="H57" s="73"/>
-      <c r="I57" s="73"/>
-      <c r="J57" s="73"/>
-      <c r="K57" s="73"/>
-    </row>
-    <row r="58" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F58" s="75"/>
-      <c r="G58" s="73"/>
-      <c r="H58" s="73"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="73"/>
-    </row>
-    <row r="59" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F59" s="75"/>
-      <c r="G59" s="73"/>
-      <c r="H59" s="73"/>
-      <c r="I59" s="73"/>
-      <c r="J59" s="73"/>
-      <c r="K59" s="73"/>
-    </row>
-    <row r="60" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F60" s="75"/>
-      <c r="G60" s="73"/>
-      <c r="H60" s="73"/>
-      <c r="I60" s="73"/>
-      <c r="J60" s="73"/>
-      <c r="K60" s="73"/>
-    </row>
-    <row r="61" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F61" s="75"/>
-      <c r="G61" s="73"/>
-      <c r="H61" s="73"/>
-      <c r="I61" s="73"/>
-      <c r="J61" s="73"/>
-      <c r="K61" s="73"/>
-    </row>
-    <row r="62" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F62" s="75"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="73"/>
-      <c r="I62" s="73"/>
-      <c r="J62" s="73"/>
-      <c r="K62" s="73"/>
-    </row>
-    <row r="63" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F63" s="75"/>
-      <c r="G63" s="73"/>
-      <c r="H63" s="73"/>
-      <c r="I63" s="73"/>
-      <c r="J63" s="73"/>
-      <c r="K63" s="73"/>
-    </row>
-    <row r="64" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F64" s="75"/>
-      <c r="G64" s="73"/>
-      <c r="H64" s="73"/>
-      <c r="I64" s="73"/>
-      <c r="J64" s="73"/>
-      <c r="K64" s="73"/>
-    </row>
-    <row r="65" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F65" s="75"/>
-      <c r="G65" s="73"/>
-      <c r="H65" s="73"/>
-      <c r="I65" s="73"/>
-      <c r="J65" s="73"/>
-      <c r="K65" s="73"/>
-    </row>
-    <row r="66" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F66" s="75"/>
-      <c r="G66" s="73"/>
-      <c r="H66" s="73"/>
-      <c r="I66" s="73"/>
-      <c r="J66" s="73"/>
-      <c r="K66" s="73"/>
-    </row>
-    <row r="67" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F67" s="75"/>
-      <c r="G67" s="73"/>
-      <c r="H67" s="73"/>
-      <c r="I67" s="73"/>
-      <c r="J67" s="73"/>
-      <c r="K67" s="73"/>
-    </row>
-    <row r="68" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F68" s="75"/>
-      <c r="G68" s="73"/>
-      <c r="H68" s="73"/>
-      <c r="I68" s="73"/>
-      <c r="J68" s="73"/>
-      <c r="K68" s="73"/>
-    </row>
-    <row r="69" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F69" s="75"/>
-      <c r="G69" s="73"/>
-      <c r="H69" s="73"/>
-      <c r="I69" s="73"/>
-      <c r="J69" s="73"/>
-      <c r="K69" s="73"/>
-    </row>
-    <row r="70" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F70" s="75"/>
-      <c r="G70" s="73"/>
-      <c r="H70" s="73"/>
-      <c r="I70" s="73"/>
-      <c r="J70" s="73"/>
-      <c r="K70" s="73"/>
-    </row>
-    <row r="71" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F71" s="75"/>
-      <c r="G71" s="73"/>
-      <c r="H71" s="73"/>
-      <c r="I71" s="73"/>
-      <c r="J71" s="73"/>
-      <c r="K71" s="73"/>
-    </row>
-    <row r="72" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F72" s="75"/>
-      <c r="G72" s="73"/>
-      <c r="H72" s="73"/>
-      <c r="I72" s="73"/>
-      <c r="J72" s="73"/>
-      <c r="K72" s="73"/>
-    </row>
-    <row r="73" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F73" s="75"/>
-      <c r="G73" s="73"/>
-      <c r="H73" s="73"/>
-      <c r="I73" s="73"/>
-      <c r="J73" s="73"/>
-      <c r="K73" s="73"/>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="61"/>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+    </row>
+    <row r="40" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H40" s="61"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="61"/>
+    </row>
+    <row r="41" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+    </row>
+    <row r="42" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="61"/>
+      <c r="K42" s="61"/>
+    </row>
+    <row r="43" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+    </row>
+    <row r="44" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+    </row>
+    <row r="45" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+    </row>
+    <row r="47" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+    </row>
+    <row r="50" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+    </row>
+    <row r="51" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H51" s="61"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="61"/>
+    </row>
+    <row r="52" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H52" s="61"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="61"/>
+      <c r="K52" s="61"/>
+    </row>
+    <row r="53" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H53" s="61"/>
+      <c r="I53" s="61"/>
+      <c r="J53" s="61"/>
+      <c r="K53" s="61"/>
+    </row>
+    <row r="54" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H54" s="61"/>
+      <c r="I54" s="61"/>
+      <c r="J54" s="61"/>
+      <c r="K54" s="61"/>
+    </row>
+    <row r="55" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H55" s="61"/>
+      <c r="I55" s="61"/>
+      <c r="J55" s="61"/>
+      <c r="K55" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
     <mergeCell ref="H53:K53"/>
     <mergeCell ref="H54:K54"/>
     <mergeCell ref="H55:K55"/>
@@ -21987,18 +21774,6 @@
     <mergeCell ref="H50:K50"/>
     <mergeCell ref="H51:K51"/>
     <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24152,49 +23927,108 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="C80:D80"/>
@@ -24219,108 +24053,49 @@
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24866,7 +24641,7 @@
         <v>1041</v>
       </c>
       <c r="D14" s="63"/>
-      <c r="E14" s="65"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="68" t="s">
         <v>463</v>
       </c>
@@ -24875,201 +24650,201 @@
       <c r="I14" s="68"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="71" t="s">
         <v>1042</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1043</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="65" t="s">
         <v>1044</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="67"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
       <c r="F15" s="64"/>
       <c r="G15" s="62"/>
       <c r="H15" s="62"/>
       <c r="I15" s="62"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="70"/>
+      <c r="A16" s="71"/>
       <c r="B16" s="42" t="s">
         <v>1045</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="65" t="s">
         <v>1046</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="67"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
       <c r="F16" s="64"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="70"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="42" t="s">
         <v>1047</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="65" t="s">
         <v>1048</v>
       </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="67"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
       <c r="F17" s="64"/>
       <c r="G17" s="62"/>
       <c r="H17" s="62"/>
       <c r="I17" s="62"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="70"/>
+      <c r="A18" s="71"/>
       <c r="B18" s="42" t="s">
         <v>1049</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="66" t="s">
         <v>1050</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
       <c r="F18" s="64"/>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
       <c r="I18" s="62"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="70"/>
+      <c r="A19" s="71"/>
       <c r="B19" s="42" t="s">
         <v>1051</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="66" t="s">
         <v>1052</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="64"/>
       <c r="G19" s="62"/>
       <c r="H19" s="62"/>
       <c r="I19" s="62"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="72" t="s">
         <v>1053</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1054</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="66" t="s">
         <v>1055</v>
       </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
       <c r="F20" s="64"/>
       <c r="G20" s="62"/>
       <c r="H20" s="62"/>
       <c r="I20" s="62"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="71"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="42" t="s">
         <v>1056</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="66" t="s">
         <v>1057</v>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="64"/>
       <c r="G21" s="62"/>
       <c r="H21" s="62"/>
       <c r="I21" s="62"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="71"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="42" t="s">
         <v>1058</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="66" t="s">
         <v>1059</v>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
       <c r="F22" s="64"/>
       <c r="G22" s="62"/>
       <c r="H22" s="62"/>
       <c r="I22" s="62"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="71"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="42" t="s">
         <v>1060</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="66" t="s">
         <v>1061</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
       <c r="F23" s="64"/>
       <c r="G23" s="62"/>
       <c r="H23" s="62"/>
       <c r="I23" s="62"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="72" t="s">
         <v>1062</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1054</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="66" t="s">
         <v>1063</v>
       </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="64"/>
       <c r="G24" s="62"/>
       <c r="H24" s="62"/>
       <c r="I24" s="62"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="71"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="42" t="s">
         <v>1064</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="66" t="s">
         <v>1065</v>
       </c>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
       <c r="F25" s="64"/>
       <c r="G25" s="62"/>
       <c r="H25" s="62"/>
       <c r="I25" s="62"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="71"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="42" t="s">
         <v>1058</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="66" t="s">
         <v>1066</v>
       </c>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
       <c r="F26" s="64"/>
       <c r="G26" s="62"/>
       <c r="H26" s="62"/>
       <c r="I26" s="62"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="71"/>
+      <c r="A27" s="72"/>
       <c r="B27" s="42" t="s">
         <v>1060</v>
       </c>
-      <c r="C27" s="72" t="s">
+      <c r="C27" s="70" t="s">
         <v>1067</v>
       </c>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
       <c r="F27" s="64"/>
       <c r="G27" s="62"/>
       <c r="H27" s="62"/>
@@ -25082,137 +24857,137 @@
       <c r="B28" s="45" t="s">
         <v>1069</v>
       </c>
-      <c r="C28" s="72" t="s">
+      <c r="C28" s="70" t="s">
         <v>1070</v>
       </c>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
       <c r="F28" s="64"/>
       <c r="G28" s="62"/>
       <c r="H28" s="62"/>
       <c r="I28" s="62"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="72" t="s">
         <v>1071</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1072</v>
       </c>
-      <c r="C29" s="72" t="s">
+      <c r="C29" s="70" t="s">
         <v>1073</v>
       </c>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
       <c r="F29" s="64"/>
       <c r="G29" s="62"/>
       <c r="H29" s="62"/>
       <c r="I29" s="62"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="71"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="45" t="s">
         <v>1074</v>
       </c>
-      <c r="C30" s="72" t="s">
+      <c r="C30" s="70" t="s">
         <v>1075</v>
       </c>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
       <c r="F30" s="64"/>
       <c r="G30" s="62"/>
       <c r="H30" s="62"/>
       <c r="I30" s="62"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="72" t="s">
         <v>1076</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1077</v>
       </c>
-      <c r="C31" s="72" t="s">
+      <c r="C31" s="70" t="s">
         <v>1078</v>
       </c>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
       <c r="F31" s="64"/>
       <c r="G31" s="62"/>
       <c r="H31" s="62"/>
       <c r="I31" s="62"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="71"/>
+      <c r="A32" s="72"/>
       <c r="B32" s="45" t="s">
         <v>1079</v>
       </c>
-      <c r="C32" s="72" t="s">
+      <c r="C32" s="70" t="s">
         <v>1080</v>
       </c>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
       <c r="F32" s="64"/>
       <c r="G32" s="62"/>
       <c r="H32" s="62"/>
       <c r="I32" s="62"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="72" t="s">
         <v>1081</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1054</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="70" t="s">
         <v>1082</v>
       </c>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
       <c r="F33" s="64"/>
       <c r="G33" s="62"/>
       <c r="H33" s="62"/>
       <c r="I33" s="62"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="71"/>
+      <c r="A34" s="72"/>
       <c r="B34" s="45" t="s">
         <v>1083</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C34" s="70" t="s">
         <v>1084</v>
       </c>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="70"/>
       <c r="F34" s="64"/>
       <c r="G34" s="62"/>
       <c r="H34" s="62"/>
       <c r="I34" s="62"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="71"/>
+      <c r="A35" s="72"/>
       <c r="B35" s="45" t="s">
         <v>1085</v>
       </c>
-      <c r="C35" s="72" t="s">
+      <c r="C35" s="70" t="s">
         <v>1086</v>
       </c>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
       <c r="F35" s="64"/>
       <c r="G35" s="62"/>
       <c r="H35" s="62"/>
       <c r="I35" s="62"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="70" t="s">
         <v>1087</v>
       </c>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
       <c r="F36" s="64"/>
       <c r="G36" s="62"/>
       <c r="H36" s="62"/>
@@ -25225,97 +25000,97 @@
       <c r="B37" s="45" t="s">
         <v>1069</v>
       </c>
-      <c r="C37" s="72" t="s">
+      <c r="C37" s="70" t="s">
         <v>1089</v>
       </c>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
       <c r="F37" s="64"/>
       <c r="G37" s="62"/>
       <c r="H37" s="62"/>
       <c r="I37" s="62"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="72" t="s">
         <v>1090</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1091</v>
       </c>
-      <c r="C38" s="72" t="s">
+      <c r="C38" s="70" t="s">
         <v>1092</v>
       </c>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
       <c r="F38" s="64"/>
       <c r="G38" s="62"/>
       <c r="H38" s="62"/>
       <c r="I38" s="62"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="71"/>
+      <c r="A39" s="72"/>
       <c r="B39" s="45" t="s">
         <v>1093</v>
       </c>
-      <c r="C39" s="72" t="s">
+      <c r="C39" s="70" t="s">
         <v>1094</v>
       </c>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
       <c r="F39" s="64"/>
       <c r="G39" s="62"/>
       <c r="H39" s="62"/>
       <c r="I39" s="62"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="71"/>
+      <c r="A40" s="72"/>
       <c r="B40" s="45" t="s">
         <v>1095</v>
       </c>
-      <c r="C40" s="72" t="s">
+      <c r="C40" s="70" t="s">
         <v>1096</v>
       </c>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="70"/>
       <c r="F40" s="64"/>
       <c r="G40" s="62"/>
       <c r="H40" s="62"/>
       <c r="I40" s="62"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="71" t="s">
+      <c r="A41" s="72" t="s">
         <v>1097</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1098</v>
       </c>
-      <c r="C41" s="72" t="s">
+      <c r="C41" s="70" t="s">
         <v>1099</v>
       </c>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="70"/>
       <c r="F41" s="64"/>
       <c r="G41" s="62"/>
       <c r="H41" s="62"/>
       <c r="I41" s="62"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="71"/>
+      <c r="A42" s="72"/>
       <c r="B42" s="45" t="s">
         <v>1100</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="70" t="s">
         <v>1101</v>
       </c>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
       <c r="F42" s="64"/>
       <c r="G42" s="62"/>
       <c r="H42" s="62"/>
       <c r="I42" s="62"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="71"/>
+      <c r="A43" s="72"/>
       <c r="B43" s="45" t="s">
         <v>1102</v>
       </c>
@@ -25330,47 +25105,47 @@
       <c r="I43" s="62"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="71"/>
+      <c r="A44" s="72"/>
       <c r="B44" s="45" t="s">
         <v>1104</v>
       </c>
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="71" t="s">
         <v>1105</v>
       </c>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
       <c r="F44" s="64"/>
       <c r="G44" s="62"/>
       <c r="H44" s="62"/>
       <c r="I44" s="62"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="71" t="s">
+      <c r="A45" s="72" t="s">
         <v>1106</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1107</v>
       </c>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="71" t="s">
         <v>1108</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
       <c r="F45" s="64"/>
       <c r="G45" s="62"/>
       <c r="H45" s="62"/>
       <c r="I45" s="62"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="71"/>
+      <c r="A46" s="72"/>
       <c r="B46" s="45" t="s">
         <v>1109</v>
       </c>
-      <c r="C46" s="70" t="s">
+      <c r="C46" s="71" t="s">
         <v>1110</v>
       </c>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="71"/>
       <c r="F46" s="64"/>
       <c r="G46" s="62"/>
       <c r="H46" s="62"/>
@@ -25383,11 +25158,11 @@
       <c r="B47" s="45" t="s">
         <v>1069</v>
       </c>
-      <c r="C47" s="70" t="s">
+      <c r="C47" s="71" t="s">
         <v>1112</v>
       </c>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
       <c r="F47" s="64"/>
       <c r="G47" s="62"/>
       <c r="H47" s="62"/>
@@ -25400,165 +25175,165 @@
       <c r="B48" s="45" t="s">
         <v>1114</v>
       </c>
-      <c r="C48" s="70" t="s">
+      <c r="C48" s="71" t="s">
         <v>1115</v>
       </c>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
       <c r="F48" s="64"/>
       <c r="G48" s="62"/>
       <c r="H48" s="62"/>
       <c r="I48" s="62"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="71" t="s">
+      <c r="A49" s="72" t="s">
         <v>1116</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1117</v>
       </c>
-      <c r="C49" s="70" t="s">
+      <c r="C49" s="71" t="s">
         <v>1118</v>
       </c>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
       <c r="F49" s="64"/>
       <c r="G49" s="62"/>
       <c r="H49" s="62"/>
       <c r="I49" s="62"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="71"/>
+      <c r="A50" s="72"/>
       <c r="B50" s="45" t="s">
         <v>1119</v>
       </c>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="71" t="s">
         <v>1120</v>
       </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
       <c r="F50" s="64"/>
       <c r="G50" s="62"/>
       <c r="H50" s="62"/>
       <c r="I50" s="62"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="71"/>
+      <c r="A51" s="72"/>
       <c r="B51" s="45" t="s">
         <v>1064</v>
       </c>
-      <c r="C51" s="70" t="s">
+      <c r="C51" s="71" t="s">
         <v>1121</v>
       </c>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="71"/>
       <c r="F51" s="64"/>
       <c r="G51" s="62"/>
       <c r="H51" s="62"/>
       <c r="I51" s="62"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="71"/>
+      <c r="A52" s="72"/>
       <c r="B52" s="45" t="s">
         <v>1122</v>
       </c>
-      <c r="C52" s="70" t="s">
+      <c r="C52" s="71" t="s">
         <v>1123</v>
       </c>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="71"/>
       <c r="F52" s="64"/>
       <c r="G52" s="62"/>
       <c r="H52" s="62"/>
       <c r="I52" s="62"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="71"/>
+      <c r="A53" s="72"/>
       <c r="B53" s="45" t="s">
         <v>1060</v>
       </c>
-      <c r="C53" s="70" t="s">
+      <c r="C53" s="71" t="s">
         <v>1124</v>
       </c>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="71"/>
       <c r="F53" s="64"/>
       <c r="G53" s="62"/>
       <c r="H53" s="62"/>
       <c r="I53" s="62"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="71" t="s">
+      <c r="A54" s="72" t="s">
         <v>1125</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1126</v>
       </c>
-      <c r="C54" s="70" t="s">
+      <c r="C54" s="71" t="s">
         <v>1127</v>
       </c>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="71"/>
       <c r="F54" s="64"/>
       <c r="G54" s="62"/>
       <c r="H54" s="62"/>
       <c r="I54" s="62"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="71"/>
+      <c r="A55" s="72"/>
       <c r="B55" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="C55" s="70" t="s">
+      <c r="C55" s="71" t="s">
         <v>1129</v>
       </c>
-      <c r="D55" s="70"/>
-      <c r="E55" s="70"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="71"/>
       <c r="F55" s="64"/>
       <c r="G55" s="62"/>
       <c r="H55" s="62"/>
       <c r="I55" s="62"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="71"/>
+      <c r="A56" s="72"/>
       <c r="B56" s="5" t="s">
         <v>1130</v>
       </c>
-      <c r="C56" s="70" t="s">
+      <c r="C56" s="71" t="s">
         <v>1131</v>
       </c>
-      <c r="D56" s="70"/>
-      <c r="E56" s="70"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="71"/>
       <c r="F56" s="64"/>
       <c r="G56" s="62"/>
       <c r="H56" s="62"/>
       <c r="I56" s="62"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="71"/>
+      <c r="A57" s="72"/>
       <c r="B57" s="5" t="s">
         <v>1132</v>
       </c>
-      <c r="C57" s="70" t="s">
+      <c r="C57" s="71" t="s">
         <v>1133</v>
       </c>
-      <c r="D57" s="70"/>
-      <c r="E57" s="70"/>
+      <c r="D57" s="71"/>
+      <c r="E57" s="71"/>
       <c r="F57" s="64"/>
       <c r="G57" s="62"/>
       <c r="H57" s="62"/>
       <c r="I57" s="62"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="71"/>
+      <c r="A58" s="72"/>
       <c r="B58" s="5" t="s">
         <v>1134</v>
       </c>
-      <c r="C58" s="70" t="s">
+      <c r="C58" s="71" t="s">
         <v>1135</v>
       </c>
-      <c r="D58" s="70"/>
-      <c r="E58" s="70"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="71"/>
       <c r="F58" s="64"/>
       <c r="G58" s="62"/>
       <c r="H58" s="62"/>
@@ -25571,88 +25346,88 @@
       <c r="B59" s="5" t="s">
         <v>1069</v>
       </c>
-      <c r="C59" s="70" t="s">
+      <c r="C59" s="71" t="s">
         <v>1137</v>
       </c>
-      <c r="D59" s="70"/>
-      <c r="E59" s="70"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="71"/>
       <c r="F59" s="64"/>
       <c r="G59" s="62"/>
       <c r="H59" s="62"/>
       <c r="I59" s="62"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="71" t="s">
+      <c r="A60" s="72" t="s">
         <v>1138</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1139</v>
       </c>
-      <c r="C60" s="70" t="s">
+      <c r="C60" s="71" t="s">
         <v>1140</v>
       </c>
-      <c r="D60" s="70"/>
-      <c r="E60" s="70"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="71"/>
       <c r="F60" s="64"/>
       <c r="G60" s="62"/>
       <c r="H60" s="62"/>
       <c r="I60" s="62"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="71"/>
+      <c r="A61" s="72"/>
       <c r="B61" s="5" t="s">
         <v>1141</v>
       </c>
-      <c r="C61" s="70" t="s">
+      <c r="C61" s="71" t="s">
         <v>1142</v>
       </c>
-      <c r="D61" s="70"/>
-      <c r="E61" s="70"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="71"/>
       <c r="F61" s="64"/>
       <c r="G61" s="62"/>
       <c r="H61" s="62"/>
       <c r="I61" s="62"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="71"/>
+      <c r="A62" s="72"/>
       <c r="B62" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C62" s="70" t="s">
+      <c r="C62" s="71" t="s">
         <v>1144</v>
       </c>
-      <c r="D62" s="70"/>
-      <c r="E62" s="70"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="71"/>
       <c r="F62" s="64"/>
       <c r="G62" s="62"/>
       <c r="H62" s="62"/>
       <c r="I62" s="62"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="71"/>
+      <c r="A63" s="72"/>
       <c r="B63" s="5" t="s">
         <v>1145</v>
       </c>
-      <c r="C63" s="70" t="s">
+      <c r="C63" s="71" t="s">
         <v>1146</v>
       </c>
-      <c r="D63" s="70"/>
-      <c r="E63" s="70"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="71"/>
       <c r="F63" s="64"/>
       <c r="G63" s="62"/>
       <c r="H63" s="62"/>
       <c r="I63" s="62"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="71"/>
+      <c r="A64" s="72"/>
       <c r="B64" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="C64" s="70" t="s">
+      <c r="C64" s="71" t="s">
         <v>1148</v>
       </c>
-      <c r="D64" s="70"/>
-      <c r="E64" s="70"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="71"/>
       <c r="F64" s="64"/>
       <c r="G64" s="62"/>
       <c r="H64" s="62"/>
@@ -25660,30 +25435,72 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
@@ -25708,72 +25525,30 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -26238,6 +26013,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C30:F30"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C20:F20"/>
@@ -26250,12 +26031,6 @@
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -27357,13 +27132,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -27376,6 +27144,13 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -27746,6 +27521,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
@@ -27753,18 +27540,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -28231,6 +28006,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -28244,19 +28032,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29233,33 +29008,29 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:I23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="C24:D24"/>
@@ -29273,29 +29044,33 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -29780,6 +29555,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -29790,13 +29572,6 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -30204,11 +29979,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -30221,6 +29991,11 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -30263,15 +30038,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -30500,6 +30266,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
   <ds:schemaRefs>
@@ -30518,14 +30293,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30542,4 +30309,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:sparkles: Add missing indexed parameters to Cardiac MRI code system
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\db\dt4h\common-data-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DA3FC2-77B9-41A7-A90D-C78EB2E77B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C09CBEC-E42A-4E6A-AA3A-A9F874FD0D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="0" windowWidth="23232" windowHeight="25296" tabRatio="901" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="12" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -7328,22 +7328,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8723,6 +8723,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -8733,13 +8740,6 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8774,8 +8774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA632DE-857A-4068-95DB-7C01FA09C153}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9439,13 +9439,13 @@
         <v>462</v>
       </c>
       <c r="D39" s="66"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="72" t="s">
+      <c r="E39" s="70"/>
+      <c r="F39" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="42" t="s">
@@ -9454,11 +9454,11 @@
       <c r="B40" s="42" t="s">
         <v>465</v>
       </c>
-      <c r="C40" s="70" t="s">
+      <c r="C40" s="68" t="s">
         <v>466</v>
       </c>
-      <c r="D40" s="70"/>
-      <c r="E40" s="71"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="69"/>
       <c r="F40" s="67"/>
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
@@ -9471,11 +9471,11 @@
       <c r="B41" s="42" t="s">
         <v>468</v>
       </c>
-      <c r="C41" s="70" t="s">
+      <c r="C41" s="68" t="s">
         <v>469</v>
       </c>
-      <c r="D41" s="70"/>
-      <c r="E41" s="71"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="67"/>
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
@@ -9488,11 +9488,11 @@
       <c r="B42" s="42" t="s">
         <v>471</v>
       </c>
-      <c r="C42" s="70" t="s">
+      <c r="C42" s="68" t="s">
         <v>472</v>
       </c>
-      <c r="D42" s="70"/>
-      <c r="E42" s="71"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="69"/>
       <c r="F42" s="67"/>
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
@@ -9505,11 +9505,11 @@
       <c r="B43" s="42" t="s">
         <v>474</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="68" t="s">
         <v>2013</v>
       </c>
-      <c r="D43" s="70"/>
-      <c r="E43" s="71"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="67"/>
       <c r="G43" s="65"/>
       <c r="H43" s="65"/>
@@ -9522,11 +9522,11 @@
       <c r="B44" s="42" t="s">
         <v>476</v>
       </c>
-      <c r="C44" s="70" t="s">
+      <c r="C44" s="68" t="s">
         <v>477</v>
       </c>
-      <c r="D44" s="70"/>
-      <c r="E44" s="71"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="69"/>
       <c r="F44" s="67"/>
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
@@ -9539,11 +9539,11 @@
       <c r="B45" s="42" t="s">
         <v>479</v>
       </c>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="68" t="s">
         <v>480</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="71"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="69"/>
       <c r="F45" s="67"/>
       <c r="G45" s="65"/>
       <c r="H45" s="65"/>
@@ -9556,11 +9556,11 @@
       <c r="B46" s="42" t="s">
         <v>482</v>
       </c>
-      <c r="C46" s="70" t="s">
+      <c r="C46" s="68" t="s">
         <v>483</v>
       </c>
-      <c r="D46" s="70"/>
-      <c r="E46" s="71"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="69"/>
       <c r="F46" s="67"/>
       <c r="G46" s="65"/>
       <c r="H46" s="65"/>
@@ -9573,11 +9573,11 @@
       <c r="B47" s="42" t="s">
         <v>485</v>
       </c>
-      <c r="C47" s="70" t="s">
+      <c r="C47" s="68" t="s">
         <v>486</v>
       </c>
-      <c r="D47" s="70"/>
-      <c r="E47" s="71"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="69"/>
       <c r="F47" s="67"/>
       <c r="G47" s="65"/>
       <c r="H47" s="65"/>
@@ -9590,11 +9590,11 @@
       <c r="B48" s="42" t="s">
         <v>487</v>
       </c>
-      <c r="C48" s="70" t="s">
+      <c r="C48" s="68" t="s">
         <v>2014</v>
       </c>
-      <c r="D48" s="70"/>
-      <c r="E48" s="71"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="69"/>
       <c r="F48" s="67"/>
       <c r="G48" s="65"/>
       <c r="H48" s="65"/>
@@ -9607,11 +9607,11 @@
       <c r="B49" s="42" t="s">
         <v>489</v>
       </c>
-      <c r="C49" s="70" t="s">
+      <c r="C49" s="68" t="s">
         <v>490</v>
       </c>
-      <c r="D49" s="70"/>
-      <c r="E49" s="71"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="69"/>
       <c r="F49" s="67"/>
       <c r="G49" s="65"/>
       <c r="H49" s="65"/>
@@ -9624,11 +9624,11 @@
       <c r="B50" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="C50" s="70" t="s">
+      <c r="C50" s="68" t="s">
         <v>493</v>
       </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="71"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="69"/>
       <c r="F50" s="67"/>
       <c r="G50" s="65"/>
       <c r="H50" s="65"/>
@@ -9641,11 +9641,11 @@
       <c r="B51" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="C51" s="70" t="s">
+      <c r="C51" s="68" t="s">
         <v>496</v>
       </c>
-      <c r="D51" s="70"/>
-      <c r="E51" s="71"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="69"/>
       <c r="F51" s="67"/>
       <c r="G51" s="65"/>
       <c r="H51" s="65"/>
@@ -9658,11 +9658,11 @@
       <c r="B52" s="42" t="s">
         <v>498</v>
       </c>
-      <c r="C52" s="70" t="s">
+      <c r="C52" s="68" t="s">
         <v>499</v>
       </c>
-      <c r="D52" s="70"/>
-      <c r="E52" s="71"/>
+      <c r="D52" s="68"/>
+      <c r="E52" s="69"/>
       <c r="F52" s="67"/>
       <c r="G52" s="65"/>
       <c r="H52" s="65"/>
@@ -9675,11 +9675,11 @@
       <c r="B53" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="C53" s="70" t="s">
+      <c r="C53" s="68" t="s">
         <v>502</v>
       </c>
-      <c r="D53" s="70"/>
-      <c r="E53" s="71"/>
+      <c r="D53" s="68"/>
+      <c r="E53" s="69"/>
       <c r="F53" s="67"/>
       <c r="G53" s="65"/>
       <c r="H53" s="65"/>
@@ -9692,11 +9692,11 @@
       <c r="B54" s="42" t="s">
         <v>504</v>
       </c>
-      <c r="C54" s="70" t="s">
+      <c r="C54" s="68" t="s">
         <v>505</v>
       </c>
-      <c r="D54" s="70"/>
-      <c r="E54" s="71"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="69"/>
       <c r="F54" s="67"/>
       <c r="G54" s="65"/>
       <c r="H54" s="65"/>
@@ -9709,11 +9709,11 @@
       <c r="B55" s="42" t="s">
         <v>507</v>
       </c>
-      <c r="C55" s="70" t="s">
+      <c r="C55" s="68" t="s">
         <v>508</v>
       </c>
-      <c r="D55" s="70"/>
-      <c r="E55" s="71"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="69"/>
       <c r="F55" s="67"/>
       <c r="G55" s="65"/>
       <c r="H55" s="65"/>
@@ -9726,11 +9726,11 @@
       <c r="B56" s="42" t="s">
         <v>510</v>
       </c>
-      <c r="C56" s="70" t="s">
+      <c r="C56" s="68" t="s">
         <v>511</v>
       </c>
-      <c r="D56" s="70"/>
-      <c r="E56" s="71"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="69"/>
       <c r="F56" s="67"/>
       <c r="G56" s="65"/>
       <c r="H56" s="65"/>
@@ -9743,11 +9743,11 @@
       <c r="B57" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C57" s="70" t="s">
+      <c r="C57" s="68" t="s">
         <v>514</v>
       </c>
-      <c r="D57" s="70"/>
-      <c r="E57" s="71"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="69"/>
       <c r="F57" s="67"/>
       <c r="G57" s="65"/>
       <c r="H57" s="65"/>
@@ -9760,11 +9760,11 @@
       <c r="B58" s="42" t="s">
         <v>516</v>
       </c>
-      <c r="C58" s="70" t="s">
+      <c r="C58" s="68" t="s">
         <v>517</v>
       </c>
-      <c r="D58" s="70"/>
-      <c r="E58" s="71"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="69"/>
       <c r="F58" s="67"/>
       <c r="G58" s="65"/>
       <c r="H58" s="65"/>
@@ -9777,11 +9777,11 @@
       <c r="B59" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="C59" s="70" t="s">
+      <c r="C59" s="68" t="s">
         <v>520</v>
       </c>
-      <c r="D59" s="70"/>
-      <c r="E59" s="71"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="69"/>
       <c r="F59" s="67"/>
       <c r="G59" s="65"/>
       <c r="H59" s="65"/>
@@ -9794,11 +9794,11 @@
       <c r="B60" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="C60" s="70" t="s">
+      <c r="C60" s="68" t="s">
         <v>523</v>
       </c>
-      <c r="D60" s="70"/>
-      <c r="E60" s="71"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="69"/>
       <c r="F60" s="67"/>
       <c r="G60" s="65"/>
       <c r="H60" s="65"/>
@@ -9811,11 +9811,11 @@
       <c r="B61" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="C61" s="70" t="s">
+      <c r="C61" s="68" t="s">
         <v>526</v>
       </c>
-      <c r="D61" s="70"/>
-      <c r="E61" s="71"/>
+      <c r="D61" s="68"/>
+      <c r="E61" s="69"/>
       <c r="F61" s="67"/>
       <c r="G61" s="65"/>
       <c r="H61" s="65"/>
@@ -9828,11 +9828,11 @@
       <c r="B62" s="42" t="s">
         <v>528</v>
       </c>
-      <c r="C62" s="70" t="s">
+      <c r="C62" s="68" t="s">
         <v>529</v>
       </c>
-      <c r="D62" s="70"/>
-      <c r="E62" s="71"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="69"/>
       <c r="F62" s="67"/>
       <c r="G62" s="65"/>
       <c r="H62" s="65"/>
@@ -9845,11 +9845,11 @@
       <c r="B63" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C63" s="70" t="s">
+      <c r="C63" s="68" t="s">
         <v>532</v>
       </c>
-      <c r="D63" s="70"/>
-      <c r="E63" s="71"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="69"/>
       <c r="F63" s="67"/>
       <c r="G63" s="65"/>
       <c r="H63" s="65"/>
@@ -9862,11 +9862,11 @@
       <c r="B64" s="42" t="s">
         <v>533</v>
       </c>
-      <c r="C64" s="70" t="s">
+      <c r="C64" s="68" t="s">
         <v>534</v>
       </c>
-      <c r="D64" s="70"/>
-      <c r="E64" s="71"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="69"/>
       <c r="F64" s="67"/>
       <c r="G64" s="65"/>
       <c r="H64" s="65"/>
@@ -9879,11 +9879,11 @@
       <c r="B65" s="42" t="s">
         <v>536</v>
       </c>
-      <c r="C65" s="70" t="s">
+      <c r="C65" s="68" t="s">
         <v>537</v>
       </c>
-      <c r="D65" s="70"/>
-      <c r="E65" s="71"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="69"/>
       <c r="F65" s="67"/>
       <c r="G65" s="65"/>
       <c r="H65" s="65"/>
@@ -9896,11 +9896,11 @@
       <c r="B66" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C66" s="70" t="s">
+      <c r="C66" s="68" t="s">
         <v>2015</v>
       </c>
-      <c r="D66" s="70"/>
-      <c r="E66" s="71"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="69"/>
       <c r="F66" s="67"/>
       <c r="G66" s="65"/>
       <c r="H66" s="65"/>
@@ -9913,11 +9913,11 @@
       <c r="B67" s="42" t="s">
         <v>541</v>
       </c>
-      <c r="C67" s="70" t="s">
+      <c r="C67" s="68" t="s">
         <v>542</v>
       </c>
-      <c r="D67" s="70"/>
-      <c r="E67" s="71"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="69"/>
       <c r="F67" s="67"/>
       <c r="G67" s="65"/>
       <c r="H67" s="65"/>
@@ -9930,11 +9930,11 @@
       <c r="B68" s="42" t="s">
         <v>544</v>
       </c>
-      <c r="C68" s="70" t="s">
+      <c r="C68" s="68" t="s">
         <v>545</v>
       </c>
-      <c r="D68" s="70"/>
-      <c r="E68" s="71"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="69"/>
       <c r="F68" s="67"/>
       <c r="G68" s="65"/>
       <c r="H68" s="65"/>
@@ -9947,11 +9947,11 @@
       <c r="B69" s="42" t="s">
         <v>547</v>
       </c>
-      <c r="C69" s="70" t="s">
+      <c r="C69" s="68" t="s">
         <v>548</v>
       </c>
-      <c r="D69" s="70"/>
-      <c r="E69" s="71"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="69"/>
       <c r="F69" s="67"/>
       <c r="G69" s="65"/>
       <c r="H69" s="65"/>
@@ -9964,11 +9964,11 @@
       <c r="B70" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="C70" s="70" t="s">
+      <c r="C70" s="68" t="s">
         <v>551</v>
       </c>
-      <c r="D70" s="70"/>
-      <c r="E70" s="71"/>
+      <c r="D70" s="68"/>
+      <c r="E70" s="69"/>
       <c r="F70" s="67"/>
       <c r="G70" s="65"/>
       <c r="H70" s="65"/>
@@ -9981,11 +9981,11 @@
       <c r="B71" s="42" t="s">
         <v>553</v>
       </c>
-      <c r="C71" s="70" t="s">
+      <c r="C71" s="68" t="s">
         <v>554</v>
       </c>
-      <c r="D71" s="70"/>
-      <c r="E71" s="71"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="69"/>
       <c r="F71" s="67"/>
       <c r="G71" s="65"/>
       <c r="H71" s="65"/>
@@ -9998,11 +9998,11 @@
       <c r="B72" s="42" t="s">
         <v>556</v>
       </c>
-      <c r="C72" s="70" t="s">
+      <c r="C72" s="68" t="s">
         <v>557</v>
       </c>
-      <c r="D72" s="70"/>
-      <c r="E72" s="71"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="69"/>
       <c r="F72" s="67"/>
       <c r="G72" s="65"/>
       <c r="H72" s="65"/>
@@ -10015,11 +10015,11 @@
       <c r="B73" s="42" t="s">
         <v>559</v>
       </c>
-      <c r="C73" s="70" t="s">
+      <c r="C73" s="68" t="s">
         <v>560</v>
       </c>
-      <c r="D73" s="70"/>
-      <c r="E73" s="71"/>
+      <c r="D73" s="68"/>
+      <c r="E73" s="69"/>
       <c r="F73" s="67"/>
       <c r="G73" s="65"/>
       <c r="H73" s="65"/>
@@ -10032,11 +10032,11 @@
       <c r="B74" s="42" t="s">
         <v>562</v>
       </c>
-      <c r="C74" s="70" t="s">
+      <c r="C74" s="68" t="s">
         <v>563</v>
       </c>
-      <c r="D74" s="70"/>
-      <c r="E74" s="71"/>
+      <c r="D74" s="68"/>
+      <c r="E74" s="69"/>
       <c r="F74" s="67"/>
       <c r="G74" s="65"/>
       <c r="H74" s="65"/>
@@ -10049,11 +10049,11 @@
       <c r="B75" s="42" t="s">
         <v>565</v>
       </c>
-      <c r="C75" s="70" t="s">
+      <c r="C75" s="68" t="s">
         <v>566</v>
       </c>
-      <c r="D75" s="70"/>
-      <c r="E75" s="71"/>
+      <c r="D75" s="68"/>
+      <c r="E75" s="69"/>
       <c r="F75" s="67"/>
       <c r="G75" s="65"/>
       <c r="H75" s="65"/>
@@ -10066,11 +10066,11 @@
       <c r="B76" s="42" t="s">
         <v>568</v>
       </c>
-      <c r="C76" s="70" t="s">
+      <c r="C76" s="68" t="s">
         <v>569</v>
       </c>
-      <c r="D76" s="70"/>
-      <c r="E76" s="71"/>
+      <c r="D76" s="68"/>
+      <c r="E76" s="69"/>
       <c r="F76" s="67"/>
       <c r="G76" s="65"/>
       <c r="H76" s="65"/>
@@ -10083,11 +10083,11 @@
       <c r="B77" s="42" t="s">
         <v>571</v>
       </c>
-      <c r="C77" s="70" t="s">
+      <c r="C77" s="68" t="s">
         <v>572</v>
       </c>
-      <c r="D77" s="70"/>
-      <c r="E77" s="71"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="69"/>
       <c r="F77" s="67"/>
       <c r="G77" s="65"/>
       <c r="H77" s="65"/>
@@ -10100,11 +10100,11 @@
       <c r="B78" s="42" t="s">
         <v>574</v>
       </c>
-      <c r="C78" s="70" t="s">
+      <c r="C78" s="68" t="s">
         <v>575</v>
       </c>
-      <c r="D78" s="70"/>
-      <c r="E78" s="71"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="69"/>
       <c r="F78" s="67"/>
       <c r="G78" s="65"/>
       <c r="H78" s="65"/>
@@ -10117,11 +10117,11 @@
       <c r="B79" s="42" t="s">
         <v>577</v>
       </c>
-      <c r="C79" s="70" t="s">
+      <c r="C79" s="68" t="s">
         <v>578</v>
       </c>
-      <c r="D79" s="70"/>
-      <c r="E79" s="71"/>
+      <c r="D79" s="68"/>
+      <c r="E79" s="69"/>
       <c r="F79" s="67"/>
       <c r="G79" s="65"/>
       <c r="H79" s="65"/>
@@ -10134,11 +10134,11 @@
       <c r="B80" s="42" t="s">
         <v>580</v>
       </c>
-      <c r="C80" s="70" t="s">
+      <c r="C80" s="68" t="s">
         <v>581</v>
       </c>
-      <c r="D80" s="70"/>
-      <c r="E80" s="71"/>
+      <c r="D80" s="68"/>
+      <c r="E80" s="69"/>
       <c r="F80" s="67"/>
       <c r="G80" s="65"/>
       <c r="H80" s="65"/>
@@ -10151,11 +10151,11 @@
       <c r="B81" s="42" t="s">
         <v>583</v>
       </c>
-      <c r="C81" s="70" t="s">
+      <c r="C81" s="68" t="s">
         <v>584</v>
       </c>
-      <c r="D81" s="70"/>
-      <c r="E81" s="71"/>
+      <c r="D81" s="68"/>
+      <c r="E81" s="69"/>
       <c r="F81" s="67"/>
       <c r="G81" s="65"/>
       <c r="H81" s="65"/>
@@ -10168,11 +10168,11 @@
       <c r="B82" t="s">
         <v>2020</v>
       </c>
-      <c r="C82" s="68" t="s">
+      <c r="C82" s="72" t="s">
         <v>2017</v>
       </c>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
+      <c r="D82" s="72"/>
+      <c r="E82" s="72"/>
       <c r="F82" s="67"/>
       <c r="G82" s="65"/>
       <c r="H82" s="65"/>
@@ -10185,11 +10185,11 @@
       <c r="B83" t="s">
         <v>2021</v>
       </c>
-      <c r="C83" s="68" t="s">
+      <c r="C83" s="72" t="s">
         <v>2019</v>
       </c>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68"/>
+      <c r="D83" s="72"/>
+      <c r="E83" s="72"/>
       <c r="F83" s="67"/>
       <c r="G83" s="65"/>
       <c r="H83" s="65"/>
@@ -10197,36 +10197,73 @@
     </row>
   </sheetData>
   <mergeCells count="121">
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="F48:I48"/>
     <mergeCell ref="F49:I49"/>
@@ -10251,73 +10288,36 @@
     <mergeCell ref="C56:E56"/>
     <mergeCell ref="F55:I55"/>
     <mergeCell ref="F56:I56"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11182,14 +11182,41 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -11206,41 +11233,14 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -12398,7 +12398,7 @@
       <c r="I34" s="65"/>
       <c r="J34" s="65"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A35" s="49" t="s">
         <v>1779</v>
       </c>
@@ -12452,29 +12452,19 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
     <mergeCell ref="G32:J32"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
@@ -12487,19 +12477,29 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="G31:J31"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:F21" xr:uid="{7FAB08B6-9907-44B4-A82A-4A3E200D36A8}">
@@ -13811,25 +13811,23 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F30:I30"/>
     <mergeCell ref="F55:I55"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="F35:I35"/>
@@ -13843,23 +13841,25 @@
     <mergeCell ref="F49:I49"/>
     <mergeCell ref="F50:I50"/>
     <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F61:I61"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -15449,8 +15449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF00AD05-AD0A-4301-B0FD-56AA1951174D}">
   <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17024,7 +17024,7 @@
         <v>1439</v>
       </c>
       <c r="E78" t="s">
-        <v>1440</v>
+        <v>668</v>
       </c>
       <c r="F78" s="33" t="s">
         <v>1520</v>
@@ -18438,24 +18438,87 @@
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="111">
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H150:K150"/>
+    <mergeCell ref="H151:K151"/>
+    <mergeCell ref="H152:K152"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H149:K149"/>
+    <mergeCell ref="H138:K138"/>
+    <mergeCell ref="H139:K139"/>
+    <mergeCell ref="H140:K140"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H132:K132"/>
+    <mergeCell ref="H133:K133"/>
+    <mergeCell ref="H134:K134"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="H136:K136"/>
+    <mergeCell ref="H137:K137"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="H128:K128"/>
+    <mergeCell ref="H129:K129"/>
+    <mergeCell ref="H130:K130"/>
+    <mergeCell ref="H131:K131"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="H121:K121"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="H125:K125"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H76:K76"/>
     <mergeCell ref="H62:K62"/>
     <mergeCell ref="H63:K63"/>
     <mergeCell ref="H64:K64"/>
@@ -18468,87 +18531,24 @@
     <mergeCell ref="H58:K58"/>
     <mergeCell ref="H60:K60"/>
     <mergeCell ref="H61:K61"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="H128:K128"/>
-    <mergeCell ref="H129:K129"/>
-    <mergeCell ref="H130:K130"/>
-    <mergeCell ref="H131:K131"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="H138:K138"/>
-    <mergeCell ref="H139:K139"/>
-    <mergeCell ref="H140:K140"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H132:K132"/>
-    <mergeCell ref="H133:K133"/>
-    <mergeCell ref="H134:K134"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="H136:K136"/>
-    <mergeCell ref="H137:K137"/>
-    <mergeCell ref="H150:K150"/>
-    <mergeCell ref="H151:K151"/>
-    <mergeCell ref="H152:K152"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="H149:K149"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="H48:K48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21128,13 +21128,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F113:I113"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="F109:I109"/>
+    <mergeCell ref="F110:I110"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="F112:I112"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
     <mergeCell ref="C126:D126"/>
     <mergeCell ref="C119:D119"/>
     <mergeCell ref="C120:D120"/>
@@ -21143,14 +21144,13 @@
     <mergeCell ref="C123:D123"/>
     <mergeCell ref="C124:D124"/>
     <mergeCell ref="C125:D125"/>
-    <mergeCell ref="F109:I109"/>
-    <mergeCell ref="F110:I110"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="F112:I112"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="F113:I113"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -21970,15 +21970,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H53:K53"/>
     <mergeCell ref="H44:K44"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="H14:K14"/>
@@ -21991,6 +21982,15 @@
     <mergeCell ref="H41:K41"/>
     <mergeCell ref="H42:K42"/>
     <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H53:K53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22340,6 +22340,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
     <mergeCell ref="H33:K33"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
@@ -22349,14 +22357,6 @@
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="H31:K31"/>
     <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -22707,11 +22707,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H17:K17"/>
@@ -22724,6 +22719,11 @@
     <mergeCell ref="H24:K24"/>
     <mergeCell ref="H25:K25"/>
     <mergeCell ref="H27:K27"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -23794,10 +23794,10 @@
       <c r="B44" s="48" t="s">
         <v>1164</v>
       </c>
-      <c r="C44" s="68" t="s">
+      <c r="C44" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D44" s="68"/>
+      <c r="D44" s="72"/>
       <c r="E44" s="5" t="s">
         <v>1165</v>
       </c>
@@ -23811,10 +23811,10 @@
       <c r="B45" s="48" t="s">
         <v>1166</v>
       </c>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="72"/>
       <c r="E45" s="5" t="s">
         <v>1167</v>
       </c>
@@ -23828,10 +23828,10 @@
       <c r="B46" s="48" t="s">
         <v>1168</v>
       </c>
-      <c r="C46" s="68" t="s">
+      <c r="C46" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D46" s="68"/>
+      <c r="D46" s="72"/>
       <c r="E46" s="5" t="s">
         <v>1169</v>
       </c>
@@ -23845,10 +23845,10 @@
       <c r="B47" s="48" t="s">
         <v>1170</v>
       </c>
-      <c r="C47" s="68" t="s">
+      <c r="C47" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D47" s="68"/>
+      <c r="D47" s="72"/>
       <c r="E47" s="5" t="s">
         <v>1171</v>
       </c>
@@ -23862,10 +23862,10 @@
       <c r="B48" s="48" t="s">
         <v>1172</v>
       </c>
-      <c r="C48" s="68" t="s">
+      <c r="C48" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D48" s="68"/>
+      <c r="D48" s="72"/>
       <c r="E48" s="5" t="s">
         <v>1173</v>
       </c>
@@ -23879,10 +23879,10 @@
       <c r="B49" s="48" t="s">
         <v>1174</v>
       </c>
-      <c r="C49" s="68" t="s">
+      <c r="C49" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D49" s="68"/>
+      <c r="D49" s="72"/>
       <c r="E49" s="5" t="s">
         <v>1175</v>
       </c>
@@ -23896,10 +23896,10 @@
       <c r="B50" s="48" t="s">
         <v>1176</v>
       </c>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="72"/>
       <c r="E50" s="5" t="s">
         <v>1177</v>
       </c>
@@ -23913,10 +23913,10 @@
       <c r="B51" s="48" t="s">
         <v>1178</v>
       </c>
-      <c r="C51" s="68" t="s">
+      <c r="C51" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D51" s="68"/>
+      <c r="D51" s="72"/>
       <c r="E51" s="5" t="s">
         <v>1179</v>
       </c>
@@ -23930,10 +23930,10 @@
       <c r="B52" s="48" t="s">
         <v>1180</v>
       </c>
-      <c r="C52" s="68" t="s">
+      <c r="C52" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D52" s="68"/>
+      <c r="D52" s="72"/>
       <c r="E52" s="5" t="s">
         <v>1181</v>
       </c>
@@ -23947,10 +23947,10 @@
       <c r="B53" s="48" t="s">
         <v>1182</v>
       </c>
-      <c r="C53" s="68" t="s">
+      <c r="C53" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D53" s="68"/>
+      <c r="D53" s="72"/>
       <c r="E53" s="5" t="s">
         <v>1183</v>
       </c>
@@ -23964,10 +23964,10 @@
       <c r="B54" s="48" t="s">
         <v>1184</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="C54" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D54" s="68"/>
+      <c r="D54" s="72"/>
       <c r="E54" s="5" t="s">
         <v>1185</v>
       </c>
@@ -23981,10 +23981,10 @@
       <c r="B55" s="48" t="s">
         <v>1186</v>
       </c>
-      <c r="C55" s="68" t="s">
+      <c r="C55" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D55" s="68"/>
+      <c r="D55" s="72"/>
       <c r="E55" s="5" t="s">
         <v>1187</v>
       </c>
@@ -23998,10 +23998,10 @@
       <c r="B56" s="48" t="s">
         <v>1188</v>
       </c>
-      <c r="C56" s="68" t="s">
+      <c r="C56" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D56" s="68"/>
+      <c r="D56" s="72"/>
       <c r="E56" s="5" t="s">
         <v>1189</v>
       </c>
@@ -24015,10 +24015,10 @@
       <c r="B57" s="48" t="s">
         <v>1190</v>
       </c>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="72"/>
       <c r="E57" s="5" t="s">
         <v>1191</v>
       </c>
@@ -24032,10 +24032,10 @@
       <c r="B58" s="48" t="s">
         <v>1192</v>
       </c>
-      <c r="C58" s="68" t="s">
+      <c r="C58" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D58" s="68"/>
+      <c r="D58" s="72"/>
       <c r="E58" s="5" t="s">
         <v>1193</v>
       </c>
@@ -24049,10 +24049,10 @@
       <c r="B59" s="48" t="s">
         <v>1194</v>
       </c>
-      <c r="C59" s="68" t="s">
+      <c r="C59" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D59" s="68"/>
+      <c r="D59" s="72"/>
       <c r="E59" s="5" t="s">
         <v>1195</v>
       </c>
@@ -24066,10 +24066,10 @@
       <c r="B60" s="48" t="s">
         <v>1196</v>
       </c>
-      <c r="C60" s="68" t="s">
+      <c r="C60" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D60" s="68"/>
+      <c r="D60" s="72"/>
       <c r="E60" s="5" t="s">
         <v>1197</v>
       </c>
@@ -24083,10 +24083,10 @@
       <c r="B61" s="48" t="s">
         <v>1198</v>
       </c>
-      <c r="C61" s="68" t="s">
+      <c r="C61" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D61" s="68"/>
+      <c r="D61" s="72"/>
       <c r="E61" s="5" t="s">
         <v>1199</v>
       </c>
@@ -24100,10 +24100,10 @@
       <c r="B62" s="48" t="s">
         <v>1200</v>
       </c>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="72"/>
       <c r="E62" s="5" t="s">
         <v>1201</v>
       </c>
@@ -24117,10 +24117,10 @@
       <c r="B63" s="48" t="s">
         <v>1202</v>
       </c>
-      <c r="C63" s="68" t="s">
+      <c r="C63" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D63" s="68"/>
+      <c r="D63" s="72"/>
       <c r="E63" s="5" t="s">
         <v>1203</v>
       </c>
@@ -24134,10 +24134,10 @@
       <c r="B64" s="48" t="s">
         <v>1204</v>
       </c>
-      <c r="C64" s="68" t="s">
+      <c r="C64" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D64" s="68"/>
+      <c r="D64" s="72"/>
       <c r="E64" s="5" t="s">
         <v>1205</v>
       </c>
@@ -24151,10 +24151,10 @@
       <c r="B65" s="48" t="s">
         <v>1206</v>
       </c>
-      <c r="C65" s="68" t="s">
+      <c r="C65" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D65" s="68"/>
+      <c r="D65" s="72"/>
       <c r="E65" s="5" t="s">
         <v>1207</v>
       </c>
@@ -24168,10 +24168,10 @@
       <c r="B66" s="48" t="s">
         <v>1208</v>
       </c>
-      <c r="C66" s="68" t="s">
+      <c r="C66" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D66" s="68"/>
+      <c r="D66" s="72"/>
       <c r="E66" s="5" t="s">
         <v>1209</v>
       </c>
@@ -24185,10 +24185,10 @@
       <c r="B67" s="48" t="s">
         <v>1210</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D67" s="68"/>
+      <c r="D67" s="72"/>
       <c r="E67" s="5" t="s">
         <v>1211</v>
       </c>
@@ -24202,10 +24202,10 @@
       <c r="B68" s="48" t="s">
         <v>1212</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="72"/>
       <c r="E68" s="5" t="s">
         <v>1213</v>
       </c>
@@ -24219,10 +24219,10 @@
       <c r="B69" s="48" t="s">
         <v>1214</v>
       </c>
-      <c r="C69" s="68" t="s">
+      <c r="C69" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D69" s="68"/>
+      <c r="D69" s="72"/>
       <c r="E69" s="5" t="s">
         <v>1215</v>
       </c>
@@ -24236,10 +24236,10 @@
       <c r="B70" s="48" t="s">
         <v>1216</v>
       </c>
-      <c r="C70" s="68" t="s">
+      <c r="C70" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D70" s="68"/>
+      <c r="D70" s="72"/>
       <c r="E70" s="5" t="s">
         <v>1217</v>
       </c>
@@ -24253,10 +24253,10 @@
       <c r="B71" s="48" t="s">
         <v>1218</v>
       </c>
-      <c r="C71" s="68" t="s">
+      <c r="C71" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D71" s="68"/>
+      <c r="D71" s="72"/>
       <c r="E71" s="5" t="s">
         <v>1219</v>
       </c>
@@ -24270,10 +24270,10 @@
       <c r="B72" s="48" t="s">
         <v>1220</v>
       </c>
-      <c r="C72" s="68" t="s">
+      <c r="C72" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D72" s="68"/>
+      <c r="D72" s="72"/>
       <c r="E72" s="5" t="s">
         <v>1221</v>
       </c>
@@ -24287,10 +24287,10 @@
       <c r="B73" s="48" t="s">
         <v>1222</v>
       </c>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="72"/>
       <c r="E73" s="5" t="s">
         <v>1223</v>
       </c>
@@ -24304,10 +24304,10 @@
       <c r="B74" s="48" t="s">
         <v>1224</v>
       </c>
-      <c r="C74" s="68" t="s">
+      <c r="C74" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D74" s="68"/>
+      <c r="D74" s="72"/>
       <c r="E74" s="5" t="s">
         <v>1225</v>
       </c>
@@ -24321,10 +24321,10 @@
       <c r="B75" s="48" t="s">
         <v>1226</v>
       </c>
-      <c r="C75" s="68" t="s">
+      <c r="C75" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D75" s="68"/>
+      <c r="D75" s="72"/>
       <c r="E75" s="5" t="s">
         <v>1227</v>
       </c>
@@ -24338,10 +24338,10 @@
       <c r="B76" s="48" t="s">
         <v>1228</v>
       </c>
-      <c r="C76" s="68" t="s">
+      <c r="C76" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D76" s="68"/>
+      <c r="D76" s="72"/>
       <c r="E76" s="5" t="s">
         <v>1229</v>
       </c>
@@ -24355,10 +24355,10 @@
       <c r="B77" s="48" t="s">
         <v>1230</v>
       </c>
-      <c r="C77" s="68" t="s">
+      <c r="C77" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D77" s="68"/>
+      <c r="D77" s="72"/>
       <c r="E77" s="5" t="s">
         <v>1231</v>
       </c>
@@ -24372,10 +24372,10 @@
       <c r="B78" s="48" t="s">
         <v>1232</v>
       </c>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="72"/>
       <c r="E78" s="5" t="s">
         <v>1233</v>
       </c>
@@ -24389,10 +24389,10 @@
       <c r="B79" s="48" t="s">
         <v>1234</v>
       </c>
-      <c r="C79" s="68" t="s">
+      <c r="C79" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D79" s="68"/>
+      <c r="D79" s="72"/>
       <c r="E79" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24406,10 +24406,10 @@
       <c r="B80" s="48" t="s">
         <v>1236</v>
       </c>
-      <c r="C80" s="68" t="s">
+      <c r="C80" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D80" s="68"/>
+      <c r="D80" s="72"/>
       <c r="E80" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24423,10 +24423,10 @@
       <c r="B81" s="48" t="s">
         <v>1238</v>
       </c>
-      <c r="C81" s="68" t="s">
+      <c r="C81" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D81" s="68"/>
+      <c r="D81" s="72"/>
       <c r="E81" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24440,10 +24440,10 @@
       <c r="B82" s="48" t="s">
         <v>1240</v>
       </c>
-      <c r="C82" s="68" t="s">
+      <c r="C82" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D82" s="68"/>
+      <c r="D82" s="72"/>
       <c r="E82" s="5" t="s">
         <v>1241</v>
       </c>
@@ -24457,10 +24457,10 @@
       <c r="B83" s="48" t="s">
         <v>1269</v>
       </c>
-      <c r="C83" s="68" t="s">
+      <c r="C83" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D83" s="68"/>
+      <c r="D83" s="72"/>
       <c r="E83" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24474,10 +24474,10 @@
       <c r="B84" s="48" t="s">
         <v>1270</v>
       </c>
-      <c r="C84" s="68" t="s">
+      <c r="C84" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D84" s="68"/>
+      <c r="D84" s="72"/>
       <c r="E84" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24491,10 +24491,10 @@
       <c r="B85" s="48" t="s">
         <v>1271</v>
       </c>
-      <c r="C85" s="68" t="s">
+      <c r="C85" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D85" s="68"/>
+      <c r="D85" s="72"/>
       <c r="E85" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24508,10 +24508,10 @@
       <c r="B86" s="48" t="s">
         <v>1272</v>
       </c>
-      <c r="C86" s="68" t="s">
+      <c r="C86" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D86" s="68"/>
+      <c r="D86" s="72"/>
       <c r="E86" s="5" t="s">
         <v>1242</v>
       </c>
@@ -24525,10 +24525,10 @@
       <c r="B87" s="48" t="s">
         <v>1243</v>
       </c>
-      <c r="C87" s="68" t="s">
+      <c r="C87" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D87" s="68"/>
+      <c r="D87" s="72"/>
       <c r="E87" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24542,10 +24542,10 @@
       <c r="B88" s="48" t="s">
         <v>1244</v>
       </c>
-      <c r="C88" s="68" t="s">
+      <c r="C88" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D88" s="68"/>
+      <c r="D88" s="72"/>
       <c r="E88" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24559,10 +24559,10 @@
       <c r="B89" s="48" t="s">
         <v>1245</v>
       </c>
-      <c r="C89" s="68" t="s">
+      <c r="C89" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D89" s="68"/>
+      <c r="D89" s="72"/>
       <c r="E89" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24576,10 +24576,10 @@
       <c r="B90" s="48" t="s">
         <v>1246</v>
       </c>
-      <c r="C90" s="68" t="s">
+      <c r="C90" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D90" s="68"/>
+      <c r="D90" s="72"/>
       <c r="E90" s="5" t="s">
         <v>1242</v>
       </c>
@@ -24593,10 +24593,10 @@
       <c r="B91" s="48" t="s">
         <v>1273</v>
       </c>
-      <c r="C91" s="68" t="s">
+      <c r="C91" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D91" s="68"/>
+      <c r="D91" s="72"/>
       <c r="E91" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24610,10 +24610,10 @@
       <c r="B92" s="48" t="s">
         <v>1274</v>
       </c>
-      <c r="C92" s="68" t="s">
+      <c r="C92" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D92" s="68"/>
+      <c r="D92" s="72"/>
       <c r="E92" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24627,10 +24627,10 @@
       <c r="B93" s="48" t="s">
         <v>1275</v>
       </c>
-      <c r="C93" s="68" t="s">
+      <c r="C93" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D93" s="68"/>
+      <c r="D93" s="72"/>
       <c r="E93" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24644,10 +24644,10 @@
       <c r="B94" s="48" t="s">
         <v>1276</v>
       </c>
-      <c r="C94" s="68" t="s">
+      <c r="C94" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D94" s="68"/>
+      <c r="D94" s="72"/>
       <c r="E94" s="5" t="s">
         <v>1242</v>
       </c>
@@ -24661,10 +24661,10 @@
       <c r="B95" s="48" t="s">
         <v>1277</v>
       </c>
-      <c r="C95" s="68" t="s">
+      <c r="C95" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D95" s="68"/>
+      <c r="D95" s="72"/>
       <c r="E95" s="5" t="s">
         <v>1247</v>
       </c>
@@ -24678,10 +24678,10 @@
       <c r="B96" s="48" t="s">
         <v>1248</v>
       </c>
-      <c r="C96" s="68" t="s">
+      <c r="C96" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D96" s="68"/>
+      <c r="D96" s="72"/>
       <c r="E96" s="5" t="s">
         <v>1249</v>
       </c>
@@ -24695,10 +24695,10 @@
       <c r="B97" s="48" t="s">
         <v>1250</v>
       </c>
-      <c r="C97" s="68" t="s">
+      <c r="C97" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D97" s="68"/>
+      <c r="D97" s="72"/>
       <c r="E97" s="5" t="s">
         <v>1251</v>
       </c>
@@ -24712,10 +24712,10 @@
       <c r="B98" s="48" t="s">
         <v>1252</v>
       </c>
-      <c r="C98" s="68" t="s">
+      <c r="C98" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D98" s="68"/>
+      <c r="D98" s="72"/>
       <c r="E98" s="5" t="s">
         <v>1253</v>
       </c>
@@ -24729,10 +24729,10 @@
       <c r="B99" s="48" t="s">
         <v>1254</v>
       </c>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="72"/>
       <c r="E99" s="5" t="s">
         <v>1255</v>
       </c>
@@ -24746,10 +24746,10 @@
       <c r="B100" s="48" t="s">
         <v>1256</v>
       </c>
-      <c r="C100" s="68" t="s">
+      <c r="C100" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D100" s="68"/>
+      <c r="D100" s="72"/>
       <c r="E100" s="5" t="s">
         <v>1257</v>
       </c>
@@ -24763,10 +24763,10 @@
       <c r="B101" s="48" t="s">
         <v>1258</v>
       </c>
-      <c r="C101" s="68" t="s">
+      <c r="C101" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D101" s="68"/>
+      <c r="D101" s="72"/>
       <c r="E101" s="5" t="s">
         <v>1259</v>
       </c>
@@ -24780,10 +24780,10 @@
       <c r="B102" s="48" t="s">
         <v>1260</v>
       </c>
-      <c r="C102" s="68" t="s">
+      <c r="C102" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D102" s="68"/>
+      <c r="D102" s="72"/>
       <c r="E102" s="5" t="s">
         <v>1253</v>
       </c>
@@ -24797,10 +24797,10 @@
       <c r="B103" s="48" t="s">
         <v>1261</v>
       </c>
-      <c r="C103" s="68" t="s">
+      <c r="C103" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D103" s="68"/>
+      <c r="D103" s="72"/>
       <c r="E103" s="5" t="s">
         <v>1255</v>
       </c>
@@ -24814,10 +24814,10 @@
       <c r="B104" s="48" t="s">
         <v>1262</v>
       </c>
-      <c r="C104" s="68" t="s">
+      <c r="C104" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D104" s="68"/>
+      <c r="D104" s="72"/>
       <c r="E104" s="5" t="s">
         <v>1257</v>
       </c>
@@ -24831,10 +24831,10 @@
       <c r="B105" s="48" t="s">
         <v>1263</v>
       </c>
-      <c r="C105" s="68" t="s">
+      <c r="C105" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D105" s="68"/>
+      <c r="D105" s="72"/>
       <c r="E105" s="5" t="s">
         <v>1259</v>
       </c>
@@ -24848,10 +24848,10 @@
       <c r="B106" s="48" t="s">
         <v>1264</v>
       </c>
-      <c r="C106" s="68" t="s">
+      <c r="C106" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D106" s="68"/>
+      <c r="D106" s="72"/>
       <c r="E106" s="5" t="s">
         <v>1265</v>
       </c>
@@ -24865,10 +24865,10 @@
       <c r="B107" s="48" t="s">
         <v>1266</v>
       </c>
-      <c r="C107" s="68" t="s">
+      <c r="C107" s="72" t="s">
         <v>1278</v>
       </c>
-      <c r="D107" s="68"/>
+      <c r="D107" s="72"/>
       <c r="E107" s="5" t="s">
         <v>1267</v>
       </c>
@@ -24879,49 +24879,108 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C79:D79"/>
     <mergeCell ref="C80:D80"/>
@@ -24946,108 +25005,49 @@
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="C75:D75"/>
     <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26938,210 +26938,210 @@
         <v>1037</v>
       </c>
       <c r="D14" s="66"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="72" t="s">
+      <c r="E14" s="70"/>
+      <c r="F14" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="74" t="s">
         <v>1038</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1039</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="68" t="s">
         <v>1040</v>
       </c>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
       <c r="F15" s="67"/>
       <c r="G15" s="65"/>
       <c r="H15" s="65"/>
       <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="73"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="42" t="s">
         <v>1041</v>
       </c>
-      <c r="C16" s="70" t="s">
+      <c r="C16" s="68" t="s">
         <v>1042</v>
       </c>
-      <c r="D16" s="70"/>
-      <c r="E16" s="71"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="69"/>
       <c r="F16" s="67"/>
       <c r="G16" s="65"/>
       <c r="H16" s="65"/>
       <c r="I16" s="65"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="73"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="42" t="s">
         <v>1043</v>
       </c>
-      <c r="C17" s="70" t="s">
+      <c r="C17" s="68" t="s">
         <v>1044</v>
       </c>
-      <c r="D17" s="70"/>
-      <c r="E17" s="71"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="67"/>
       <c r="G17" s="65"/>
       <c r="H17" s="65"/>
       <c r="I17" s="65"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="73"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="42" t="s">
         <v>1045</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="69" t="s">
         <v>1046</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="67"/>
       <c r="G18" s="65"/>
       <c r="H18" s="65"/>
       <c r="I18" s="65"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="73"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="42" t="s">
         <v>1047</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="69" t="s">
         <v>1048</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="67"/>
       <c r="G19" s="65"/>
       <c r="H19" s="65"/>
       <c r="I19" s="65"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="75" t="s">
         <v>1049</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1050</v>
       </c>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="69" t="s">
         <v>1051</v>
       </c>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
       <c r="F20" s="67"/>
       <c r="G20" s="65"/>
       <c r="H20" s="65"/>
       <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="74"/>
+      <c r="A21" s="75"/>
       <c r="B21" s="42" t="s">
         <v>1052</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="69" t="s">
         <v>1053</v>
       </c>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="67"/>
       <c r="G21" s="65"/>
       <c r="H21" s="65"/>
       <c r="I21" s="65"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="74"/>
+      <c r="A22" s="75"/>
       <c r="B22" s="42" t="s">
         <v>1054</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="69" t="s">
         <v>1055</v>
       </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
       <c r="F22" s="67"/>
       <c r="G22" s="65"/>
       <c r="H22" s="65"/>
       <c r="I22" s="65"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="74"/>
+      <c r="A23" s="75"/>
       <c r="B23" s="42" t="s">
         <v>1056</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="69" t="s">
         <v>1057</v>
       </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="67"/>
       <c r="G23" s="65"/>
       <c r="H23" s="65"/>
       <c r="I23" s="65"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="75" t="s">
         <v>1058</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1050</v>
       </c>
-      <c r="C24" s="71" t="s">
+      <c r="C24" s="69" t="s">
         <v>1059</v>
       </c>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="67"/>
       <c r="G24" s="65"/>
       <c r="H24" s="65"/>
       <c r="I24" s="65"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="74"/>
+      <c r="A25" s="75"/>
       <c r="B25" s="42" t="s">
         <v>1060</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="69" t="s">
         <v>1061</v>
       </c>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="67"/>
       <c r="G25" s="65"/>
       <c r="H25" s="65"/>
       <c r="I25" s="65"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="74"/>
+      <c r="A26" s="75"/>
       <c r="B26" s="42" t="s">
         <v>1054</v>
       </c>
-      <c r="C26" s="71" t="s">
+      <c r="C26" s="69" t="s">
         <v>1062</v>
       </c>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="67"/>
       <c r="G26" s="65"/>
       <c r="H26" s="65"/>
       <c r="I26" s="65"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="74"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="42" t="s">
         <v>1056</v>
       </c>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="73" t="s">
         <v>1063</v>
       </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
       <c r="F27" s="67"/>
       <c r="G27" s="65"/>
       <c r="H27" s="65"/>
@@ -27154,137 +27154,137 @@
       <c r="B28" s="45" t="s">
         <v>1065</v>
       </c>
-      <c r="C28" s="75" t="s">
+      <c r="C28" s="73" t="s">
         <v>1066</v>
       </c>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
       <c r="F28" s="67"/>
       <c r="G28" s="65"/>
       <c r="H28" s="65"/>
       <c r="I28" s="65"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="75" t="s">
         <v>1067</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1068</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="73" t="s">
         <v>1069</v>
       </c>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73"/>
       <c r="F29" s="67"/>
       <c r="G29" s="65"/>
       <c r="H29" s="65"/>
       <c r="I29" s="65"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="74"/>
+      <c r="A30" s="75"/>
       <c r="B30" s="45" t="s">
         <v>1070</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="73" t="s">
         <v>1071</v>
       </c>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="73"/>
       <c r="F30" s="67"/>
       <c r="G30" s="65"/>
       <c r="H30" s="65"/>
       <c r="I30" s="65"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="75" t="s">
         <v>1072</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1073</v>
       </c>
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="73" t="s">
         <v>1074</v>
       </c>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
       <c r="F31" s="67"/>
       <c r="G31" s="65"/>
       <c r="H31" s="65"/>
       <c r="I31" s="65"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="74"/>
+      <c r="A32" s="75"/>
       <c r="B32" s="45" t="s">
         <v>1075</v>
       </c>
-      <c r="C32" s="75" t="s">
+      <c r="C32" s="73" t="s">
         <v>1076</v>
       </c>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="73"/>
       <c r="F32" s="67"/>
       <c r="G32" s="65"/>
       <c r="H32" s="65"/>
       <c r="I32" s="65"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="75" t="s">
         <v>1077</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1050</v>
       </c>
-      <c r="C33" s="75" t="s">
+      <c r="C33" s="73" t="s">
         <v>1078</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
+      <c r="D33" s="73"/>
+      <c r="E33" s="73"/>
       <c r="F33" s="67"/>
       <c r="G33" s="65"/>
       <c r="H33" s="65"/>
       <c r="I33" s="65"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="74"/>
+      <c r="A34" s="75"/>
       <c r="B34" s="45" t="s">
         <v>1079</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="73" t="s">
         <v>1080</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
       <c r="F34" s="67"/>
       <c r="G34" s="65"/>
       <c r="H34" s="65"/>
       <c r="I34" s="65"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="74"/>
+      <c r="A35" s="75"/>
       <c r="B35" s="45" t="s">
         <v>1081</v>
       </c>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="73" t="s">
         <v>1082</v>
       </c>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="73"/>
       <c r="F35" s="67"/>
       <c r="G35" s="65"/>
       <c r="H35" s="65"/>
       <c r="I35" s="65"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="74"/>
+      <c r="A36" s="75"/>
       <c r="B36" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="73" t="s">
         <v>1083</v>
       </c>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
       <c r="F36" s="67"/>
       <c r="G36" s="65"/>
       <c r="H36" s="65"/>
@@ -27297,97 +27297,97 @@
       <c r="B37" s="45" t="s">
         <v>1065</v>
       </c>
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="73" t="s">
         <v>1085</v>
       </c>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
       <c r="F37" s="67"/>
       <c r="G37" s="65"/>
       <c r="H37" s="65"/>
       <c r="I37" s="65"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="74" t="s">
+      <c r="A38" s="75" t="s">
         <v>1086</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1087</v>
       </c>
-      <c r="C38" s="75" t="s">
+      <c r="C38" s="73" t="s">
         <v>1088</v>
       </c>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
       <c r="F38" s="67"/>
       <c r="G38" s="65"/>
       <c r="H38" s="65"/>
       <c r="I38" s="65"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="74"/>
+      <c r="A39" s="75"/>
       <c r="B39" s="45" t="s">
         <v>1089</v>
       </c>
-      <c r="C39" s="75" t="s">
+      <c r="C39" s="73" t="s">
         <v>1090</v>
       </c>
-      <c r="D39" s="75"/>
-      <c r="E39" s="75"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
       <c r="F39" s="67"/>
       <c r="G39" s="65"/>
       <c r="H39" s="65"/>
       <c r="I39" s="65"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="74"/>
+      <c r="A40" s="75"/>
       <c r="B40" s="45" t="s">
         <v>1091</v>
       </c>
-      <c r="C40" s="75" t="s">
+      <c r="C40" s="73" t="s">
         <v>1092</v>
       </c>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
       <c r="F40" s="67"/>
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
       <c r="I40" s="65"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="74" t="s">
+      <c r="A41" s="75" t="s">
         <v>1093</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1094</v>
       </c>
-      <c r="C41" s="75" t="s">
+      <c r="C41" s="73" t="s">
         <v>1095</v>
       </c>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
       <c r="F41" s="67"/>
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
       <c r="I41" s="65"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="74"/>
+      <c r="A42" s="75"/>
       <c r="B42" s="45" t="s">
         <v>1096</v>
       </c>
-      <c r="C42" s="75" t="s">
+      <c r="C42" s="73" t="s">
         <v>1097</v>
       </c>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
       <c r="F42" s="67"/>
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
       <c r="I42" s="65"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="74"/>
+      <c r="A43" s="75"/>
       <c r="B43" s="45" t="s">
         <v>1098</v>
       </c>
@@ -27402,47 +27402,47 @@
       <c r="I43" s="65"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="74"/>
+      <c r="A44" s="75"/>
       <c r="B44" s="45" t="s">
         <v>1100</v>
       </c>
-      <c r="C44" s="73" t="s">
+      <c r="C44" s="74" t="s">
         <v>1101</v>
       </c>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
       <c r="F44" s="67"/>
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
       <c r="I44" s="65"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="74" t="s">
+      <c r="A45" s="75" t="s">
         <v>1102</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1103</v>
       </c>
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="74" t="s">
         <v>1104</v>
       </c>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
       <c r="F45" s="67"/>
       <c r="G45" s="65"/>
       <c r="H45" s="65"/>
       <c r="I45" s="65"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="74"/>
+      <c r="A46" s="75"/>
       <c r="B46" s="45" t="s">
         <v>1105</v>
       </c>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="74" t="s">
         <v>1106</v>
       </c>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
       <c r="F46" s="67"/>
       <c r="G46" s="65"/>
       <c r="H46" s="65"/>
@@ -27455,11 +27455,11 @@
       <c r="B47" s="45" t="s">
         <v>1065</v>
       </c>
-      <c r="C47" s="73" t="s">
+      <c r="C47" s="74" t="s">
         <v>1108</v>
       </c>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
       <c r="F47" s="67"/>
       <c r="G47" s="65"/>
       <c r="H47" s="65"/>
@@ -27472,165 +27472,165 @@
       <c r="B48" s="45" t="s">
         <v>1110</v>
       </c>
-      <c r="C48" s="73" t="s">
+      <c r="C48" s="74" t="s">
         <v>1111</v>
       </c>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
       <c r="F48" s="67"/>
       <c r="G48" s="65"/>
       <c r="H48" s="65"/>
       <c r="I48" s="65"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="74" t="s">
+      <c r="A49" s="75" t="s">
         <v>1112</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1113</v>
       </c>
-      <c r="C49" s="73" t="s">
+      <c r="C49" s="74" t="s">
         <v>1114</v>
       </c>
-      <c r="D49" s="73"/>
-      <c r="E49" s="73"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
       <c r="F49" s="67"/>
       <c r="G49" s="65"/>
       <c r="H49" s="65"/>
       <c r="I49" s="65"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="74"/>
+      <c r="A50" s="75"/>
       <c r="B50" s="45" t="s">
         <v>1115</v>
       </c>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="74" t="s">
         <v>1116</v>
       </c>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
       <c r="F50" s="67"/>
       <c r="G50" s="65"/>
       <c r="H50" s="65"/>
       <c r="I50" s="65"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="74"/>
+      <c r="A51" s="75"/>
       <c r="B51" s="45" t="s">
         <v>1060</v>
       </c>
-      <c r="C51" s="73" t="s">
+      <c r="C51" s="74" t="s">
         <v>1117</v>
       </c>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
       <c r="F51" s="67"/>
       <c r="G51" s="65"/>
       <c r="H51" s="65"/>
       <c r="I51" s="65"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="74"/>
+      <c r="A52" s="75"/>
       <c r="B52" s="45" t="s">
         <v>1118</v>
       </c>
-      <c r="C52" s="73" t="s">
+      <c r="C52" s="74" t="s">
         <v>1119</v>
       </c>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
       <c r="F52" s="67"/>
       <c r="G52" s="65"/>
       <c r="H52" s="65"/>
       <c r="I52" s="65"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="74"/>
+      <c r="A53" s="75"/>
       <c r="B53" s="45" t="s">
         <v>1056</v>
       </c>
-      <c r="C53" s="73" t="s">
+      <c r="C53" s="74" t="s">
         <v>1120</v>
       </c>
-      <c r="D53" s="73"/>
-      <c r="E53" s="73"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
       <c r="F53" s="67"/>
       <c r="G53" s="65"/>
       <c r="H53" s="65"/>
       <c r="I53" s="65"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="74" t="s">
+      <c r="A54" s="75" t="s">
         <v>1121</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1122</v>
       </c>
-      <c r="C54" s="73" t="s">
+      <c r="C54" s="74" t="s">
         <v>1123</v>
       </c>
-      <c r="D54" s="73"/>
-      <c r="E54" s="73"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
       <c r="F54" s="67"/>
       <c r="G54" s="65"/>
       <c r="H54" s="65"/>
       <c r="I54" s="65"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="74"/>
+      <c r="A55" s="75"/>
       <c r="B55" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="C55" s="73" t="s">
+      <c r="C55" s="74" t="s">
         <v>1125</v>
       </c>
-      <c r="D55" s="73"/>
-      <c r="E55" s="73"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
       <c r="F55" s="67"/>
       <c r="G55" s="65"/>
       <c r="H55" s="65"/>
       <c r="I55" s="65"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="74"/>
+      <c r="A56" s="75"/>
       <c r="B56" s="5" t="s">
         <v>1126</v>
       </c>
-      <c r="C56" s="73" t="s">
+      <c r="C56" s="74" t="s">
         <v>1127</v>
       </c>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
       <c r="F56" s="67"/>
       <c r="G56" s="65"/>
       <c r="H56" s="65"/>
       <c r="I56" s="65"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="74"/>
+      <c r="A57" s="75"/>
       <c r="B57" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="C57" s="73" t="s">
+      <c r="C57" s="74" t="s">
         <v>1129</v>
       </c>
-      <c r="D57" s="73"/>
-      <c r="E57" s="73"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
       <c r="F57" s="67"/>
       <c r="G57" s="65"/>
       <c r="H57" s="65"/>
       <c r="I57" s="65"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="74"/>
+      <c r="A58" s="75"/>
       <c r="B58" s="5" t="s">
         <v>1130</v>
       </c>
-      <c r="C58" s="73" t="s">
+      <c r="C58" s="74" t="s">
         <v>1131</v>
       </c>
-      <c r="D58" s="73"/>
-      <c r="E58" s="73"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
       <c r="F58" s="67"/>
       <c r="G58" s="65"/>
       <c r="H58" s="65"/>
@@ -27643,88 +27643,88 @@
       <c r="B59" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="C59" s="73" t="s">
+      <c r="C59" s="74" t="s">
         <v>1133</v>
       </c>
-      <c r="D59" s="73"/>
-      <c r="E59" s="73"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="74"/>
       <c r="F59" s="67"/>
       <c r="G59" s="65"/>
       <c r="H59" s="65"/>
       <c r="I59" s="65"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="74" t="s">
+      <c r="A60" s="75" t="s">
         <v>1134</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1135</v>
       </c>
-      <c r="C60" s="73" t="s">
+      <c r="C60" s="74" t="s">
         <v>1136</v>
       </c>
-      <c r="D60" s="73"/>
-      <c r="E60" s="73"/>
+      <c r="D60" s="74"/>
+      <c r="E60" s="74"/>
       <c r="F60" s="67"/>
       <c r="G60" s="65"/>
       <c r="H60" s="65"/>
       <c r="I60" s="65"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="74"/>
+      <c r="A61" s="75"/>
       <c r="B61" s="5" t="s">
         <v>1137</v>
       </c>
-      <c r="C61" s="73" t="s">
+      <c r="C61" s="74" t="s">
         <v>1138</v>
       </c>
-      <c r="D61" s="73"/>
-      <c r="E61" s="73"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
       <c r="F61" s="67"/>
       <c r="G61" s="65"/>
       <c r="H61" s="65"/>
       <c r="I61" s="65"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="74"/>
+      <c r="A62" s="75"/>
       <c r="B62" s="5" t="s">
         <v>1139</v>
       </c>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="74" t="s">
         <v>1140</v>
       </c>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
       <c r="F62" s="67"/>
       <c r="G62" s="65"/>
       <c r="H62" s="65"/>
       <c r="I62" s="65"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="74"/>
+      <c r="A63" s="75"/>
       <c r="B63" s="5" t="s">
         <v>1141</v>
       </c>
-      <c r="C63" s="73" t="s">
+      <c r="C63" s="74" t="s">
         <v>1142</v>
       </c>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
       <c r="F63" s="67"/>
       <c r="G63" s="65"/>
       <c r="H63" s="65"/>
       <c r="I63" s="65"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="74"/>
+      <c r="A64" s="75"/>
       <c r="B64" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C64" s="73" t="s">
+      <c r="C64" s="74" t="s">
         <v>1144</v>
       </c>
-      <c r="D64" s="73"/>
-      <c r="E64" s="73"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
       <c r="F64" s="67"/>
       <c r="G64" s="65"/>
       <c r="H64" s="65"/>
@@ -27732,30 +27732,72 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
@@ -27780,72 +27822,30 @@
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -28310,6 +28310,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C30:F30"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C20:F20"/>
@@ -28322,12 +28328,6 @@
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29108,13 +29108,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -29127,6 +29120,13 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29497,6 +29497,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
@@ -29504,18 +29516,6 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29982,6 +29982,19 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -29995,19 +30008,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -30984,33 +30984,29 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:I23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="C24:D24"/>
@@ -31024,29 +31020,33 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31531,6 +31531,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -31541,13 +31548,6 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -31955,11 +31955,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -31972,6 +31967,11 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -32003,15 +32003,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -32240,6 +32231,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -32252,14 +32252,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32274,6 +32266,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
:bug: Fix the typos in the names of some lab results
</commit_message>
<xml_diff>
--- a/CommonDataModel.xlsx
+++ b/CommonDataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doguk\OneDrive\Desktop\DT4H\Repositories\common-data-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C09CBEC-E42A-4E6A-AA3A-A9F874FD0D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E168337C-2B2D-4BC7-A51B-996CF7D9C983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="901" firstSheet="12" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="901" firstSheet="6" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="10" r:id="rId1"/>
@@ -7328,22 +7328,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8723,13 +8723,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -8740,6 +8733,13 @@
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9439,13 +9439,13 @@
         <v>462</v>
       </c>
       <c r="D39" s="66"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="71" t="s">
+      <c r="E39" s="69"/>
+      <c r="F39" s="72" t="s">
         <v>463</v>
       </c>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="42" t="s">
@@ -9454,11 +9454,11 @@
       <c r="B40" s="42" t="s">
         <v>465</v>
       </c>
-      <c r="C40" s="68" t="s">
+      <c r="C40" s="70" t="s">
         <v>466</v>
       </c>
-      <c r="D40" s="68"/>
-      <c r="E40" s="69"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="71"/>
       <c r="F40" s="67"/>
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
@@ -9471,11 +9471,11 @@
       <c r="B41" s="42" t="s">
         <v>468</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="C41" s="70" t="s">
         <v>469</v>
       </c>
-      <c r="D41" s="68"/>
-      <c r="E41" s="69"/>
+      <c r="D41" s="70"/>
+      <c r="E41" s="71"/>
       <c r="F41" s="67"/>
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
@@ -9488,11 +9488,11 @@
       <c r="B42" s="42" t="s">
         <v>471</v>
       </c>
-      <c r="C42" s="68" t="s">
+      <c r="C42" s="70" t="s">
         <v>472</v>
       </c>
-      <c r="D42" s="68"/>
-      <c r="E42" s="69"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="71"/>
       <c r="F42" s="67"/>
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
@@ -9505,11 +9505,11 @@
       <c r="B43" s="42" t="s">
         <v>474</v>
       </c>
-      <c r="C43" s="68" t="s">
+      <c r="C43" s="70" t="s">
         <v>2013</v>
       </c>
-      <c r="D43" s="68"/>
-      <c r="E43" s="69"/>
+      <c r="D43" s="70"/>
+      <c r="E43" s="71"/>
       <c r="F43" s="67"/>
       <c r="G43" s="65"/>
       <c r="H43" s="65"/>
@@ -9522,11 +9522,11 @@
       <c r="B44" s="42" t="s">
         <v>476</v>
       </c>
-      <c r="C44" s="68" t="s">
+      <c r="C44" s="70" t="s">
         <v>477</v>
       </c>
-      <c r="D44" s="68"/>
-      <c r="E44" s="69"/>
+      <c r="D44" s="70"/>
+      <c r="E44" s="71"/>
       <c r="F44" s="67"/>
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
@@ -9539,11 +9539,11 @@
       <c r="B45" s="42" t="s">
         <v>479</v>
       </c>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="70" t="s">
         <v>480</v>
       </c>
-      <c r="D45" s="68"/>
-      <c r="E45" s="69"/>
+      <c r="D45" s="70"/>
+      <c r="E45" s="71"/>
       <c r="F45" s="67"/>
       <c r="G45" s="65"/>
       <c r="H45" s="65"/>
@@ -9556,11 +9556,11 @@
       <c r="B46" s="42" t="s">
         <v>482</v>
       </c>
-      <c r="C46" s="68" t="s">
+      <c r="C46" s="70" t="s">
         <v>483</v>
       </c>
-      <c r="D46" s="68"/>
-      <c r="E46" s="69"/>
+      <c r="D46" s="70"/>
+      <c r="E46" s="71"/>
       <c r="F46" s="67"/>
       <c r="G46" s="65"/>
       <c r="H46" s="65"/>
@@ -9573,11 +9573,11 @@
       <c r="B47" s="42" t="s">
         <v>485</v>
       </c>
-      <c r="C47" s="68" t="s">
+      <c r="C47" s="70" t="s">
         <v>486</v>
       </c>
-      <c r="D47" s="68"/>
-      <c r="E47" s="69"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="71"/>
       <c r="F47" s="67"/>
       <c r="G47" s="65"/>
       <c r="H47" s="65"/>
@@ -9590,11 +9590,11 @@
       <c r="B48" s="42" t="s">
         <v>487</v>
       </c>
-      <c r="C48" s="68" t="s">
+      <c r="C48" s="70" t="s">
         <v>2014</v>
       </c>
-      <c r="D48" s="68"/>
-      <c r="E48" s="69"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="71"/>
       <c r="F48" s="67"/>
       <c r="G48" s="65"/>
       <c r="H48" s="65"/>
@@ -9607,11 +9607,11 @@
       <c r="B49" s="42" t="s">
         <v>489</v>
       </c>
-      <c r="C49" s="68" t="s">
+      <c r="C49" s="70" t="s">
         <v>490</v>
       </c>
-      <c r="D49" s="68"/>
-      <c r="E49" s="69"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="71"/>
       <c r="F49" s="67"/>
       <c r="G49" s="65"/>
       <c r="H49" s="65"/>
@@ -9624,11 +9624,11 @@
       <c r="B50" s="42" t="s">
         <v>492</v>
       </c>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="70" t="s">
         <v>493</v>
       </c>
-      <c r="D50" s="68"/>
-      <c r="E50" s="69"/>
+      <c r="D50" s="70"/>
+      <c r="E50" s="71"/>
       <c r="F50" s="67"/>
       <c r="G50" s="65"/>
       <c r="H50" s="65"/>
@@ -9641,11 +9641,11 @@
       <c r="B51" s="42" t="s">
         <v>495</v>
       </c>
-      <c r="C51" s="68" t="s">
+      <c r="C51" s="70" t="s">
         <v>496</v>
       </c>
-      <c r="D51" s="68"/>
-      <c r="E51" s="69"/>
+      <c r="D51" s="70"/>
+      <c r="E51" s="71"/>
       <c r="F51" s="67"/>
       <c r="G51" s="65"/>
       <c r="H51" s="65"/>
@@ -9658,11 +9658,11 @@
       <c r="B52" s="42" t="s">
         <v>498</v>
       </c>
-      <c r="C52" s="68" t="s">
+      <c r="C52" s="70" t="s">
         <v>499</v>
       </c>
-      <c r="D52" s="68"/>
-      <c r="E52" s="69"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="71"/>
       <c r="F52" s="67"/>
       <c r="G52" s="65"/>
       <c r="H52" s="65"/>
@@ -9675,11 +9675,11 @@
       <c r="B53" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="C53" s="68" t="s">
+      <c r="C53" s="70" t="s">
         <v>502</v>
       </c>
-      <c r="D53" s="68"/>
-      <c r="E53" s="69"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="71"/>
       <c r="F53" s="67"/>
       <c r="G53" s="65"/>
       <c r="H53" s="65"/>
@@ -9692,11 +9692,11 @@
       <c r="B54" s="42" t="s">
         <v>504</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="C54" s="70" t="s">
         <v>505</v>
       </c>
-      <c r="D54" s="68"/>
-      <c r="E54" s="69"/>
+      <c r="D54" s="70"/>
+      <c r="E54" s="71"/>
       <c r="F54" s="67"/>
       <c r="G54" s="65"/>
       <c r="H54" s="65"/>
@@ -9709,11 +9709,11 @@
       <c r="B55" s="42" t="s">
         <v>507</v>
       </c>
-      <c r="C55" s="68" t="s">
+      <c r="C55" s="70" t="s">
         <v>508</v>
       </c>
-      <c r="D55" s="68"/>
-      <c r="E55" s="69"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="71"/>
       <c r="F55" s="67"/>
       <c r="G55" s="65"/>
       <c r="H55" s="65"/>
@@ -9726,11 +9726,11 @@
       <c r="B56" s="42" t="s">
         <v>510</v>
       </c>
-      <c r="C56" s="68" t="s">
+      <c r="C56" s="70" t="s">
         <v>511</v>
       </c>
-      <c r="D56" s="68"/>
-      <c r="E56" s="69"/>
+      <c r="D56" s="70"/>
+      <c r="E56" s="71"/>
       <c r="F56" s="67"/>
       <c r="G56" s="65"/>
       <c r="H56" s="65"/>
@@ -9743,11 +9743,11 @@
       <c r="B57" s="42" t="s">
         <v>513</v>
       </c>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="70" t="s">
         <v>514</v>
       </c>
-      <c r="D57" s="68"/>
-      <c r="E57" s="69"/>
+      <c r="D57" s="70"/>
+      <c r="E57" s="71"/>
       <c r="F57" s="67"/>
       <c r="G57" s="65"/>
       <c r="H57" s="65"/>
@@ -9760,11 +9760,11 @@
       <c r="B58" s="42" t="s">
         <v>516</v>
       </c>
-      <c r="C58" s="68" t="s">
+      <c r="C58" s="70" t="s">
         <v>517</v>
       </c>
-      <c r="D58" s="68"/>
-      <c r="E58" s="69"/>
+      <c r="D58" s="70"/>
+      <c r="E58" s="71"/>
       <c r="F58" s="67"/>
       <c r="G58" s="65"/>
       <c r="H58" s="65"/>
@@ -9777,11 +9777,11 @@
       <c r="B59" s="42" t="s">
         <v>519</v>
       </c>
-      <c r="C59" s="68" t="s">
+      <c r="C59" s="70" t="s">
         <v>520</v>
       </c>
-      <c r="D59" s="68"/>
-      <c r="E59" s="69"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="71"/>
       <c r="F59" s="67"/>
       <c r="G59" s="65"/>
       <c r="H59" s="65"/>
@@ -9794,11 +9794,11 @@
       <c r="B60" s="42" t="s">
         <v>522</v>
       </c>
-      <c r="C60" s="68" t="s">
+      <c r="C60" s="70" t="s">
         <v>523</v>
       </c>
-      <c r="D60" s="68"/>
-      <c r="E60" s="69"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="71"/>
       <c r="F60" s="67"/>
       <c r="G60" s="65"/>
       <c r="H60" s="65"/>
@@ -9811,11 +9811,11 @@
       <c r="B61" s="42" t="s">
         <v>525</v>
       </c>
-      <c r="C61" s="68" t="s">
+      <c r="C61" s="70" t="s">
         <v>526</v>
       </c>
-      <c r="D61" s="68"/>
-      <c r="E61" s="69"/>
+      <c r="D61" s="70"/>
+      <c r="E61" s="71"/>
       <c r="F61" s="67"/>
       <c r="G61" s="65"/>
       <c r="H61" s="65"/>
@@ -9828,11 +9828,11 @@
       <c r="B62" s="42" t="s">
         <v>528</v>
       </c>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="70" t="s">
         <v>529</v>
       </c>
-      <c r="D62" s="68"/>
-      <c r="E62" s="69"/>
+      <c r="D62" s="70"/>
+      <c r="E62" s="71"/>
       <c r="F62" s="67"/>
       <c r="G62" s="65"/>
       <c r="H62" s="65"/>
@@ -9845,11 +9845,11 @@
       <c r="B63" s="42" t="s">
         <v>531</v>
       </c>
-      <c r="C63" s="68" t="s">
+      <c r="C63" s="70" t="s">
         <v>532</v>
       </c>
-      <c r="D63" s="68"/>
-      <c r="E63" s="69"/>
+      <c r="D63" s="70"/>
+      <c r="E63" s="71"/>
       <c r="F63" s="67"/>
       <c r="G63" s="65"/>
       <c r="H63" s="65"/>
@@ -9862,11 +9862,11 @@
       <c r="B64" s="42" t="s">
         <v>533</v>
       </c>
-      <c r="C64" s="68" t="s">
+      <c r="C64" s="70" t="s">
         <v>534</v>
       </c>
-      <c r="D64" s="68"/>
-      <c r="E64" s="69"/>
+      <c r="D64" s="70"/>
+      <c r="E64" s="71"/>
       <c r="F64" s="67"/>
       <c r="G64" s="65"/>
       <c r="H64" s="65"/>
@@ -9879,11 +9879,11 @@
       <c r="B65" s="42" t="s">
         <v>536</v>
       </c>
-      <c r="C65" s="68" t="s">
+      <c r="C65" s="70" t="s">
         <v>537</v>
       </c>
-      <c r="D65" s="68"/>
-      <c r="E65" s="69"/>
+      <c r="D65" s="70"/>
+      <c r="E65" s="71"/>
       <c r="F65" s="67"/>
       <c r="G65" s="65"/>
       <c r="H65" s="65"/>
@@ -9896,11 +9896,11 @@
       <c r="B66" s="42" t="s">
         <v>539</v>
       </c>
-      <c r="C66" s="68" t="s">
+      <c r="C66" s="70" t="s">
         <v>2015</v>
       </c>
-      <c r="D66" s="68"/>
-      <c r="E66" s="69"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="71"/>
       <c r="F66" s="67"/>
       <c r="G66" s="65"/>
       <c r="H66" s="65"/>
@@ -9913,11 +9913,11 @@
       <c r="B67" s="42" t="s">
         <v>541</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="70" t="s">
         <v>542</v>
       </c>
-      <c r="D67" s="68"/>
-      <c r="E67" s="69"/>
+      <c r="D67" s="70"/>
+      <c r="E67" s="71"/>
       <c r="F67" s="67"/>
       <c r="G67" s="65"/>
       <c r="H67" s="65"/>
@@ -9930,11 +9930,11 @@
       <c r="B68" s="42" t="s">
         <v>544</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="70" t="s">
         <v>545</v>
       </c>
-      <c r="D68" s="68"/>
-      <c r="E68" s="69"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="71"/>
       <c r="F68" s="67"/>
       <c r="G68" s="65"/>
       <c r="H68" s="65"/>
@@ -9947,11 +9947,11 @@
       <c r="B69" s="42" t="s">
         <v>547</v>
       </c>
-      <c r="C69" s="68" t="s">
+      <c r="C69" s="70" t="s">
         <v>548</v>
       </c>
-      <c r="D69" s="68"/>
-      <c r="E69" s="69"/>
+      <c r="D69" s="70"/>
+      <c r="E69" s="71"/>
       <c r="F69" s="67"/>
       <c r="G69" s="65"/>
       <c r="H69" s="65"/>
@@ -9964,11 +9964,11 @@
       <c r="B70" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="C70" s="68" t="s">
+      <c r="C70" s="70" t="s">
         <v>551</v>
       </c>
-      <c r="D70" s="68"/>
-      <c r="E70" s="69"/>
+      <c r="D70" s="70"/>
+      <c r="E70" s="71"/>
       <c r="F70" s="67"/>
       <c r="G70" s="65"/>
       <c r="H70" s="65"/>
@@ -9981,11 +9981,11 @@
       <c r="B71" s="42" t="s">
         <v>553</v>
       </c>
-      <c r="C71" s="68" t="s">
+      <c r="C71" s="70" t="s">
         <v>554</v>
       </c>
-      <c r="D71" s="68"/>
-      <c r="E71" s="69"/>
+      <c r="D71" s="70"/>
+      <c r="E71" s="71"/>
       <c r="F71" s="67"/>
       <c r="G71" s="65"/>
       <c r="H71" s="65"/>
@@ -9998,11 +9998,11 @@
       <c r="B72" s="42" t="s">
         <v>556</v>
       </c>
-      <c r="C72" s="68" t="s">
+      <c r="C72" s="70" t="s">
         <v>557</v>
       </c>
-      <c r="D72" s="68"/>
-      <c r="E72" s="69"/>
+      <c r="D72" s="70"/>
+      <c r="E72" s="71"/>
       <c r="F72" s="67"/>
       <c r="G72" s="65"/>
       <c r="H72" s="65"/>
@@ -10015,11 +10015,11 @@
       <c r="B73" s="42" t="s">
         <v>559</v>
       </c>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="70" t="s">
         <v>560</v>
       </c>
-      <c r="D73" s="68"/>
-      <c r="E73" s="69"/>
+      <c r="D73" s="70"/>
+      <c r="E73" s="71"/>
       <c r="F73" s="67"/>
       <c r="G73" s="65"/>
       <c r="H73" s="65"/>
@@ -10032,11 +10032,11 @@
       <c r="B74" s="42" t="s">
         <v>562</v>
       </c>
-      <c r="C74" s="68" t="s">
+      <c r="C74" s="70" t="s">
         <v>563</v>
       </c>
-      <c r="D74" s="68"/>
-      <c r="E74" s="69"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="71"/>
       <c r="F74" s="67"/>
       <c r="G74" s="65"/>
       <c r="H74" s="65"/>
@@ -10049,11 +10049,11 @@
       <c r="B75" s="42" t="s">
         <v>565</v>
       </c>
-      <c r="C75" s="68" t="s">
+      <c r="C75" s="70" t="s">
         <v>566</v>
       </c>
-      <c r="D75" s="68"/>
-      <c r="E75" s="69"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="71"/>
       <c r="F75" s="67"/>
       <c r="G75" s="65"/>
       <c r="H75" s="65"/>
@@ -10066,11 +10066,11 @@
       <c r="B76" s="42" t="s">
         <v>568</v>
       </c>
-      <c r="C76" s="68" t="s">
+      <c r="C76" s="70" t="s">
         <v>569</v>
       </c>
-      <c r="D76" s="68"/>
-      <c r="E76" s="69"/>
+      <c r="D76" s="70"/>
+      <c r="E76" s="71"/>
       <c r="F76" s="67"/>
       <c r="G76" s="65"/>
       <c r="H76" s="65"/>
@@ -10083,11 +10083,11 @@
       <c r="B77" s="42" t="s">
         <v>571</v>
       </c>
-      <c r="C77" s="68" t="s">
+      <c r="C77" s="70" t="s">
         <v>572</v>
       </c>
-      <c r="D77" s="68"/>
-      <c r="E77" s="69"/>
+      <c r="D77" s="70"/>
+      <c r="E77" s="71"/>
       <c r="F77" s="67"/>
       <c r="G77" s="65"/>
       <c r="H77" s="65"/>
@@ -10100,11 +10100,11 @@
       <c r="B78" s="42" t="s">
         <v>574</v>
       </c>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="70" t="s">
         <v>575</v>
       </c>
-      <c r="D78" s="68"/>
-      <c r="E78" s="69"/>
+      <c r="D78" s="70"/>
+      <c r="E78" s="71"/>
       <c r="F78" s="67"/>
       <c r="G78" s="65"/>
       <c r="H78" s="65"/>
@@ -10117,11 +10117,11 @@
       <c r="B79" s="42" t="s">
         <v>577</v>
       </c>
-      <c r="C79" s="68" t="s">
+      <c r="C79" s="70" t="s">
         <v>578</v>
       </c>
-      <c r="D79" s="68"/>
-      <c r="E79" s="69"/>
+      <c r="D79" s="70"/>
+      <c r="E79" s="71"/>
       <c r="F79" s="67"/>
       <c r="G79" s="65"/>
       <c r="H79" s="65"/>
@@ -10134,11 +10134,11 @@
       <c r="B80" s="42" t="s">
         <v>580</v>
       </c>
-      <c r="C80" s="68" t="s">
+      <c r="C80" s="70" t="s">
         <v>581</v>
       </c>
-      <c r="D80" s="68"/>
-      <c r="E80" s="69"/>
+      <c r="D80" s="70"/>
+      <c r="E80" s="71"/>
       <c r="F80" s="67"/>
       <c r="G80" s="65"/>
       <c r="H80" s="65"/>
@@ -10151,11 +10151,11 @@
       <c r="B81" s="42" t="s">
         <v>583</v>
       </c>
-      <c r="C81" s="68" t="s">
+      <c r="C81" s="70" t="s">
         <v>584</v>
       </c>
-      <c r="D81" s="68"/>
-      <c r="E81" s="69"/>
+      <c r="D81" s="70"/>
+      <c r="E81" s="71"/>
       <c r="F81" s="67"/>
       <c r="G81" s="65"/>
       <c r="H81" s="65"/>
@@ -10168,11 +10168,11 @@
       <c r="B82" t="s">
         <v>2020</v>
       </c>
-      <c r="C82" s="72" t="s">
+      <c r="C82" s="68" t="s">
         <v>2017</v>
       </c>
-      <c r="D82" s="72"/>
-      <c r="E82" s="72"/>
+      <c r="D82" s="68"/>
+      <c r="E82" s="68"/>
       <c r="F82" s="67"/>
       <c r="G82" s="65"/>
       <c r="H82" s="65"/>
@@ -10185,11 +10185,11 @@
       <c r="B83" t="s">
         <v>2021</v>
       </c>
-      <c r="C83" s="72" t="s">
+      <c r="C83" s="68" t="s">
         <v>2019</v>
       </c>
-      <c r="D83" s="72"/>
-      <c r="E83" s="72"/>
+      <c r="D83" s="68"/>
+      <c r="E83" s="68"/>
       <c r="F83" s="67"/>
       <c r="G83" s="65"/>
       <c r="H83" s="65"/>
@@ -10197,6 +10197,103 @@
     </row>
   </sheetData>
   <mergeCells count="121">
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
     <mergeCell ref="C82:E82"/>
     <mergeCell ref="C83:E83"/>
     <mergeCell ref="F82:I82"/>
@@ -10221,103 +10318,6 @@
     <mergeCell ref="F34:I34"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C80:E80"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="F74:I74"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11182,41 +11182,14 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -11233,14 +11206,41 @@
     <mergeCell ref="F31:I31"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E41" xr:uid="{14C408A9-075A-4B77-84C3-9F689D082B68}">
@@ -12452,19 +12452,29 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="G32:J32"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
@@ -12477,29 +12487,19 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="G31:J31"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:F21" xr:uid="{7FAB08B6-9907-44B4-A82A-4A3E200D36A8}">
@@ -12539,8 +12539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BB695D-4821-4052-8E37-D71854C5F317}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12946,7 +12946,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="B21" t="s">
         <v>695</v>
@@ -12967,7 +12967,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B22" t="s">
         <v>699</v>
@@ -13811,23 +13811,25 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
     <mergeCell ref="F55:I55"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="F35:I35"/>
@@ -13841,25 +13843,23 @@
     <mergeCell ref="F49:I49"/>
     <mergeCell ref="F50:I50"/>
     <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="1">
@@ -15449,7 +15449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF00AD05-AD0A-4301-B0FD-56AA1951174D}">
   <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
@@ -18438,15 +18438,96 @@
   </sheetData>
   <dataConsolidate link="1"/>
   <mergeCells count="111">
-    <mergeCell ref="H150:K150"/>
-    <mergeCell ref="H151:K151"/>
-    <mergeCell ref="H152:K152"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="H149:K149"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H62:K62"/>
+    <mergeCell ref="H63:K63"/>
+    <mergeCell ref="H64:K64"/>
+    <mergeCell ref="H65:K65"/>
+    <mergeCell ref="H66:K66"/>
+    <mergeCell ref="H68:K68"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="H58:K58"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="H61:K61"/>
+    <mergeCell ref="H77:K77"/>
+    <mergeCell ref="H78:K78"/>
+    <mergeCell ref="H79:K79"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="H82:K82"/>
+    <mergeCell ref="H69:K69"/>
+    <mergeCell ref="H70:K70"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="H75:K75"/>
+    <mergeCell ref="H76:K76"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="H90:K90"/>
+    <mergeCell ref="H91:K91"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="H83:K83"/>
+    <mergeCell ref="H84:K84"/>
+    <mergeCell ref="H85:K85"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="H87:K87"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H101:K101"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="H103:K103"/>
+    <mergeCell ref="H104:K104"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="H107:K107"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="H96:K96"/>
+    <mergeCell ref="H97:K97"/>
+    <mergeCell ref="H98:K98"/>
+    <mergeCell ref="H99:K99"/>
+    <mergeCell ref="H100:K100"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H116:K116"/>
+    <mergeCell ref="H117:K117"/>
+    <mergeCell ref="H118:K118"/>
+    <mergeCell ref="H119:K119"/>
+    <mergeCell ref="H108:K108"/>
+    <mergeCell ref="H109:K109"/>
+    <mergeCell ref="H110:K110"/>
+    <mergeCell ref="H111:K111"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H126:K126"/>
+    <mergeCell ref="H127:K127"/>
+    <mergeCell ref="H128:K128"/>
+    <mergeCell ref="H129:K129"/>
+    <mergeCell ref="H130:K130"/>
+    <mergeCell ref="H131:K131"/>
+    <mergeCell ref="H120:K120"/>
+    <mergeCell ref="H121:K121"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:K123"/>
+    <mergeCell ref="H124:K124"/>
+    <mergeCell ref="H125:K125"/>
     <mergeCell ref="H138:K138"/>
     <mergeCell ref="H139:K139"/>
     <mergeCell ref="H140:K140"/>
@@ -18459,96 +18540,15 @@
     <mergeCell ref="H135:K135"/>
     <mergeCell ref="H136:K136"/>
     <mergeCell ref="H137:K137"/>
-    <mergeCell ref="H126:K126"/>
-    <mergeCell ref="H127:K127"/>
-    <mergeCell ref="H128:K128"/>
-    <mergeCell ref="H129:K129"/>
-    <mergeCell ref="H130:K130"/>
-    <mergeCell ref="H131:K131"/>
-    <mergeCell ref="H120:K120"/>
-    <mergeCell ref="H121:K121"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:K123"/>
-    <mergeCell ref="H124:K124"/>
-    <mergeCell ref="H125:K125"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H116:K116"/>
-    <mergeCell ref="H117:K117"/>
-    <mergeCell ref="H118:K118"/>
-    <mergeCell ref="H119:K119"/>
-    <mergeCell ref="H108:K108"/>
-    <mergeCell ref="H109:K109"/>
-    <mergeCell ref="H110:K110"/>
-    <mergeCell ref="H111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H101:K101"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="H103:K103"/>
-    <mergeCell ref="H104:K104"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="H107:K107"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="H96:K96"/>
-    <mergeCell ref="H97:K97"/>
-    <mergeCell ref="H98:K98"/>
-    <mergeCell ref="H99:K99"/>
-    <mergeCell ref="H100:K100"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="H90:K90"/>
-    <mergeCell ref="H91:K91"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="H83:K83"/>
-    <mergeCell ref="H84:K84"/>
-    <mergeCell ref="H85:K85"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="H87:K87"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H77:K77"/>
-    <mergeCell ref="H78:K78"/>
-    <mergeCell ref="H79:K79"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="H82:K82"/>
-    <mergeCell ref="H69:K69"/>
-    <mergeCell ref="H70:K70"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="H75:K75"/>
-    <mergeCell ref="H76:K76"/>
-    <mergeCell ref="H62:K62"/>
-    <mergeCell ref="H63:K63"/>
-    <mergeCell ref="H64:K64"/>
-    <mergeCell ref="H65:K65"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="H68:K68"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="H58:K58"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="H61:K61"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H150:K150"/>
+    <mergeCell ref="H151:K151"/>
+    <mergeCell ref="H152:K152"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="H149:K149"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21128,6 +21128,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="F113:I113"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
     <mergeCell ref="F109:I109"/>
     <mergeCell ref="F110:I110"/>
     <mergeCell ref="F111:I111"/>
@@ -21136,21 +21151,6 @@
     <mergeCell ref="C110:D110"/>
     <mergeCell ref="C111:D111"/>
     <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="F113:I113"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -21970,6 +21970,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="H45:K45"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H53:K53"/>
     <mergeCell ref="H44:K44"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="H14:K14"/>
@@ -21982,15 +21991,6 @@
     <mergeCell ref="H41:K41"/>
     <mergeCell ref="H42:K42"/>
     <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H53:K53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22340,14 +22340,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H22:K22"/>
     <mergeCell ref="H33:K33"/>
     <mergeCell ref="H34:K34"/>
     <mergeCell ref="H35:K35"/>
@@ -22357,6 +22349,14 @@
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="H31:K31"/>
     <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -22707,6 +22707,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H17:K17"/>
@@ -22719,11 +22724,6 @@
     <mergeCell ref="H24:K24"/>
     <mergeCell ref="H25:K25"/>
     <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -23794,10 +23794,10 @@
       <c r="B44" s="48" t="s">
         <v>1164</v>
       </c>
-      <c r="C44" s="72" t="s">
+      <c r="C44" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D44" s="72"/>
+      <c r="D44" s="68"/>
       <c r="E44" s="5" t="s">
         <v>1165</v>
       </c>
@@ -23811,10 +23811,10 @@
       <c r="B45" s="48" t="s">
         <v>1166</v>
       </c>
-      <c r="C45" s="72" t="s">
+      <c r="C45" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D45" s="72"/>
+      <c r="D45" s="68"/>
       <c r="E45" s="5" t="s">
         <v>1167</v>
       </c>
@@ -23828,10 +23828,10 @@
       <c r="B46" s="48" t="s">
         <v>1168</v>
       </c>
-      <c r="C46" s="72" t="s">
+      <c r="C46" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D46" s="72"/>
+      <c r="D46" s="68"/>
       <c r="E46" s="5" t="s">
         <v>1169</v>
       </c>
@@ -23845,10 +23845,10 @@
       <c r="B47" s="48" t="s">
         <v>1170</v>
       </c>
-      <c r="C47" s="72" t="s">
+      <c r="C47" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D47" s="72"/>
+      <c r="D47" s="68"/>
       <c r="E47" s="5" t="s">
         <v>1171</v>
       </c>
@@ -23862,10 +23862,10 @@
       <c r="B48" s="48" t="s">
         <v>1172</v>
       </c>
-      <c r="C48" s="72" t="s">
+      <c r="C48" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D48" s="72"/>
+      <c r="D48" s="68"/>
       <c r="E48" s="5" t="s">
         <v>1173</v>
       </c>
@@ -23879,10 +23879,10 @@
       <c r="B49" s="48" t="s">
         <v>1174</v>
       </c>
-      <c r="C49" s="72" t="s">
+      <c r="C49" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D49" s="72"/>
+      <c r="D49" s="68"/>
       <c r="E49" s="5" t="s">
         <v>1175</v>
       </c>
@@ -23896,10 +23896,10 @@
       <c r="B50" s="48" t="s">
         <v>1176</v>
       </c>
-      <c r="C50" s="72" t="s">
+      <c r="C50" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D50" s="72"/>
+      <c r="D50" s="68"/>
       <c r="E50" s="5" t="s">
         <v>1177</v>
       </c>
@@ -23913,10 +23913,10 @@
       <c r="B51" s="48" t="s">
         <v>1178</v>
       </c>
-      <c r="C51" s="72" t="s">
+      <c r="C51" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D51" s="72"/>
+      <c r="D51" s="68"/>
       <c r="E51" s="5" t="s">
         <v>1179</v>
       </c>
@@ -23930,10 +23930,10 @@
       <c r="B52" s="48" t="s">
         <v>1180</v>
       </c>
-      <c r="C52" s="72" t="s">
+      <c r="C52" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D52" s="72"/>
+      <c r="D52" s="68"/>
       <c r="E52" s="5" t="s">
         <v>1181</v>
       </c>
@@ -23947,10 +23947,10 @@
       <c r="B53" s="48" t="s">
         <v>1182</v>
       </c>
-      <c r="C53" s="72" t="s">
+      <c r="C53" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D53" s="72"/>
+      <c r="D53" s="68"/>
       <c r="E53" s="5" t="s">
         <v>1183</v>
       </c>
@@ -23964,10 +23964,10 @@
       <c r="B54" s="48" t="s">
         <v>1184</v>
       </c>
-      <c r="C54" s="72" t="s">
+      <c r="C54" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D54" s="72"/>
+      <c r="D54" s="68"/>
       <c r="E54" s="5" t="s">
         <v>1185</v>
       </c>
@@ -23981,10 +23981,10 @@
       <c r="B55" s="48" t="s">
         <v>1186</v>
       </c>
-      <c r="C55" s="72" t="s">
+      <c r="C55" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D55" s="72"/>
+      <c r="D55" s="68"/>
       <c r="E55" s="5" t="s">
         <v>1187</v>
       </c>
@@ -23998,10 +23998,10 @@
       <c r="B56" s="48" t="s">
         <v>1188</v>
       </c>
-      <c r="C56" s="72" t="s">
+      <c r="C56" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D56" s="72"/>
+      <c r="D56" s="68"/>
       <c r="E56" s="5" t="s">
         <v>1189</v>
       </c>
@@ -24015,10 +24015,10 @@
       <c r="B57" s="48" t="s">
         <v>1190</v>
       </c>
-      <c r="C57" s="72" t="s">
+      <c r="C57" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D57" s="72"/>
+      <c r="D57" s="68"/>
       <c r="E57" s="5" t="s">
         <v>1191</v>
       </c>
@@ -24032,10 +24032,10 @@
       <c r="B58" s="48" t="s">
         <v>1192</v>
       </c>
-      <c r="C58" s="72" t="s">
+      <c r="C58" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D58" s="72"/>
+      <c r="D58" s="68"/>
       <c r="E58" s="5" t="s">
         <v>1193</v>
       </c>
@@ -24049,10 +24049,10 @@
       <c r="B59" s="48" t="s">
         <v>1194</v>
       </c>
-      <c r="C59" s="72" t="s">
+      <c r="C59" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D59" s="72"/>
+      <c r="D59" s="68"/>
       <c r="E59" s="5" t="s">
         <v>1195</v>
       </c>
@@ -24066,10 +24066,10 @@
       <c r="B60" s="48" t="s">
         <v>1196</v>
       </c>
-      <c r="C60" s="72" t="s">
+      <c r="C60" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D60" s="72"/>
+      <c r="D60" s="68"/>
       <c r="E60" s="5" t="s">
         <v>1197</v>
       </c>
@@ -24083,10 +24083,10 @@
       <c r="B61" s="48" t="s">
         <v>1198</v>
       </c>
-      <c r="C61" s="72" t="s">
+      <c r="C61" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D61" s="72"/>
+      <c r="D61" s="68"/>
       <c r="E61" s="5" t="s">
         <v>1199</v>
       </c>
@@ -24100,10 +24100,10 @@
       <c r="B62" s="48" t="s">
         <v>1200</v>
       </c>
-      <c r="C62" s="72" t="s">
+      <c r="C62" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D62" s="72"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="5" t="s">
         <v>1201</v>
       </c>
@@ -24117,10 +24117,10 @@
       <c r="B63" s="48" t="s">
         <v>1202</v>
       </c>
-      <c r="C63" s="72" t="s">
+      <c r="C63" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D63" s="72"/>
+      <c r="D63" s="68"/>
       <c r="E63" s="5" t="s">
         <v>1203</v>
       </c>
@@ -24134,10 +24134,10 @@
       <c r="B64" s="48" t="s">
         <v>1204</v>
       </c>
-      <c r="C64" s="72" t="s">
+      <c r="C64" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D64" s="72"/>
+      <c r="D64" s="68"/>
       <c r="E64" s="5" t="s">
         <v>1205</v>
       </c>
@@ -24151,10 +24151,10 @@
       <c r="B65" s="48" t="s">
         <v>1206</v>
       </c>
-      <c r="C65" s="72" t="s">
+      <c r="C65" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D65" s="72"/>
+      <c r="D65" s="68"/>
       <c r="E65" s="5" t="s">
         <v>1207</v>
       </c>
@@ -24168,10 +24168,10 @@
       <c r="B66" s="48" t="s">
         <v>1208</v>
       </c>
-      <c r="C66" s="72" t="s">
+      <c r="C66" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D66" s="72"/>
+      <c r="D66" s="68"/>
       <c r="E66" s="5" t="s">
         <v>1209</v>
       </c>
@@ -24185,10 +24185,10 @@
       <c r="B67" s="48" t="s">
         <v>1210</v>
       </c>
-      <c r="C67" s="72" t="s">
+      <c r="C67" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D67" s="72"/>
+      <c r="D67" s="68"/>
       <c r="E67" s="5" t="s">
         <v>1211</v>
       </c>
@@ -24202,10 +24202,10 @@
       <c r="B68" s="48" t="s">
         <v>1212</v>
       </c>
-      <c r="C68" s="72" t="s">
+      <c r="C68" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D68" s="72"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="5" t="s">
         <v>1213</v>
       </c>
@@ -24219,10 +24219,10 @@
       <c r="B69" s="48" t="s">
         <v>1214</v>
       </c>
-      <c r="C69" s="72" t="s">
+      <c r="C69" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D69" s="72"/>
+      <c r="D69" s="68"/>
       <c r="E69" s="5" t="s">
         <v>1215</v>
       </c>
@@ -24236,10 +24236,10 @@
       <c r="B70" s="48" t="s">
         <v>1216</v>
       </c>
-      <c r="C70" s="72" t="s">
+      <c r="C70" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D70" s="72"/>
+      <c r="D70" s="68"/>
       <c r="E70" s="5" t="s">
         <v>1217</v>
       </c>
@@ -24253,10 +24253,10 @@
       <c r="B71" s="48" t="s">
         <v>1218</v>
       </c>
-      <c r="C71" s="72" t="s">
+      <c r="C71" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D71" s="72"/>
+      <c r="D71" s="68"/>
       <c r="E71" s="5" t="s">
         <v>1219</v>
       </c>
@@ -24270,10 +24270,10 @@
       <c r="B72" s="48" t="s">
         <v>1220</v>
       </c>
-      <c r="C72" s="72" t="s">
+      <c r="C72" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D72" s="72"/>
+      <c r="D72" s="68"/>
       <c r="E72" s="5" t="s">
         <v>1221</v>
       </c>
@@ -24287,10 +24287,10 @@
       <c r="B73" s="48" t="s">
         <v>1222</v>
       </c>
-      <c r="C73" s="72" t="s">
+      <c r="C73" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D73" s="72"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="5" t="s">
         <v>1223</v>
       </c>
@@ -24304,10 +24304,10 @@
       <c r="B74" s="48" t="s">
         <v>1224</v>
       </c>
-      <c r="C74" s="72" t="s">
+      <c r="C74" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D74" s="72"/>
+      <c r="D74" s="68"/>
       <c r="E74" s="5" t="s">
         <v>1225</v>
       </c>
@@ -24321,10 +24321,10 @@
       <c r="B75" s="48" t="s">
         <v>1226</v>
       </c>
-      <c r="C75" s="72" t="s">
+      <c r="C75" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D75" s="72"/>
+      <c r="D75" s="68"/>
       <c r="E75" s="5" t="s">
         <v>1227</v>
       </c>
@@ -24338,10 +24338,10 @@
       <c r="B76" s="48" t="s">
         <v>1228</v>
       </c>
-      <c r="C76" s="72" t="s">
+      <c r="C76" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D76" s="72"/>
+      <c r="D76" s="68"/>
       <c r="E76" s="5" t="s">
         <v>1229</v>
       </c>
@@ -24355,10 +24355,10 @@
       <c r="B77" s="48" t="s">
         <v>1230</v>
       </c>
-      <c r="C77" s="72" t="s">
+      <c r="C77" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D77" s="72"/>
+      <c r="D77" s="68"/>
       <c r="E77" s="5" t="s">
         <v>1231</v>
       </c>
@@ -24372,10 +24372,10 @@
       <c r="B78" s="48" t="s">
         <v>1232</v>
       </c>
-      <c r="C78" s="72" t="s">
+      <c r="C78" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D78" s="72"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="5" t="s">
         <v>1233</v>
       </c>
@@ -24389,10 +24389,10 @@
       <c r="B79" s="48" t="s">
         <v>1234</v>
       </c>
-      <c r="C79" s="72" t="s">
+      <c r="C79" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D79" s="72"/>
+      <c r="D79" s="68"/>
       <c r="E79" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24406,10 +24406,10 @@
       <c r="B80" s="48" t="s">
         <v>1236</v>
       </c>
-      <c r="C80" s="72" t="s">
+      <c r="C80" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D80" s="72"/>
+      <c r="D80" s="68"/>
       <c r="E80" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24423,10 +24423,10 @@
       <c r="B81" s="48" t="s">
         <v>1238</v>
       </c>
-      <c r="C81" s="72" t="s">
+      <c r="C81" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D81" s="72"/>
+      <c r="D81" s="68"/>
       <c r="E81" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24440,10 +24440,10 @@
       <c r="B82" s="48" t="s">
         <v>1240</v>
       </c>
-      <c r="C82" s="72" t="s">
+      <c r="C82" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D82" s="72"/>
+      <c r="D82" s="68"/>
       <c r="E82" s="5" t="s">
         <v>1241</v>
       </c>
@@ -24457,10 +24457,10 @@
       <c r="B83" s="48" t="s">
         <v>1269</v>
       </c>
-      <c r="C83" s="72" t="s">
+      <c r="C83" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D83" s="72"/>
+      <c r="D83" s="68"/>
       <c r="E83" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24474,10 +24474,10 @@
       <c r="B84" s="48" t="s">
         <v>1270</v>
       </c>
-      <c r="C84" s="72" t="s">
+      <c r="C84" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D84" s="72"/>
+      <c r="D84" s="68"/>
       <c r="E84" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24491,10 +24491,10 @@
       <c r="B85" s="48" t="s">
         <v>1271</v>
       </c>
-      <c r="C85" s="72" t="s">
+      <c r="C85" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D85" s="72"/>
+      <c r="D85" s="68"/>
       <c r="E85" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24508,10 +24508,10 @@
       <c r="B86" s="48" t="s">
         <v>1272</v>
       </c>
-      <c r="C86" s="72" t="s">
+      <c r="C86" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D86" s="72"/>
+      <c r="D86" s="68"/>
       <c r="E86" s="5" t="s">
         <v>1242</v>
       </c>
@@ -24525,10 +24525,10 @@
       <c r="B87" s="48" t="s">
         <v>1243</v>
       </c>
-      <c r="C87" s="72" t="s">
+      <c r="C87" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D87" s="72"/>
+      <c r="D87" s="68"/>
       <c r="E87" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24542,10 +24542,10 @@
       <c r="B88" s="48" t="s">
         <v>1244</v>
       </c>
-      <c r="C88" s="72" t="s">
+      <c r="C88" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D88" s="72"/>
+      <c r="D88" s="68"/>
       <c r="E88" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24559,10 +24559,10 @@
       <c r="B89" s="48" t="s">
         <v>1245</v>
       </c>
-      <c r="C89" s="72" t="s">
+      <c r="C89" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D89" s="72"/>
+      <c r="D89" s="68"/>
       <c r="E89" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24576,10 +24576,10 @@
       <c r="B90" s="48" t="s">
         <v>1246</v>
       </c>
-      <c r="C90" s="72" t="s">
+      <c r="C90" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D90" s="72"/>
+      <c r="D90" s="68"/>
       <c r="E90" s="5" t="s">
         <v>1242</v>
       </c>
@@ -24593,10 +24593,10 @@
       <c r="B91" s="48" t="s">
         <v>1273</v>
       </c>
-      <c r="C91" s="72" t="s">
+      <c r="C91" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D91" s="72"/>
+      <c r="D91" s="68"/>
       <c r="E91" s="5" t="s">
         <v>1235</v>
       </c>
@@ -24610,10 +24610,10 @@
       <c r="B92" s="48" t="s">
         <v>1274</v>
       </c>
-      <c r="C92" s="72" t="s">
+      <c r="C92" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D92" s="72"/>
+      <c r="D92" s="68"/>
       <c r="E92" s="5" t="s">
         <v>1237</v>
       </c>
@@ -24627,10 +24627,10 @@
       <c r="B93" s="48" t="s">
         <v>1275</v>
       </c>
-      <c r="C93" s="72" t="s">
+      <c r="C93" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D93" s="72"/>
+      <c r="D93" s="68"/>
       <c r="E93" s="5" t="s">
         <v>1239</v>
       </c>
@@ -24644,10 +24644,10 @@
       <c r="B94" s="48" t="s">
         <v>1276</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C94" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D94" s="72"/>
+      <c r="D94" s="68"/>
       <c r="E94" s="5" t="s">
         <v>1242</v>
       </c>
@@ -24661,10 +24661,10 @@
       <c r="B95" s="48" t="s">
         <v>1277</v>
       </c>
-      <c r="C95" s="72" t="s">
+      <c r="C95" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D95" s="72"/>
+      <c r="D95" s="68"/>
       <c r="E95" s="5" t="s">
         <v>1247</v>
       </c>
@@ -24678,10 +24678,10 @@
       <c r="B96" s="48" t="s">
         <v>1248</v>
       </c>
-      <c r="C96" s="72" t="s">
+      <c r="C96" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D96" s="72"/>
+      <c r="D96" s="68"/>
       <c r="E96" s="5" t="s">
         <v>1249</v>
       </c>
@@ -24695,10 +24695,10 @@
       <c r="B97" s="48" t="s">
         <v>1250</v>
       </c>
-      <c r="C97" s="72" t="s">
+      <c r="C97" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D97" s="72"/>
+      <c r="D97" s="68"/>
       <c r="E97" s="5" t="s">
         <v>1251</v>
       </c>
@@ -24712,10 +24712,10 @@
       <c r="B98" s="48" t="s">
         <v>1252</v>
       </c>
-      <c r="C98" s="72" t="s">
+      <c r="C98" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D98" s="72"/>
+      <c r="D98" s="68"/>
       <c r="E98" s="5" t="s">
         <v>1253</v>
       </c>
@@ -24729,10 +24729,10 @@
       <c r="B99" s="48" t="s">
         <v>1254</v>
       </c>
-      <c r="C99" s="72" t="s">
+      <c r="C99" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D99" s="72"/>
+      <c r="D99" s="68"/>
       <c r="E99" s="5" t="s">
         <v>1255</v>
       </c>
@@ -24746,10 +24746,10 @@
       <c r="B100" s="48" t="s">
         <v>1256</v>
       </c>
-      <c r="C100" s="72" t="s">
+      <c r="C100" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D100" s="72"/>
+      <c r="D100" s="68"/>
       <c r="E100" s="5" t="s">
         <v>1257</v>
       </c>
@@ -24763,10 +24763,10 @@
       <c r="B101" s="48" t="s">
         <v>1258</v>
       </c>
-      <c r="C101" s="72" t="s">
+      <c r="C101" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D101" s="72"/>
+      <c r="D101" s="68"/>
       <c r="E101" s="5" t="s">
         <v>1259</v>
       </c>
@@ -24780,10 +24780,10 @@
       <c r="B102" s="48" t="s">
         <v>1260</v>
       </c>
-      <c r="C102" s="72" t="s">
+      <c r="C102" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D102" s="72"/>
+      <c r="D102" s="68"/>
       <c r="E102" s="5" t="s">
         <v>1253</v>
       </c>
@@ -24797,10 +24797,10 @@
       <c r="B103" s="48" t="s">
         <v>1261</v>
       </c>
-      <c r="C103" s="72" t="s">
+      <c r="C103" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D103" s="72"/>
+      <c r="D103" s="68"/>
       <c r="E103" s="5" t="s">
         <v>1255</v>
       </c>
@@ -24814,10 +24814,10 @@
       <c r="B104" s="48" t="s">
         <v>1262</v>
       </c>
-      <c r="C104" s="72" t="s">
+      <c r="C104" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D104" s="72"/>
+      <c r="D104" s="68"/>
       <c r="E104" s="5" t="s">
         <v>1257</v>
       </c>
@@ -24831,10 +24831,10 @@
       <c r="B105" s="48" t="s">
         <v>1263</v>
       </c>
-      <c r="C105" s="72" t="s">
+      <c r="C105" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D105" s="72"/>
+      <c r="D105" s="68"/>
       <c r="E105" s="5" t="s">
         <v>1259</v>
       </c>
@@ -24848,10 +24848,10 @@
       <c r="B106" s="48" t="s">
         <v>1264</v>
       </c>
-      <c r="C106" s="72" t="s">
+      <c r="C106" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D106" s="72"/>
+      <c r="D106" s="68"/>
       <c r="E106" s="5" t="s">
         <v>1265</v>
       </c>
@@ -24865,10 +24865,10 @@
       <c r="B107" s="48" t="s">
         <v>1266</v>
       </c>
-      <c r="C107" s="72" t="s">
+      <c r="C107" s="68" t="s">
         <v>1278</v>
       </c>
-      <c r="D107" s="72"/>
+      <c r="D107" s="68"/>
       <c r="E107" s="5" t="s">
         <v>1267</v>
       </c>
@@ -24879,48 +24879,109 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="F105:I105"/>
+    <mergeCell ref="F106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F102:I102"/>
+    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F89:I89"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F92:I92"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="F84:I84"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="F86:I86"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="F68:I68"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F74:I74"/>
+    <mergeCell ref="F75:I75"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="F78:I78"/>
+    <mergeCell ref="F69:I69"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F72:I72"/>
+    <mergeCell ref="F73:I73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
@@ -24945,109 +25006,48 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F74:I74"/>
-    <mergeCell ref="F75:I75"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="F77:I77"/>
-    <mergeCell ref="F78:I78"/>
-    <mergeCell ref="F69:I69"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F72:I72"/>
-    <mergeCell ref="F73:I73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="F68:I68"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F84:I84"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="F86:I86"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="F95:I95"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F89:I89"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F92:I92"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="F105:I105"/>
-    <mergeCell ref="F106:I106"/>
-    <mergeCell ref="F107:I107"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F102:I102"/>
-    <mergeCell ref="F103:I103"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26938,210 +26938,210 @@
         <v>1037</v>
       </c>
       <c r="D14" s="66"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="71" t="s">
+      <c r="E14" s="69"/>
+      <c r="F14" s="72" t="s">
         <v>463</v>
       </c>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="73" t="s">
         <v>1038</v>
       </c>
       <c r="B15" s="42" t="s">
         <v>1039</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="70" t="s">
         <v>1040</v>
       </c>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
       <c r="F15" s="67"/>
       <c r="G15" s="65"/>
       <c r="H15" s="65"/>
       <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="74"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="42" t="s">
         <v>1041</v>
       </c>
-      <c r="C16" s="68" t="s">
+      <c r="C16" s="70" t="s">
         <v>1042</v>
       </c>
-      <c r="D16" s="68"/>
-      <c r="E16" s="69"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="71"/>
       <c r="F16" s="67"/>
       <c r="G16" s="65"/>
       <c r="H16" s="65"/>
       <c r="I16" s="65"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="74"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="42" t="s">
         <v>1043</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="70" t="s">
         <v>1044</v>
       </c>
-      <c r="D17" s="68"/>
-      <c r="E17" s="69"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="67"/>
       <c r="G17" s="65"/>
       <c r="H17" s="65"/>
       <c r="I17" s="65"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="74"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="42" t="s">
         <v>1045</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="71" t="s">
         <v>1046</v>
       </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
       <c r="F18" s="67"/>
       <c r="G18" s="65"/>
       <c r="H18" s="65"/>
       <c r="I18" s="65"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="74"/>
+      <c r="A19" s="73"/>
       <c r="B19" s="42" t="s">
         <v>1047</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="71" t="s">
         <v>1048</v>
       </c>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
       <c r="F19" s="67"/>
       <c r="G19" s="65"/>
       <c r="H19" s="65"/>
       <c r="I19" s="65"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="74" t="s">
         <v>1049</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>1050</v>
       </c>
-      <c r="C20" s="69" t="s">
+      <c r="C20" s="71" t="s">
         <v>1051</v>
       </c>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
       <c r="F20" s="67"/>
       <c r="G20" s="65"/>
       <c r="H20" s="65"/>
       <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="75"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="42" t="s">
         <v>1052</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="71" t="s">
         <v>1053</v>
       </c>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
       <c r="F21" s="67"/>
       <c r="G21" s="65"/>
       <c r="H21" s="65"/>
       <c r="I21" s="65"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="75"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="42" t="s">
         <v>1054</v>
       </c>
-      <c r="C22" s="69" t="s">
+      <c r="C22" s="71" t="s">
         <v>1055</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
       <c r="F22" s="67"/>
       <c r="G22" s="65"/>
       <c r="H22" s="65"/>
       <c r="I22" s="65"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="75"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="42" t="s">
         <v>1056</v>
       </c>
-      <c r="C23" s="69" t="s">
+      <c r="C23" s="71" t="s">
         <v>1057</v>
       </c>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
       <c r="F23" s="67"/>
       <c r="G23" s="65"/>
       <c r="H23" s="65"/>
       <c r="I23" s="65"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="74" t="s">
         <v>1058</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>1050</v>
       </c>
-      <c r="C24" s="69" t="s">
+      <c r="C24" s="71" t="s">
         <v>1059</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
       <c r="F24" s="67"/>
       <c r="G24" s="65"/>
       <c r="H24" s="65"/>
       <c r="I24" s="65"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="42" t="s">
         <v>1060</v>
       </c>
-      <c r="C25" s="69" t="s">
+      <c r="C25" s="71" t="s">
         <v>1061</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
       <c r="F25" s="67"/>
       <c r="G25" s="65"/>
       <c r="H25" s="65"/>
       <c r="I25" s="65"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="75"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="42" t="s">
         <v>1054</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="71" t="s">
         <v>1062</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
       <c r="F26" s="67"/>
       <c r="G26" s="65"/>
       <c r="H26" s="65"/>
       <c r="I26" s="65"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="75"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="42" t="s">
         <v>1056</v>
       </c>
-      <c r="C27" s="73" t="s">
+      <c r="C27" s="75" t="s">
         <v>1063</v>
       </c>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
       <c r="F27" s="67"/>
       <c r="G27" s="65"/>
       <c r="H27" s="65"/>
@@ -27154,137 +27154,137 @@
       <c r="B28" s="45" t="s">
         <v>1065</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="75" t="s">
         <v>1066</v>
       </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
       <c r="F28" s="67"/>
       <c r="G28" s="65"/>
       <c r="H28" s="65"/>
       <c r="I28" s="65"/>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="75" t="s">
+      <c r="A29" s="74" t="s">
         <v>1067</v>
       </c>
       <c r="B29" s="45" t="s">
         <v>1068</v>
       </c>
-      <c r="C29" s="73" t="s">
+      <c r="C29" s="75" t="s">
         <v>1069</v>
       </c>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
       <c r="F29" s="67"/>
       <c r="G29" s="65"/>
       <c r="H29" s="65"/>
       <c r="I29" s="65"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="75"/>
+      <c r="A30" s="74"/>
       <c r="B30" s="45" t="s">
         <v>1070</v>
       </c>
-      <c r="C30" s="73" t="s">
+      <c r="C30" s="75" t="s">
         <v>1071</v>
       </c>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
       <c r="F30" s="67"/>
       <c r="G30" s="65"/>
       <c r="H30" s="65"/>
       <c r="I30" s="65"/>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="74" t="s">
         <v>1072</v>
       </c>
       <c r="B31" s="45" t="s">
         <v>1073</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C31" s="75" t="s">
         <v>1074</v>
       </c>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
       <c r="F31" s="67"/>
       <c r="G31" s="65"/>
       <c r="H31" s="65"/>
       <c r="I31" s="65"/>
     </row>
     <row r="32" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="45" t="s">
         <v>1075</v>
       </c>
-      <c r="C32" s="73" t="s">
+      <c r="C32" s="75" t="s">
         <v>1076</v>
       </c>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
       <c r="F32" s="67"/>
       <c r="G32" s="65"/>
       <c r="H32" s="65"/>
       <c r="I32" s="65"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="74" t="s">
         <v>1077</v>
       </c>
       <c r="B33" s="45" t="s">
         <v>1050</v>
       </c>
-      <c r="C33" s="73" t="s">
+      <c r="C33" s="75" t="s">
         <v>1078</v>
       </c>
-      <c r="D33" s="73"/>
-      <c r="E33" s="73"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
       <c r="F33" s="67"/>
       <c r="G33" s="65"/>
       <c r="H33" s="65"/>
       <c r="I33" s="65"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="75"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="45" t="s">
         <v>1079</v>
       </c>
-      <c r="C34" s="73" t="s">
+      <c r="C34" s="75" t="s">
         <v>1080</v>
       </c>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
       <c r="F34" s="67"/>
       <c r="G34" s="65"/>
       <c r="H34" s="65"/>
       <c r="I34" s="65"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="75"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="45" t="s">
         <v>1081</v>
       </c>
-      <c r="C35" s="73" t="s">
+      <c r="C35" s="75" t="s">
         <v>1082</v>
       </c>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
       <c r="F35" s="67"/>
       <c r="G35" s="65"/>
       <c r="H35" s="65"/>
       <c r="I35" s="65"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="75"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C36" s="73" t="s">
+      <c r="C36" s="75" t="s">
         <v>1083</v>
       </c>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="67"/>
       <c r="G36" s="65"/>
       <c r="H36" s="65"/>
@@ -27297,97 +27297,97 @@
       <c r="B37" s="45" t="s">
         <v>1065</v>
       </c>
-      <c r="C37" s="73" t="s">
+      <c r="C37" s="75" t="s">
         <v>1085</v>
       </c>
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
       <c r="F37" s="67"/>
       <c r="G37" s="65"/>
       <c r="H37" s="65"/>
       <c r="I37" s="65"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="74" t="s">
         <v>1086</v>
       </c>
       <c r="B38" s="45" t="s">
         <v>1087</v>
       </c>
-      <c r="C38" s="73" t="s">
+      <c r="C38" s="75" t="s">
         <v>1088</v>
       </c>
-      <c r="D38" s="73"/>
-      <c r="E38" s="73"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
       <c r="F38" s="67"/>
       <c r="G38" s="65"/>
       <c r="H38" s="65"/>
       <c r="I38" s="65"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="75"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="45" t="s">
         <v>1089</v>
       </c>
-      <c r="C39" s="73" t="s">
+      <c r="C39" s="75" t="s">
         <v>1090</v>
       </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
       <c r="F39" s="67"/>
       <c r="G39" s="65"/>
       <c r="H39" s="65"/>
       <c r="I39" s="65"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="75"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="45" t="s">
         <v>1091</v>
       </c>
-      <c r="C40" s="73" t="s">
+      <c r="C40" s="75" t="s">
         <v>1092</v>
       </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="73"/>
+      <c r="D40" s="75"/>
+      <c r="E40" s="75"/>
       <c r="F40" s="67"/>
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
       <c r="I40" s="65"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="75" t="s">
+      <c r="A41" s="74" t="s">
         <v>1093</v>
       </c>
       <c r="B41" s="45" t="s">
         <v>1094</v>
       </c>
-      <c r="C41" s="73" t="s">
+      <c r="C41" s="75" t="s">
         <v>1095</v>
       </c>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="75"/>
       <c r="F41" s="67"/>
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
       <c r="I41" s="65"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="75"/>
+      <c r="A42" s="74"/>
       <c r="B42" s="45" t="s">
         <v>1096</v>
       </c>
-      <c r="C42" s="73" t="s">
+      <c r="C42" s="75" t="s">
         <v>1097</v>
       </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="75"/>
       <c r="F42" s="67"/>
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
       <c r="I42" s="65"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="75"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="45" t="s">
         <v>1098</v>
       </c>
@@ -27402,47 +27402,47 @@
       <c r="I43" s="65"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="75"/>
+      <c r="A44" s="74"/>
       <c r="B44" s="45" t="s">
         <v>1100</v>
       </c>
-      <c r="C44" s="74" t="s">
+      <c r="C44" s="73" t="s">
         <v>1101</v>
       </c>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
       <c r="F44" s="67"/>
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
       <c r="I44" s="65"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="75" t="s">
+      <c r="A45" s="74" t="s">
         <v>1102</v>
       </c>
       <c r="B45" s="45" t="s">
         <v>1103</v>
       </c>
-      <c r="C45" s="74" t="s">
+      <c r="C45" s="73" t="s">
         <v>1104</v>
       </c>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73"/>
       <c r="F45" s="67"/>
       <c r="G45" s="65"/>
       <c r="H45" s="65"/>
       <c r="I45" s="65"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="75"/>
+      <c r="A46" s="74"/>
       <c r="B46" s="45" t="s">
         <v>1105</v>
       </c>
-      <c r="C46" s="74" t="s">
+      <c r="C46" s="73" t="s">
         <v>1106</v>
       </c>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
       <c r="F46" s="67"/>
       <c r="G46" s="65"/>
       <c r="H46" s="65"/>
@@ -27455,11 +27455,11 @@
       <c r="B47" s="45" t="s">
         <v>1065</v>
       </c>
-      <c r="C47" s="74" t="s">
+      <c r="C47" s="73" t="s">
         <v>1108</v>
       </c>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="73"/>
       <c r="F47" s="67"/>
       <c r="G47" s="65"/>
       <c r="H47" s="65"/>
@@ -27472,165 +27472,165 @@
       <c r="B48" s="45" t="s">
         <v>1110</v>
       </c>
-      <c r="C48" s="74" t="s">
+      <c r="C48" s="73" t="s">
         <v>1111</v>
       </c>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="73"/>
       <c r="F48" s="67"/>
       <c r="G48" s="65"/>
       <c r="H48" s="65"/>
       <c r="I48" s="65"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="75" t="s">
+      <c r="A49" s="74" t="s">
         <v>1112</v>
       </c>
       <c r="B49" s="45" t="s">
         <v>1113</v>
       </c>
-      <c r="C49" s="74" t="s">
+      <c r="C49" s="73" t="s">
         <v>1114</v>
       </c>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="73"/>
       <c r="F49" s="67"/>
       <c r="G49" s="65"/>
       <c r="H49" s="65"/>
       <c r="I49" s="65"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="75"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="45" t="s">
         <v>1115</v>
       </c>
-      <c r="C50" s="74" t="s">
+      <c r="C50" s="73" t="s">
         <v>1116</v>
       </c>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
       <c r="F50" s="67"/>
       <c r="G50" s="65"/>
       <c r="H50" s="65"/>
       <c r="I50" s="65"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="75"/>
+      <c r="A51" s="74"/>
       <c r="B51" s="45" t="s">
         <v>1060</v>
       </c>
-      <c r="C51" s="74" t="s">
+      <c r="C51" s="73" t="s">
         <v>1117</v>
       </c>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="73"/>
       <c r="F51" s="67"/>
       <c r="G51" s="65"/>
       <c r="H51" s="65"/>
       <c r="I51" s="65"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="75"/>
+      <c r="A52" s="74"/>
       <c r="B52" s="45" t="s">
         <v>1118</v>
       </c>
-      <c r="C52" s="74" t="s">
+      <c r="C52" s="73" t="s">
         <v>1119</v>
       </c>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73"/>
       <c r="F52" s="67"/>
       <c r="G52" s="65"/>
       <c r="H52" s="65"/>
       <c r="I52" s="65"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="75"/>
+      <c r="A53" s="74"/>
       <c r="B53" s="45" t="s">
         <v>1056</v>
       </c>
-      <c r="C53" s="74" t="s">
+      <c r="C53" s="73" t="s">
         <v>1120</v>
       </c>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
+      <c r="D53" s="73"/>
+      <c r="E53" s="73"/>
       <c r="F53" s="67"/>
       <c r="G53" s="65"/>
       <c r="H53" s="65"/>
       <c r="I53" s="65"/>
     </row>
     <row r="54" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="75" t="s">
+      <c r="A54" s="74" t="s">
         <v>1121</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>1122</v>
       </c>
-      <c r="C54" s="74" t="s">
+      <c r="C54" s="73" t="s">
         <v>1123</v>
       </c>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="73"/>
       <c r="F54" s="67"/>
       <c r="G54" s="65"/>
       <c r="H54" s="65"/>
       <c r="I54" s="65"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="75"/>
+      <c r="A55" s="74"/>
       <c r="B55" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="C55" s="74" t="s">
+      <c r="C55" s="73" t="s">
         <v>1125</v>
       </c>
-      <c r="D55" s="74"/>
-      <c r="E55" s="74"/>
+      <c r="D55" s="73"/>
+      <c r="E55" s="73"/>
       <c r="F55" s="67"/>
       <c r="G55" s="65"/>
       <c r="H55" s="65"/>
       <c r="I55" s="65"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="75"/>
+      <c r="A56" s="74"/>
       <c r="B56" s="5" t="s">
         <v>1126</v>
       </c>
-      <c r="C56" s="74" t="s">
+      <c r="C56" s="73" t="s">
         <v>1127</v>
       </c>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
       <c r="F56" s="67"/>
       <c r="G56" s="65"/>
       <c r="H56" s="65"/>
       <c r="I56" s="65"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="75"/>
+      <c r="A57" s="74"/>
       <c r="B57" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="C57" s="74" t="s">
+      <c r="C57" s="73" t="s">
         <v>1129</v>
       </c>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
+      <c r="D57" s="73"/>
+      <c r="E57" s="73"/>
       <c r="F57" s="67"/>
       <c r="G57" s="65"/>
       <c r="H57" s="65"/>
       <c r="I57" s="65"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="75"/>
+      <c r="A58" s="74"/>
       <c r="B58" s="5" t="s">
         <v>1130</v>
       </c>
-      <c r="C58" s="74" t="s">
+      <c r="C58" s="73" t="s">
         <v>1131</v>
       </c>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
       <c r="F58" s="67"/>
       <c r="G58" s="65"/>
       <c r="H58" s="65"/>
@@ -27643,88 +27643,88 @@
       <c r="B59" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="C59" s="74" t="s">
+      <c r="C59" s="73" t="s">
         <v>1133</v>
       </c>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
       <c r="F59" s="67"/>
       <c r="G59" s="65"/>
       <c r="H59" s="65"/>
       <c r="I59" s="65"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="75" t="s">
+      <c r="A60" s="74" t="s">
         <v>1134</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>1135</v>
       </c>
-      <c r="C60" s="74" t="s">
+      <c r="C60" s="73" t="s">
         <v>1136</v>
       </c>
-      <c r="D60" s="74"/>
-      <c r="E60" s="74"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="73"/>
       <c r="F60" s="67"/>
       <c r="G60" s="65"/>
       <c r="H60" s="65"/>
       <c r="I60" s="65"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="75"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="5" t="s">
         <v>1137</v>
       </c>
-      <c r="C61" s="74" t="s">
+      <c r="C61" s="73" t="s">
         <v>1138</v>
       </c>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
       <c r="F61" s="67"/>
       <c r="G61" s="65"/>
       <c r="H61" s="65"/>
       <c r="I61" s="65"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="75"/>
+      <c r="A62" s="74"/>
       <c r="B62" s="5" t="s">
         <v>1139</v>
       </c>
-      <c r="C62" s="74" t="s">
+      <c r="C62" s="73" t="s">
         <v>1140</v>
       </c>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
       <c r="F62" s="67"/>
       <c r="G62" s="65"/>
       <c r="H62" s="65"/>
       <c r="I62" s="65"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="75"/>
+      <c r="A63" s="74"/>
       <c r="B63" s="5" t="s">
         <v>1141</v>
       </c>
-      <c r="C63" s="74" t="s">
+      <c r="C63" s="73" t="s">
         <v>1142</v>
       </c>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
       <c r="F63" s="67"/>
       <c r="G63" s="65"/>
       <c r="H63" s="65"/>
       <c r="I63" s="65"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="75"/>
+      <c r="A64" s="74"/>
       <c r="B64" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="C64" s="74" t="s">
+      <c r="C64" s="73" t="s">
         <v>1144</v>
       </c>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
       <c r="F64" s="67"/>
       <c r="G64" s="65"/>
       <c r="H64" s="65"/>
@@ -27732,36 +27732,66 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F37:I37"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="F29:I29"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="C64:E64"/>
     <mergeCell ref="A54:A58"/>
@@ -27786,66 +27816,36 @@
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="C52:E52"/>
     <mergeCell ref="C53:E53"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -28310,12 +28310,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C30:F30"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C20:F20"/>
@@ -28328,6 +28322,12 @@
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29108,6 +29108,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F17:I17"/>
@@ -29120,13 +29127,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="F29:I29"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29497,6 +29497,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="F12:I12"/>
     <mergeCell ref="F9:I9"/>
@@ -29504,18 +29516,6 @@
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="F11:I11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -29982,19 +29982,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
@@ -30008,6 +29995,19 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -30984,29 +30984,33 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="F35:I35"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="F32:I32"/>
     <mergeCell ref="C24:D24"/>
@@ -31020,33 +31024,29 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31531,13 +31531,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="F15:I15"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C20:D20"/>
@@ -31548,6 +31541,13 @@
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="F15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -31955,6 +31955,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="F19:I19"/>
     <mergeCell ref="C20:D20"/>
@@ -31967,11 +31972,6 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F17:I17"/>
     <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -32003,6 +32003,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004592A3ADBB772D4689FCD56C8516F45D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6dee92c918a6173969cc6829137ba01">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c" xmlns:ns3="eda01c43-580c-44af-a5fd-4ea1802e476c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e0be94b10bd652582aed8d62fec2d74" ns2:_="" ns3:_="">
     <xsd:import namespace="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
@@ -32231,27 +32251,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="eda01c43-580c-44af-a5fd-4ea1802e476c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA0A127A-D0D0-4182-84ED-7D64B945D928}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32268,29 +32293,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB40FF6F-009E-4D48-B4D3-33D1A3C62497}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44895076-51AC-48B4-9F72-A977D30F13F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9a1da51d-87f1-4c78-b9e6-a6488d1ad35c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eda01c43-580c-44af-a5fd-4ea1802e476c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>